<commit_message>
Möjlighet att ha samma individuella voltigör på olika hästar i samma klass
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll_2019_mixklass lag(mall).xlsx
+++ b/mallar/Protokoll/Protokoll_2019_mixklass lag(mall).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13095"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="13095"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="27" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <definedName name="result" localSheetId="3">'Mixklass E grund'!$K$38</definedName>
     <definedName name="result" localSheetId="4">'Mixklass lagkür typ 2'!$L$35</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="125">
   <si>
     <t>1)</t>
   </si>
@@ -493,6 +493,9 @@
   </si>
   <si>
     <t>3-6 voltigörer</t>
+  </si>
+  <si>
+    <t>Protokollen uppdaterades senast 2019-03-28.</t>
   </si>
 </sst>
 </file>
@@ -508,11 +511,18 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1291,836 +1301,837 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="310">
+  <cellXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="30" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="14" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="28" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="30" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="30" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="14" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="28" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="30" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="3" fillId="2" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="7" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Dezimal 2" xfId="2"/>
@@ -2497,94 +2508,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B20" activeCellId="1" sqref="E18 B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="18" width="15.73046875" customWidth="1"/>
+    <col min="1" max="18" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="84" customFormat="1" ht="20.65" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" s="84" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="83" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="84" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="84" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="84" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="152" customFormat="1" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:5" s="152" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" s="152" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="310" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="152" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="152" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="152" customFormat="1" ht="14.25" x14ac:dyDescent="0.45"/>
-    <row r="6" spans="1:5" s="84" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:5" s="76" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" s="152" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:5" s="76" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="76" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="77" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="77" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="77" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="77" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="77" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="77"/>
     </row>
-    <row r="13" spans="1:5" s="78" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="78" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="79" t="s">
         <v>69</v>
       </c>
       <c r="C14" s="77"/>
     </row>
-    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="306" t="s">
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="163" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="307" t="s">
+      <c r="C15" s="164" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="305" t="s">
+      <c r="D15" s="162" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="308" t="s">
+      <c r="B16" s="165" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="308" t="s">
+      <c r="C16" s="165" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="309" t="s">
+      <c r="D16" s="166" t="s">
         <v>123</v>
       </c>
       <c r="E16" s="155"/>
     </row>
-    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="77"/>
       <c r="B17" s="80" t="s">
         <v>114</v>
@@ -2594,30 +2609,30 @@
       </c>
       <c r="D17" s="151"/>
     </row>
-    <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="77"/>
       <c r="B18" s="153"/>
       <c r="C18" s="153"/>
       <c r="D18" s="154"/>
     </row>
-    <row r="19" spans="1:8" s="152" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" s="152" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="308" t="s">
+      <c r="B19" s="165" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="309" t="s">
+      <c r="C19" s="166" t="s">
         <v>111</v>
       </c>
-      <c r="D19" s="309" t="s">
+      <c r="D19" s="166" t="s">
         <v>123</v>
       </c>
       <c r="E19" s="154"/>
       <c r="F19" s="154"/>
       <c r="G19" s="154"/>
     </row>
-    <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="77"/>
       <c r="B20" s="80" t="s">
         <v>114</v>
@@ -2630,7 +2645,7 @@
       <c r="F20" s="153"/>
       <c r="G20" s="153"/>
     </row>
-    <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="77"/>
       <c r="B21" s="153"/>
       <c r="C21" s="153"/>
@@ -2640,24 +2655,24 @@
       <c r="G21" s="153"/>
       <c r="H21" s="153"/>
     </row>
-    <row r="25" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N34" s="79"/>
     </row>
-    <row r="35" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N35" s="78"/>
       <c r="O35" s="78"/>
       <c r="P35" s="78"/>
       <c r="Q35" s="78"/>
     </row>
-    <row r="36" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:17" s="84" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:17" s="84" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -2672,7 +2687,7 @@
       <c r="L40"/>
       <c r="M40"/>
     </row>
-    <row r="41" spans="1:17" s="82" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -2687,7 +2702,7 @@
       <c r="L41"/>
       <c r="M41"/>
     </row>
-    <row r="42" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -2702,7 +2717,7 @@
       <c r="L42"/>
       <c r="M42"/>
     </row>
-    <row r="43" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -2717,7 +2732,7 @@
       <c r="L43"/>
       <c r="M43"/>
     </row>
-    <row r="44" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -2742,29 +2757,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A21" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A35" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.73046875" style="47" customWidth="1"/>
-    <col min="2" max="2" width="10.265625" style="47" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" style="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.73046875" style="47" customWidth="1"/>
-    <col min="5" max="5" width="7.265625" style="47" customWidth="1"/>
-    <col min="6" max="6" width="14.59765625" style="47" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="47" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="47" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" style="47" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="47" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="47" customWidth="1"/>
     <col min="7" max="7" width="7" style="47" customWidth="1"/>
-    <col min="8" max="8" width="9.59765625" style="47" customWidth="1"/>
-    <col min="9" max="9" width="5.73046875" style="47" customWidth="1"/>
-    <col min="10" max="10" width="5.59765625" style="47" customWidth="1"/>
-    <col min="11" max="11" width="7.1328125" style="47" customWidth="1"/>
-    <col min="12" max="12" width="7.265625" style="47" customWidth="1"/>
-    <col min="13" max="16384" width="9.1328125" style="47"/>
+    <col min="8" max="8" width="9.5703125" style="47" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" style="47" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" style="47" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="47" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" style="47" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>78</v>
       </c>
@@ -2776,7 +2791,7 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -2788,7 +2803,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2804,14 +2819,14 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="162"/>
-      <c r="E5" s="162"/>
+      <c r="C5" s="193"/>
+      <c r="D5" s="193"/>
+      <c r="E5" s="193"/>
       <c r="G5" s="9"/>
       <c r="H5" s="13" t="s">
         <v>11</v>
@@ -2820,19 +2835,19 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162"/>
-      <c r="E6" s="162"/>
+      <c r="C6" s="193"/>
+      <c r="D6" s="193"/>
+      <c r="E6" s="193"/>
       <c r="G6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>62</v>
       </c>
@@ -2843,79 +2858,79 @@
       <c r="G7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="163"/>
-      <c r="I7" s="164"/>
-      <c r="J7" s="164"/>
-      <c r="K7" s="165"/>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="192"/>
+      <c r="I7" s="201"/>
+      <c r="J7" s="201"/>
+      <c r="K7" s="202"/>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
+      <c r="C8" s="192"/>
+      <c r="D8" s="192"/>
+      <c r="E8" s="192"/>
       <c r="G8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="162"/>
-      <c r="I8" s="168"/>
-      <c r="J8" s="168"/>
-      <c r="K8" s="169"/>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="193"/>
+      <c r="I8" s="194"/>
+      <c r="J8" s="194"/>
+      <c r="K8" s="195"/>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="162"/>
-      <c r="D9" s="162"/>
-      <c r="E9" s="162"/>
+      <c r="C9" s="193"/>
+      <c r="D9" s="193"/>
+      <c r="E9" s="193"/>
       <c r="G9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="162"/>
-      <c r="I9" s="168"/>
-      <c r="J9" s="168"/>
-      <c r="K9" s="169"/>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="193"/>
+      <c r="I9" s="194"/>
+      <c r="J9" s="194"/>
+      <c r="K9" s="195"/>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="162"/>
-      <c r="E10" s="162"/>
+      <c r="C10" s="193"/>
+      <c r="D10" s="193"/>
+      <c r="E10" s="193"/>
       <c r="G10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="162"/>
-      <c r="I10" s="168"/>
-      <c r="J10" s="168"/>
-      <c r="K10" s="169"/>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="193"/>
+      <c r="I10" s="194"/>
+      <c r="J10" s="194"/>
+      <c r="K10" s="195"/>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="162"/>
-      <c r="I11" s="168"/>
-      <c r="J11" s="168"/>
-      <c r="K11" s="169"/>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="193"/>
+      <c r="I11" s="194"/>
+      <c r="J11" s="194"/>
+      <c r="K11" s="195"/>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="16"/>
       <c r="G12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="162"/>
-      <c r="I12" s="168"/>
-      <c r="J12" s="168"/>
-      <c r="K12" s="169"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="193"/>
+      <c r="I12" s="194"/>
+      <c r="J12" s="194"/>
+      <c r="K12" s="195"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="16"/>
       <c r="G13" s="3"/>
       <c r="H13" s="46"/>
@@ -2923,206 +2938,206 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G14" s="180" t="s">
+    <row r="14" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="196" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="181"/>
-      <c r="I14" s="182" t="s">
+      <c r="H14" s="197"/>
+      <c r="I14" s="198" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="183"/>
-      <c r="K14" s="184"/>
-    </row>
-    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="185" t="s">
+      <c r="J14" s="199"/>
+      <c r="K14" s="200"/>
+    </row>
+    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="169" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="188" t="s">
+      <c r="B15" s="183" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="188" t="s">
+      <c r="C15" s="183" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="188"/>
-      <c r="E15" s="189" t="s">
+      <c r="D15" s="183"/>
+      <c r="E15" s="186" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="190"/>
+      <c r="F15" s="187"/>
       <c r="G15" s="48"/>
       <c r="H15" s="49"/>
-      <c r="I15" s="191" t="s">
+      <c r="I15" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="175"/>
-      <c r="K15" s="170">
+      <c r="J15" s="207"/>
+      <c r="K15" s="205">
         <f>ROUND(J15*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="186"/>
-      <c r="B16" s="172"/>
-      <c r="C16" s="172" t="s">
+    <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="170"/>
+      <c r="B16" s="177"/>
+      <c r="C16" s="177" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="172"/>
-      <c r="E16" s="173" t="s">
+      <c r="D16" s="177"/>
+      <c r="E16" s="178" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="174"/>
+      <c r="F16" s="179"/>
       <c r="G16" s="50"/>
       <c r="H16" s="51"/>
-      <c r="I16" s="192"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="171"/>
-    </row>
-    <row r="17" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="186"/>
-      <c r="B17" s="172"/>
-      <c r="C17" s="172" t="s">
+      <c r="I16" s="176"/>
+      <c r="J16" s="208"/>
+      <c r="K16" s="206"/>
+    </row>
+    <row r="17" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="170"/>
+      <c r="B17" s="177"/>
+      <c r="C17" s="177" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="172"/>
-      <c r="E17" s="173" t="s">
+      <c r="D17" s="177"/>
+      <c r="E17" s="178" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="174"/>
+      <c r="F17" s="179"/>
       <c r="G17" s="52"/>
       <c r="H17" s="53"/>
-      <c r="I17" s="192"/>
-      <c r="J17" s="176"/>
-      <c r="K17" s="171"/>
-    </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="186"/>
-      <c r="B18" s="193" t="s">
+      <c r="I17" s="176"/>
+      <c r="J17" s="208"/>
+      <c r="K17" s="206"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="170"/>
+      <c r="B18" s="188" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="172" t="s">
+      <c r="C18" s="177" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="172"/>
-      <c r="E18" s="173" t="s">
+      <c r="D18" s="177"/>
+      <c r="E18" s="178" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="174"/>
+      <c r="F18" s="179"/>
       <c r="G18" s="54"/>
       <c r="H18" s="55"/>
-      <c r="I18" s="192" t="s">
+      <c r="I18" s="176" t="s">
         <v>8</v>
       </c>
-      <c r="J18" s="176"/>
-      <c r="K18" s="171">
+      <c r="J18" s="208"/>
+      <c r="K18" s="206">
         <f>ROUND(J18*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="186"/>
-      <c r="B19" s="194"/>
-      <c r="C19" s="172" t="s">
+    <row r="19" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="170"/>
+      <c r="B19" s="189"/>
+      <c r="C19" s="177" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="172"/>
-      <c r="E19" s="173" t="s">
+      <c r="D19" s="177"/>
+      <c r="E19" s="178" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="174"/>
+      <c r="F19" s="179"/>
       <c r="G19" s="50"/>
       <c r="H19" s="51"/>
-      <c r="I19" s="192"/>
-      <c r="J19" s="176"/>
-      <c r="K19" s="171"/>
-    </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="187"/>
-      <c r="B20" s="195"/>
-      <c r="C20" s="197" t="s">
+      <c r="I19" s="176"/>
+      <c r="J19" s="208"/>
+      <c r="K19" s="206"/>
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="171"/>
+      <c r="B20" s="190"/>
+      <c r="C20" s="180" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="197"/>
-      <c r="E20" s="198" t="s">
+      <c r="D20" s="180"/>
+      <c r="E20" s="181" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="199"/>
+      <c r="F20" s="182"/>
       <c r="G20" s="56"/>
       <c r="H20" s="57"/>
-      <c r="I20" s="196"/>
-      <c r="J20" s="177"/>
-      <c r="K20" s="178"/>
-    </row>
-    <row r="21" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="185" t="s">
+      <c r="I20" s="191"/>
+      <c r="J20" s="209"/>
+      <c r="K20" s="210"/>
+    </row>
+    <row r="21" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="169" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="202" t="s">
+      <c r="B21" s="172" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="188" t="s">
+      <c r="C21" s="183" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="188"/>
-      <c r="E21" s="205" t="s">
+      <c r="D21" s="183"/>
+      <c r="E21" s="184" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="206"/>
+      <c r="F21" s="185"/>
       <c r="G21" s="58"/>
       <c r="H21" s="59"/>
-      <c r="I21" s="191" t="s">
+      <c r="I21" s="175" t="s">
         <v>65</v>
       </c>
-      <c r="J21" s="175"/>
-      <c r="K21" s="170">
+      <c r="J21" s="207"/>
+      <c r="K21" s="205">
         <f>ROUND(J21*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="186"/>
-      <c r="B22" s="203"/>
-      <c r="C22" s="172" t="s">
+    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="170"/>
+      <c r="B22" s="173"/>
+      <c r="C22" s="177" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="172"/>
-      <c r="E22" s="173" t="s">
+      <c r="D22" s="177"/>
+      <c r="E22" s="178" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="174"/>
+      <c r="F22" s="179"/>
       <c r="G22" s="50"/>
       <c r="H22" s="51"/>
-      <c r="I22" s="192"/>
-      <c r="J22" s="176"/>
-      <c r="K22" s="171"/>
-    </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="186"/>
-      <c r="B23" s="204"/>
-      <c r="C23" s="172" t="s">
+      <c r="I22" s="176"/>
+      <c r="J22" s="208"/>
+      <c r="K22" s="206"/>
+    </row>
+    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="170"/>
+      <c r="B23" s="174"/>
+      <c r="C23" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="172"/>
-      <c r="E23" s="173" t="s">
+      <c r="D23" s="177"/>
+      <c r="E23" s="178" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="174"/>
+      <c r="F23" s="179"/>
       <c r="G23" s="52"/>
       <c r="H23" s="53"/>
-      <c r="I23" s="192"/>
-      <c r="J23" s="176"/>
-      <c r="K23" s="171"/>
-    </row>
-    <row r="24" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="187"/>
+      <c r="I23" s="176"/>
+      <c r="J23" s="208"/>
+      <c r="K23" s="206"/>
+    </row>
+    <row r="24" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="171"/>
       <c r="B24" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="197"/>
-      <c r="D24" s="197"/>
-      <c r="E24" s="198" t="s">
+      <c r="C24" s="180"/>
+      <c r="D24" s="180"/>
+      <c r="E24" s="181" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="199"/>
+      <c r="F24" s="182"/>
       <c r="G24" s="61"/>
       <c r="H24" s="62"/>
       <c r="I24" s="63" t="s">
@@ -3134,21 +3149,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="64" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="179" t="s">
+      <c r="C25" s="211" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="179"/>
-      <c r="E25" s="200" t="s">
+      <c r="D25" s="211"/>
+      <c r="E25" s="167" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="201"/>
+      <c r="F25" s="168"/>
       <c r="G25" s="65"/>
       <c r="H25" s="66"/>
       <c r="I25" s="67" t="s">
@@ -3160,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="69"/>
       <c r="B26" s="69"/>
       <c r="C26" s="69"/>
@@ -3173,7 +3188,7 @@
       <c r="J26" s="69"/>
       <c r="K26" s="69"/>
     </row>
-    <row r="27" spans="1:11" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="69"/>
       <c r="B27" s="69"/>
       <c r="C27" s="69"/>
@@ -3185,13 +3200,13 @@
         <v>10</v>
       </c>
       <c r="I27" s="71"/>
-      <c r="J27" s="166">
+      <c r="J27" s="203">
         <f>SUM(K15:K25)</f>
         <v>0</v>
       </c>
-      <c r="K27" s="167"/>
-    </row>
-    <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="K27" s="204"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
@@ -3210,40 +3225,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="C6:E6"/>
@@ -3260,6 +3241,40 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3267,6 +3282,7 @@
     <oddHeader xml:space="preserve">&amp;L&amp;G
 &amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LAGKLASS
 </oddHeader>
+    <oddFooter>&amp;R2019-03-28</oddFooter>
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>
@@ -3276,26 +3292,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" style="1"/>
-    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="11" width="7.265625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.59765625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1328125" style="1"/>
+    <col min="9" max="11" width="7.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>78</v>
       </c>
@@ -3307,7 +3323,7 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>79</v>
       </c>
@@ -3319,7 +3335,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3336,15 +3352,15 @@
       <c r="K4" s="11"/>
       <c r="L4" s="91"/>
     </row>
-    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="162"/>
-      <c r="D5" s="162"/>
-      <c r="E5" s="162"/>
-      <c r="F5" s="162"/>
+      <c r="C5" s="193"/>
+      <c r="D5" s="193"/>
+      <c r="E5" s="193"/>
+      <c r="F5" s="193"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>11</v>
@@ -3353,20 +3369,20 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162"/>
-      <c r="E6" s="162"/>
-      <c r="F6" s="162"/>
+      <c r="C6" s="193"/>
+      <c r="D6" s="193"/>
+      <c r="E6" s="193"/>
+      <c r="F6" s="193"/>
       <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>62</v>
       </c>
@@ -3378,89 +3394,89 @@
       <c r="H7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="163"/>
-      <c r="J7" s="164"/>
-      <c r="K7" s="164"/>
-      <c r="L7" s="164"/>
-    </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="192"/>
+      <c r="J7" s="201"/>
+      <c r="K7" s="201"/>
+      <c r="L7" s="201"/>
+    </row>
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
+      <c r="C8" s="192"/>
+      <c r="D8" s="192"/>
+      <c r="E8" s="192"/>
+      <c r="F8" s="192"/>
       <c r="H8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="162"/>
-      <c r="J8" s="168"/>
-      <c r="K8" s="168"/>
-      <c r="L8" s="168"/>
-    </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="193"/>
+      <c r="J8" s="194"/>
+      <c r="K8" s="194"/>
+      <c r="L8" s="194"/>
+    </row>
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="162"/>
-      <c r="D9" s="162"/>
-      <c r="E9" s="162"/>
-      <c r="F9" s="162"/>
+      <c r="C9" s="193"/>
+      <c r="D9" s="193"/>
+      <c r="E9" s="193"/>
+      <c r="F9" s="193"/>
       <c r="H9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="162"/>
-      <c r="J9" s="168"/>
-      <c r="K9" s="168"/>
-      <c r="L9" s="168"/>
-    </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="193"/>
+      <c r="J9" s="194"/>
+      <c r="K9" s="194"/>
+      <c r="L9" s="194"/>
+    </row>
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="162"/>
-      <c r="D10" s="162"/>
-      <c r="E10" s="162"/>
-      <c r="F10" s="162"/>
+      <c r="C10" s="193"/>
+      <c r="D10" s="193"/>
+      <c r="E10" s="193"/>
+      <c r="F10" s="193"/>
       <c r="H10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="162"/>
-      <c r="J10" s="168"/>
-      <c r="K10" s="168"/>
-      <c r="L10" s="168"/>
-    </row>
-    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="193"/>
+      <c r="J10" s="194"/>
+      <c r="K10" s="194"/>
+      <c r="L10" s="194"/>
+    </row>
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="162"/>
-      <c r="J11" s="168"/>
-      <c r="K11" s="168"/>
-      <c r="L11" s="168"/>
-    </row>
-    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="193"/>
+      <c r="J11" s="194"/>
+      <c r="K11" s="194"/>
+      <c r="L11" s="194"/>
+    </row>
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="16"/>
       <c r="H12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="162"/>
-      <c r="J12" s="168"/>
-      <c r="K12" s="168"/>
-      <c r="L12" s="168"/>
-    </row>
-    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="193"/>
+      <c r="J12" s="194"/>
+      <c r="K12" s="194"/>
+      <c r="L12" s="194"/>
+    </row>
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -3475,7 +3491,7 @@
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F15" s="20">
         <v>1</v>
       </c>
@@ -3498,13 +3514,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="214"/>
-      <c r="B16" s="215" t="s">
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="212"/>
+      <c r="B16" s="213" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="208"/>
-      <c r="D16" s="208"/>
+      <c r="C16" s="214"/>
+      <c r="D16" s="214"/>
       <c r="E16" s="21"/>
       <c r="F16" s="90"/>
       <c r="G16" s="90"/>
@@ -3517,13 +3533,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="214"/>
-      <c r="B17" s="207" t="s">
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="212"/>
+      <c r="B17" s="215" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="208"/>
-      <c r="D17" s="208"/>
+      <c r="C17" s="214"/>
+      <c r="D17" s="214"/>
       <c r="E17" s="21"/>
       <c r="F17" s="90"/>
       <c r="G17" s="90"/>
@@ -3536,12 +3552,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="207" t="s">
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="215" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="208"/>
-      <c r="D18" s="208"/>
+      <c r="C18" s="214"/>
+      <c r="D18" s="214"/>
       <c r="E18" s="21"/>
       <c r="F18" s="90"/>
       <c r="G18" s="90"/>
@@ -3554,12 +3570,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="212" t="s">
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="219" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="208"/>
-      <c r="D19" s="208"/>
+      <c r="C19" s="214"/>
+      <c r="D19" s="214"/>
       <c r="E19" s="21"/>
       <c r="F19" s="90"/>
       <c r="G19" s="90"/>
@@ -3572,13 +3588,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="207" t="s">
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="215" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="208"/>
-      <c r="D20" s="208"/>
-      <c r="E20" s="213"/>
+      <c r="C20" s="214"/>
+      <c r="D20" s="214"/>
+      <c r="E20" s="220"/>
       <c r="F20" s="90"/>
       <c r="G20" s="90"/>
       <c r="H20" s="90"/>
@@ -3590,12 +3606,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="207" t="s">
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="215" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="208"/>
-      <c r="D21" s="208"/>
+      <c r="C21" s="214"/>
+      <c r="D21" s="214"/>
       <c r="E21" s="21"/>
       <c r="F21" s="90"/>
       <c r="G21" s="90"/>
@@ -3608,13 +3624,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="209" t="s">
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="216" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="210"/>
-      <c r="D22" s="210"/>
-      <c r="E22" s="211"/>
+      <c r="C22" s="217"/>
+      <c r="D22" s="217"/>
+      <c r="E22" s="218"/>
       <c r="F22" s="90"/>
       <c r="G22" s="90"/>
       <c r="H22" s="90"/>
@@ -3626,10 +3642,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L23" s="23"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="24" t="s">
         <v>53</v>
       </c>
@@ -3647,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="28"/>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -3664,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B26" s="28"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -3676,7 +3692,7 @@
       <c r="J26" s="33"/>
       <c r="L26" s="34"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B27" s="35"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3690,8 +3706,8 @@
       </c>
       <c r="L27" s="33"/>
     </row>
-    <row r="28" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H29" s="37"/>
       <c r="I29" s="38" t="s">
         <v>57</v>
@@ -3703,7 +3719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -3715,7 +3731,7 @@
       <c r="K30" s="27"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -3727,8 +3743,8 @@
       <c r="K31" s="27"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -3745,7 +3761,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
@@ -3757,7 +3773,7 @@
       <c r="K34" s="27"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="45"/>
       <c r="B35" s="45"/>
       <c r="C35" s="45"/>
@@ -3772,24 +3788,31 @@
       <c r="L35" s="45"/>
       <c r="M35" s="45"/>
     </row>
-    <row r="36" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:E20"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="I8:L8"/>
@@ -3802,19 +3825,13 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader xml:space="preserve">&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LAGKLASS
 </oddHeader>
+    <oddFooter>&amp;R2019-03-28</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="35" max="16383" man="1"/>
@@ -3830,21 +3847,21 @@
   </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A12" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.73046875" style="93" customWidth="1"/>
-    <col min="3" max="10" width="7.59765625" style="93" customWidth="1"/>
-    <col min="11" max="11" width="7.3984375" style="93" customWidth="1"/>
-    <col min="12" max="12" width="7.73046875" style="93" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="8.7109375" style="93" customWidth="1"/>
+    <col min="3" max="10" width="7.5703125" style="93" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" style="93" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="93" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="93"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="142" t="s">
         <v>80</v>
       </c>
@@ -3856,7 +3873,7 @@
       <c r="J2" s="135"/>
       <c r="K2" s="135"/>
     </row>
-    <row r="3" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="141" t="s">
         <v>75</v>
       </c>
@@ -3868,13 +3885,13 @@
       <c r="J3" s="135"/>
       <c r="K3" s="135"/>
     </row>
-    <row r="4" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="99"/>
-      <c r="C4" s="267"/>
-      <c r="D4" s="267"/>
+      <c r="C4" s="229"/>
+      <c r="D4" s="229"/>
       <c r="E4" s="140"/>
       <c r="G4" s="138"/>
       <c r="H4" s="137" t="s">
@@ -3884,14 +3901,14 @@
       <c r="J4" s="135"/>
       <c r="K4" s="135"/>
     </row>
-    <row r="5" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="133" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="133"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
+      <c r="C5" s="230"/>
+      <c r="D5" s="230"/>
+      <c r="E5" s="230"/>
       <c r="G5" s="138"/>
       <c r="H5" s="137" t="s">
         <v>11</v>
@@ -3900,7 +3917,7 @@
       <c r="J5" s="135"/>
       <c r="K5" s="135"/>
     </row>
-    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="93" t="s">
         <v>62</v>
       </c>
@@ -3908,94 +3925,94 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="133" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="133"/>
-      <c r="C7" s="268"/>
-      <c r="D7" s="268"/>
-      <c r="E7" s="268"/>
+      <c r="C7" s="230"/>
+      <c r="D7" s="230"/>
+      <c r="E7" s="230"/>
       <c r="G7" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="269"/>
-      <c r="I7" s="270"/>
-      <c r="J7" s="270"/>
-      <c r="K7" s="270"/>
-    </row>
-    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="231"/>
+      <c r="I7" s="232"/>
+      <c r="J7" s="232"/>
+      <c r="K7" s="232"/>
+    </row>
+    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="99" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="99"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="271"/>
-      <c r="E8" s="271"/>
+      <c r="C8" s="233"/>
+      <c r="D8" s="233"/>
+      <c r="E8" s="233"/>
       <c r="G8" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="262"/>
-      <c r="I8" s="263"/>
-      <c r="J8" s="263"/>
-      <c r="K8" s="263"/>
-    </row>
-    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="221"/>
+      <c r="I8" s="222"/>
+      <c r="J8" s="222"/>
+      <c r="K8" s="222"/>
+    </row>
+    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="133" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="133"/>
-      <c r="C9" s="268"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="268"/>
+      <c r="C9" s="230"/>
+      <c r="D9" s="230"/>
+      <c r="E9" s="230"/>
       <c r="G9" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="262"/>
-      <c r="I9" s="263"/>
-      <c r="J9" s="263"/>
-      <c r="K9" s="263"/>
-    </row>
-    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="221"/>
+      <c r="I9" s="222"/>
+      <c r="J9" s="222"/>
+      <c r="K9" s="222"/>
+    </row>
+    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="133" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="133"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
+      <c r="C10" s="230"/>
+      <c r="D10" s="230"/>
+      <c r="E10" s="230"/>
       <c r="G10" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="262"/>
-      <c r="I10" s="263"/>
-      <c r="J10" s="263"/>
-      <c r="K10" s="263"/>
-    </row>
-    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="221"/>
+      <c r="I10" s="222"/>
+      <c r="J10" s="222"/>
+      <c r="K10" s="222"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G11" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="262"/>
-      <c r="I11" s="263"/>
-      <c r="J11" s="263"/>
-      <c r="K11" s="263"/>
-    </row>
-    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="221"/>
+      <c r="I11" s="222"/>
+      <c r="J11" s="222"/>
+      <c r="K11" s="222"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="134"/>
       <c r="G12" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="262"/>
-      <c r="I12" s="263"/>
-      <c r="J12" s="263"/>
-      <c r="K12" s="263"/>
-    </row>
-    <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="221"/>
+      <c r="I12" s="222"/>
+      <c r="J12" s="222"/>
+      <c r="K12" s="222"/>
+    </row>
+    <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="132"/>
       <c r="B13" s="131"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" s="130">
         <v>1</v>
       </c>
@@ -4018,12 +4035,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="264" t="s">
+    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="223" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="265"/>
-      <c r="C15" s="266"/>
+      <c r="B15" s="224"/>
+      <c r="C15" s="225"/>
       <c r="D15" s="156"/>
       <c r="E15" s="156"/>
       <c r="F15" s="156"/>
@@ -4035,12 +4052,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="241" t="s">
+    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="226" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="242"/>
-      <c r="C16" s="243"/>
+      <c r="B16" s="227"/>
+      <c r="C16" s="228"/>
       <c r="D16" s="156"/>
       <c r="E16" s="156"/>
       <c r="F16" s="156"/>
@@ -4052,12 +4069,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="241" t="s">
+    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="226" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="242"/>
-      <c r="C17" s="243"/>
+      <c r="B17" s="227"/>
+      <c r="C17" s="228"/>
       <c r="D17" s="156"/>
       <c r="E17" s="156"/>
       <c r="F17" s="156"/>
@@ -4069,12 +4086,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="238" t="s">
+    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="234" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="239"/>
-      <c r="C18" s="240"/>
+      <c r="B18" s="235"/>
+      <c r="C18" s="236"/>
       <c r="D18" s="156"/>
       <c r="E18" s="156"/>
       <c r="F18" s="156"/>
@@ -4086,12 +4103,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="241" t="s">
+    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="226" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="242"/>
-      <c r="C19" s="243"/>
+      <c r="B19" s="227"/>
+      <c r="C19" s="228"/>
       <c r="D19" s="156"/>
       <c r="E19" s="156"/>
       <c r="F19" s="156"/>
@@ -4103,12 +4120,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="241" t="s">
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="226" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="242"/>
-      <c r="C20" s="243"/>
+      <c r="B20" s="227"/>
+      <c r="C20" s="228"/>
       <c r="D20" s="156"/>
       <c r="E20" s="156"/>
       <c r="F20" s="156"/>
@@ -4120,10 +4137,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J21" s="129"/>
     </row>
-    <row r="22" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="128" t="s">
         <v>53</v>
       </c>
@@ -4140,7 +4157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="122"/>
       <c r="E23" s="125"/>
       <c r="G23" s="95" t="s">
@@ -4153,7 +4170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="123"/>
       <c r="B24" s="99"/>
       <c r="C24" s="99"/>
@@ -4162,12 +4179,12 @@
       <c r="F24" s="122"/>
       <c r="J24" s="121"/>
     </row>
-    <row r="25" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J25" s="95" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G26" s="120" t="s">
         <v>57</v>
       </c>
@@ -4178,7 +4195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E27" s="98"/>
       <c r="G27" s="97"/>
       <c r="H27" s="97"/>
@@ -4186,7 +4203,7 @@
       <c r="J27" s="95"/>
       <c r="K27" s="94"/>
     </row>
-    <row r="28" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="116" t="s">
         <v>91</v>
       </c>
@@ -4195,91 +4212,91 @@
       <c r="D28" s="115"/>
       <c r="E28" s="115"/>
       <c r="F28" s="115"/>
-      <c r="G28" s="244" t="s">
+      <c r="G28" s="237" t="s">
         <v>53</v>
       </c>
-      <c r="H28" s="245"/>
-      <c r="I28" s="246" t="s">
+      <c r="H28" s="238"/>
+      <c r="I28" s="239" t="s">
         <v>61</v>
       </c>
-      <c r="J28" s="247"/>
-      <c r="K28" s="248"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="224" t="s">
+      <c r="J28" s="240"/>
+      <c r="K28" s="241"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="242" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="250" t="s">
+      <c r="B29" s="245" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="250" t="s">
+      <c r="C29" s="245" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="250"/>
-      <c r="E29" s="251" t="s">
+      <c r="D29" s="245"/>
+      <c r="E29" s="247" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="252"/>
-      <c r="G29" s="253"/>
-      <c r="H29" s="254"/>
-      <c r="I29" s="255">
+      <c r="F29" s="248"/>
+      <c r="G29" s="249"/>
+      <c r="H29" s="250"/>
+      <c r="I29" s="251">
         <v>0.2</v>
       </c>
-      <c r="J29" s="258"/>
-      <c r="K29" s="260">
+      <c r="J29" s="254"/>
+      <c r="K29" s="256">
         <f>J29*0.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="249"/>
-      <c r="B30" s="250"/>
-      <c r="C30" s="250" t="s">
+    <row r="30" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="243"/>
+      <c r="B30" s="245"/>
+      <c r="C30" s="245" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="250"/>
-      <c r="E30" s="217" t="s">
+      <c r="D30" s="245"/>
+      <c r="E30" s="258" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="218"/>
-      <c r="G30" s="231"/>
-      <c r="H30" s="232"/>
-      <c r="I30" s="256"/>
-      <c r="J30" s="258"/>
-      <c r="K30" s="260"/>
-    </row>
-    <row r="31" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="225"/>
-      <c r="B31" s="216"/>
-      <c r="C31" s="216" t="s">
+      <c r="F30" s="259"/>
+      <c r="G30" s="260"/>
+      <c r="H30" s="261"/>
+      <c r="I30" s="252"/>
+      <c r="J30" s="254"/>
+      <c r="K30" s="256"/>
+    </row>
+    <row r="31" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="244"/>
+      <c r="B31" s="246"/>
+      <c r="C31" s="246" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="216"/>
-      <c r="E31" s="217" t="s">
+      <c r="D31" s="246"/>
+      <c r="E31" s="258" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="218"/>
-      <c r="G31" s="219"/>
-      <c r="H31" s="220"/>
-      <c r="I31" s="257"/>
-      <c r="J31" s="259"/>
-      <c r="K31" s="261"/>
-    </row>
-    <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="224" t="s">
+      <c r="F31" s="259"/>
+      <c r="G31" s="262"/>
+      <c r="H31" s="263"/>
+      <c r="I31" s="253"/>
+      <c r="J31" s="255"/>
+      <c r="K31" s="257"/>
+    </row>
+    <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="242" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="226" t="s">
+      <c r="B32" s="267" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="227"/>
-      <c r="D32" s="228"/>
-      <c r="E32" s="229" t="s">
+      <c r="C32" s="268"/>
+      <c r="D32" s="269"/>
+      <c r="E32" s="270" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="230"/>
-      <c r="G32" s="231"/>
-      <c r="H32" s="232"/>
+      <c r="F32" s="271"/>
+      <c r="G32" s="260"/>
+      <c r="H32" s="261"/>
       <c r="I32" s="114">
         <v>0.4</v>
       </c>
@@ -4289,19 +4306,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="225"/>
-      <c r="B33" s="233" t="s">
+    <row r="33" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="244"/>
+      <c r="B33" s="272" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="234"/>
-      <c r="D33" s="235"/>
-      <c r="E33" s="236" t="s">
+      <c r="C33" s="273"/>
+      <c r="D33" s="274"/>
+      <c r="E33" s="275" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="237"/>
-      <c r="G33" s="231"/>
-      <c r="H33" s="232"/>
+      <c r="F33" s="276"/>
+      <c r="G33" s="260"/>
+      <c r="H33" s="261"/>
       <c r="I33" s="114">
         <v>0.4</v>
       </c>
@@ -4311,24 +4328,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="221" t="s">
+      <c r="B34" s="264" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="222"/>
-      <c r="D34" s="222"/>
-      <c r="E34" s="222"/>
-      <c r="F34" s="222"/>
-      <c r="G34" s="222"/>
-      <c r="H34" s="222"/>
-      <c r="I34" s="223"/>
+      <c r="C34" s="265"/>
+      <c r="D34" s="265"/>
+      <c r="E34" s="265"/>
+      <c r="F34" s="265"/>
+      <c r="G34" s="265"/>
+      <c r="H34" s="265"/>
+      <c r="I34" s="266"/>
       <c r="J34" s="160"/>
       <c r="K34" s="159"/>
     </row>
-    <row r="35" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G35" s="109"/>
       <c r="H35" s="109"/>
       <c r="I35" s="110"/>
@@ -4340,7 +4357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G36" s="109"/>
       <c r="H36" s="109"/>
       <c r="I36" s="108"/>
@@ -4352,7 +4369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G37" s="109"/>
       <c r="H37" s="109"/>
       <c r="I37" s="108" t="s">
@@ -4364,7 +4381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E38" s="98"/>
       <c r="G38" s="97"/>
       <c r="H38" s="105"/>
@@ -4379,8 +4396,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="99" t="s">
         <v>30</v>
       </c>
@@ -4396,7 +4413,7 @@
       <c r="J40" s="99"/>
       <c r="K40" s="99"/>
     </row>
-    <row r="41" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E41" s="98"/>
       <c r="G41" s="97"/>
       <c r="H41" s="97"/>
@@ -4404,25 +4421,21 @@
       <c r="J41" s="95"/>
       <c r="K41" s="94"/>
     </row>
-    <row r="46" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="G28:H28"/>
@@ -4439,17 +4452,21 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
   </mergeCells>
   <conditionalFormatting sqref="K29:K37">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
@@ -4471,6 +4488,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LAGKLASS</oddHeader>
+    <oddFooter>&amp;R2019-03-28</oddFooter>
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>
@@ -4483,27 +4501,27 @@
   </sheetPr>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.265625" style="93" customWidth="1"/>
-    <col min="2" max="3" width="9.1328125" style="93"/>
-    <col min="4" max="4" width="2.73046875" style="93" customWidth="1"/>
-    <col min="5" max="6" width="7.265625" style="93" customWidth="1"/>
-    <col min="7" max="7" width="6.86328125" style="93" customWidth="1"/>
-    <col min="8" max="8" width="6.59765625" style="93" customWidth="1"/>
-    <col min="9" max="9" width="6.1328125" style="93" customWidth="1"/>
-    <col min="10" max="11" width="7.265625" style="93" customWidth="1"/>
-    <col min="12" max="12" width="8.73046875" style="93" customWidth="1"/>
-    <col min="13" max="13" width="7.265625" style="93" hidden="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1328125" style="93"/>
+    <col min="1" max="1" width="8.28515625" style="93" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="93"/>
+    <col min="4" max="4" width="2.7109375" style="93" customWidth="1"/>
+    <col min="5" max="6" width="7.28515625" style="93" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" style="93" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="93" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="93" customWidth="1"/>
+    <col min="10" max="11" width="7.28515625" style="93" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="93" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" style="93" hidden="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="93"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="142" t="s">
         <v>116</v>
       </c>
@@ -4515,7 +4533,7 @@
       <c r="K2" s="135"/>
       <c r="L2" s="135"/>
     </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="141" t="s">
         <v>98</v>
       </c>
@@ -4527,14 +4545,14 @@
       <c r="K3" s="135"/>
       <c r="L3" s="135"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="99"/>
-      <c r="C4" s="271"/>
-      <c r="D4" s="271"/>
-      <c r="E4" s="271"/>
+      <c r="C4" s="233"/>
+      <c r="D4" s="233"/>
+      <c r="E4" s="233"/>
       <c r="F4" s="140"/>
       <c r="H4" s="138"/>
       <c r="I4" s="137" t="s">
@@ -4544,15 +4562,15 @@
       <c r="K4" s="135"/>
       <c r="L4" s="135"/>
     </row>
-    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="133" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="133"/>
-      <c r="C5" s="268"/>
-      <c r="D5" s="268"/>
-      <c r="E5" s="268"/>
-      <c r="F5" s="268"/>
+      <c r="C5" s="230"/>
+      <c r="D5" s="230"/>
+      <c r="E5" s="230"/>
+      <c r="F5" s="230"/>
       <c r="H5" s="138"/>
       <c r="I5" s="137" t="s">
         <v>11</v>
@@ -4561,7 +4579,7 @@
       <c r="K5" s="135"/>
       <c r="L5" s="135"/>
     </row>
-    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="93" t="s">
         <v>62</v>
       </c>
@@ -4569,98 +4587,98 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="133" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="133"/>
-      <c r="C7" s="268"/>
-      <c r="D7" s="268"/>
-      <c r="E7" s="268"/>
-      <c r="F7" s="268"/>
+      <c r="C7" s="230"/>
+      <c r="D7" s="230"/>
+      <c r="E7" s="230"/>
+      <c r="F7" s="230"/>
       <c r="H7" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="269"/>
-      <c r="J7" s="270"/>
-      <c r="K7" s="270"/>
-      <c r="L7" s="270"/>
-    </row>
-    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="231"/>
+      <c r="J7" s="232"/>
+      <c r="K7" s="232"/>
+      <c r="L7" s="232"/>
+    </row>
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="99" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="99"/>
-      <c r="C8" s="271"/>
-      <c r="D8" s="271"/>
-      <c r="E8" s="271"/>
-      <c r="F8" s="271"/>
+      <c r="C8" s="233"/>
+      <c r="D8" s="233"/>
+      <c r="E8" s="233"/>
+      <c r="F8" s="233"/>
       <c r="H8" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="262"/>
-      <c r="J8" s="263"/>
-      <c r="K8" s="263"/>
-      <c r="L8" s="263"/>
-    </row>
-    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="221"/>
+      <c r="J8" s="222"/>
+      <c r="K8" s="222"/>
+      <c r="L8" s="222"/>
+    </row>
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="133" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="133"/>
-      <c r="C9" s="268"/>
-      <c r="D9" s="268"/>
-      <c r="E9" s="268"/>
-      <c r="F9" s="268"/>
+      <c r="C9" s="230"/>
+      <c r="D9" s="230"/>
+      <c r="E9" s="230"/>
+      <c r="F9" s="230"/>
       <c r="H9" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="262"/>
-      <c r="J9" s="263"/>
-      <c r="K9" s="263"/>
-      <c r="L9" s="263"/>
-    </row>
-    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="221"/>
+      <c r="J9" s="222"/>
+      <c r="K9" s="222"/>
+      <c r="L9" s="222"/>
+    </row>
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="133" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="133"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
+      <c r="C10" s="230"/>
+      <c r="D10" s="230"/>
+      <c r="E10" s="230"/>
+      <c r="F10" s="230"/>
       <c r="H10" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="262"/>
-      <c r="J10" s="263"/>
-      <c r="K10" s="263"/>
-      <c r="L10" s="263"/>
-    </row>
-    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="221"/>
+      <c r="J10" s="222"/>
+      <c r="K10" s="222"/>
+      <c r="L10" s="222"/>
+    </row>
+    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H11" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="262"/>
-      <c r="J11" s="263"/>
-      <c r="K11" s="263"/>
-      <c r="L11" s="263"/>
-    </row>
-    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="221"/>
+      <c r="J11" s="222"/>
+      <c r="K11" s="222"/>
+      <c r="L11" s="222"/>
+    </row>
+    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="134"/>
       <c r="H12" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="262"/>
-      <c r="J12" s="263"/>
-      <c r="K12" s="263"/>
-      <c r="L12" s="263"/>
-    </row>
-    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="221"/>
+      <c r="J12" s="222"/>
+      <c r="K12" s="222"/>
+      <c r="L12" s="222"/>
+    </row>
+    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="132"/>
       <c r="B13" s="131"/>
     </row>
-    <row r="14" spans="1:12" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="116" t="s">
         <v>91</v>
       </c>
@@ -4670,97 +4688,97 @@
       <c r="E14" s="115"/>
       <c r="F14" s="115"/>
       <c r="G14" s="115"/>
-      <c r="H14" s="244" t="s">
+      <c r="H14" s="237" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="245"/>
-      <c r="J14" s="246" t="s">
+      <c r="I14" s="238"/>
+      <c r="J14" s="239" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="247"/>
-      <c r="L14" s="248"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="287" t="s">
+      <c r="K14" s="240"/>
+      <c r="L14" s="241"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="277" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="300" t="s">
+      <c r="B15" s="280" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="300" t="s">
+      <c r="C15" s="280" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="300"/>
-      <c r="E15" s="300"/>
-      <c r="F15" s="292" t="s">
+      <c r="D15" s="280"/>
+      <c r="E15" s="280"/>
+      <c r="F15" s="282" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="302"/>
-      <c r="H15" s="253"/>
-      <c r="I15" s="254"/>
-      <c r="J15" s="255">
+      <c r="G15" s="283"/>
+      <c r="H15" s="249"/>
+      <c r="I15" s="250"/>
+      <c r="J15" s="251">
         <v>0.2</v>
       </c>
-      <c r="K15" s="258">
+      <c r="K15" s="254">
         <v>0</v>
       </c>
-      <c r="L15" s="260">
+      <c r="L15" s="256">
         <f>K15*0.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="299"/>
-      <c r="B16" s="300"/>
-      <c r="C16" s="300" t="s">
+    <row r="16" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="278"/>
+      <c r="B16" s="280"/>
+      <c r="C16" s="280" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="300"/>
-      <c r="E16" s="300"/>
-      <c r="F16" s="303" t="s">
+      <c r="D16" s="280"/>
+      <c r="E16" s="280"/>
+      <c r="F16" s="284" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="304"/>
-      <c r="H16" s="231"/>
-      <c r="I16" s="232"/>
-      <c r="J16" s="256"/>
-      <c r="K16" s="258"/>
-      <c r="L16" s="260"/>
-    </row>
-    <row r="17" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="288"/>
-      <c r="B17" s="301"/>
-      <c r="C17" s="301" t="s">
+      <c r="G16" s="285"/>
+      <c r="H16" s="260"/>
+      <c r="I16" s="261"/>
+      <c r="J16" s="252"/>
+      <c r="K16" s="254"/>
+      <c r="L16" s="256"/>
+    </row>
+    <row r="17" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="279"/>
+      <c r="B17" s="281"/>
+      <c r="C17" s="281" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="301"/>
-      <c r="E17" s="301"/>
-      <c r="F17" s="303" t="s">
+      <c r="D17" s="281"/>
+      <c r="E17" s="281"/>
+      <c r="F17" s="284" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="304"/>
-      <c r="H17" s="219"/>
-      <c r="I17" s="220"/>
-      <c r="J17" s="257"/>
-      <c r="K17" s="259"/>
-      <c r="L17" s="261"/>
-    </row>
-    <row r="18" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="287" t="s">
+      <c r="G17" s="285"/>
+      <c r="H17" s="262"/>
+      <c r="I17" s="263"/>
+      <c r="J17" s="253"/>
+      <c r="K17" s="255"/>
+      <c r="L17" s="257"/>
+    </row>
+    <row r="18" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="277" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="289" t="s">
+      <c r="B18" s="286" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="290"/>
-      <c r="D18" s="290"/>
-      <c r="E18" s="291"/>
-      <c r="F18" s="292" t="s">
+      <c r="C18" s="287"/>
+      <c r="D18" s="287"/>
+      <c r="E18" s="288"/>
+      <c r="F18" s="282" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="293"/>
-      <c r="H18" s="231"/>
-      <c r="I18" s="232"/>
+      <c r="G18" s="289"/>
+      <c r="H18" s="260"/>
+      <c r="I18" s="261"/>
       <c r="J18" s="114">
         <v>0.4</v>
       </c>
@@ -4773,20 +4791,20 @@
       </c>
       <c r="M18" s="143"/>
     </row>
-    <row r="19" spans="1:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="288"/>
-      <c r="B19" s="294" t="s">
+    <row r="19" spans="1:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="279"/>
+      <c r="B19" s="290" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="295"/>
-      <c r="D19" s="295"/>
-      <c r="E19" s="296"/>
-      <c r="F19" s="297" t="s">
+      <c r="C19" s="291"/>
+      <c r="D19" s="291"/>
+      <c r="E19" s="292"/>
+      <c r="F19" s="293" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="298"/>
-      <c r="H19" s="231"/>
-      <c r="I19" s="232"/>
+      <c r="G19" s="294"/>
+      <c r="H19" s="260"/>
+      <c r="I19" s="261"/>
       <c r="J19" s="114">
         <v>0.4</v>
       </c>
@@ -4798,25 +4816,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="13.15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="221" t="s">
+      <c r="B20" s="264" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="222"/>
-      <c r="D20" s="222"/>
-      <c r="E20" s="222"/>
-      <c r="F20" s="222"/>
-      <c r="G20" s="222"/>
-      <c r="H20" s="222"/>
-      <c r="I20" s="222"/>
-      <c r="J20" s="223"/>
+      <c r="C20" s="265"/>
+      <c r="D20" s="265"/>
+      <c r="E20" s="265"/>
+      <c r="F20" s="265"/>
+      <c r="G20" s="265"/>
+      <c r="H20" s="265"/>
+      <c r="I20" s="265"/>
+      <c r="J20" s="266"/>
       <c r="K20" s="113"/>
       <c r="L20" s="161"/>
     </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H21" s="109"/>
       <c r="I21" s="109"/>
       <c r="L21" s="144">
@@ -4824,96 +4842,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="142" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="278" t="s">
+    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="295" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="279"/>
-      <c r="C23" s="279"/>
-      <c r="D23" s="279"/>
-      <c r="E23" s="279"/>
-      <c r="F23" s="279"/>
-      <c r="G23" s="279"/>
-      <c r="H23" s="279"/>
-      <c r="I23" s="279"/>
-      <c r="J23" s="279"/>
-      <c r="K23" s="279"/>
-      <c r="L23" s="280"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="281"/>
-      <c r="B24" s="282"/>
-      <c r="C24" s="282"/>
-      <c r="D24" s="282"/>
-      <c r="E24" s="282"/>
-      <c r="F24" s="282"/>
-      <c r="G24" s="282"/>
-      <c r="H24" s="282"/>
-      <c r="I24" s="282"/>
-      <c r="J24" s="282"/>
-      <c r="K24" s="282"/>
-      <c r="L24" s="283"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="281"/>
-      <c r="B25" s="282"/>
-      <c r="C25" s="282"/>
-      <c r="D25" s="282"/>
-      <c r="E25" s="282"/>
-      <c r="F25" s="282"/>
-      <c r="G25" s="282"/>
-      <c r="H25" s="282"/>
-      <c r="I25" s="282"/>
-      <c r="J25" s="282"/>
-      <c r="K25" s="282"/>
-      <c r="L25" s="283"/>
-    </row>
-    <row r="26" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="281"/>
-      <c r="B26" s="282"/>
-      <c r="C26" s="282"/>
-      <c r="D26" s="282"/>
-      <c r="E26" s="282"/>
-      <c r="F26" s="282"/>
-      <c r="G26" s="282"/>
-      <c r="H26" s="282"/>
-      <c r="I26" s="282"/>
-      <c r="J26" s="282"/>
-      <c r="K26" s="282"/>
-      <c r="L26" s="283"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="284"/>
-      <c r="B27" s="285"/>
-      <c r="C27" s="285"/>
-      <c r="D27" s="285"/>
-      <c r="E27" s="285"/>
-      <c r="F27" s="285"/>
-      <c r="G27" s="285"/>
-      <c r="H27" s="285"/>
-      <c r="I27" s="285"/>
-      <c r="J27" s="285"/>
-      <c r="K27" s="285"/>
-      <c r="L27" s="286"/>
-    </row>
-    <row r="29" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="275" t="s">
+      <c r="B23" s="296"/>
+      <c r="C23" s="296"/>
+      <c r="D23" s="296"/>
+      <c r="E23" s="296"/>
+      <c r="F23" s="296"/>
+      <c r="G23" s="296"/>
+      <c r="H23" s="296"/>
+      <c r="I23" s="296"/>
+      <c r="J23" s="296"/>
+      <c r="K23" s="296"/>
+      <c r="L23" s="297"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="298"/>
+      <c r="B24" s="299"/>
+      <c r="C24" s="299"/>
+      <c r="D24" s="299"/>
+      <c r="E24" s="299"/>
+      <c r="F24" s="299"/>
+      <c r="G24" s="299"/>
+      <c r="H24" s="299"/>
+      <c r="I24" s="299"/>
+      <c r="J24" s="299"/>
+      <c r="K24" s="299"/>
+      <c r="L24" s="300"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="298"/>
+      <c r="B25" s="299"/>
+      <c r="C25" s="299"/>
+      <c r="D25" s="299"/>
+      <c r="E25" s="299"/>
+      <c r="F25" s="299"/>
+      <c r="G25" s="299"/>
+      <c r="H25" s="299"/>
+      <c r="I25" s="299"/>
+      <c r="J25" s="299"/>
+      <c r="K25" s="299"/>
+      <c r="L25" s="300"/>
+    </row>
+    <row r="26" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="298"/>
+      <c r="B26" s="299"/>
+      <c r="C26" s="299"/>
+      <c r="D26" s="299"/>
+      <c r="E26" s="299"/>
+      <c r="F26" s="299"/>
+      <c r="G26" s="299"/>
+      <c r="H26" s="299"/>
+      <c r="I26" s="299"/>
+      <c r="J26" s="299"/>
+      <c r="K26" s="299"/>
+      <c r="L26" s="300"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="301"/>
+      <c r="B27" s="302"/>
+      <c r="C27" s="302"/>
+      <c r="D27" s="302"/>
+      <c r="E27" s="302"/>
+      <c r="F27" s="302"/>
+      <c r="G27" s="302"/>
+      <c r="H27" s="302"/>
+      <c r="I27" s="302"/>
+      <c r="J27" s="302"/>
+      <c r="K27" s="302"/>
+      <c r="L27" s="303"/>
+    </row>
+    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="304" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="275"/>
-      <c r="C29" s="275"/>
-      <c r="D29" s="275"/>
-      <c r="E29" s="275"/>
-      <c r="F29" s="275"/>
-      <c r="G29" s="275"/>
-      <c r="H29" s="275"/>
-      <c r="I29" s="276"/>
-      <c r="J29" s="276"/>
+      <c r="B29" s="304"/>
+      <c r="C29" s="304"/>
+      <c r="D29" s="304"/>
+      <c r="E29" s="304"/>
+      <c r="F29" s="304"/>
+      <c r="G29" s="304"/>
+      <c r="H29" s="304"/>
+      <c r="I29" s="305"/>
+      <c r="J29" s="305"/>
       <c r="K29" s="145" t="s">
         <v>103</v>
       </c>
@@ -4922,19 +4940,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="275" t="s">
+    <row r="30" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="304" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="275"/>
-      <c r="C30" s="275"/>
-      <c r="D30" s="275"/>
-      <c r="E30" s="275"/>
-      <c r="F30" s="275"/>
-      <c r="G30" s="275"/>
-      <c r="H30" s="275"/>
-      <c r="I30" s="276"/>
-      <c r="J30" s="276"/>
+      <c r="B30" s="304"/>
+      <c r="C30" s="304"/>
+      <c r="D30" s="304"/>
+      <c r="E30" s="304"/>
+      <c r="F30" s="304"/>
+      <c r="G30" s="304"/>
+      <c r="H30" s="304"/>
+      <c r="I30" s="305"/>
+      <c r="J30" s="305"/>
       <c r="K30" s="130" t="s">
         <v>103</v>
       </c>
@@ -4943,19 +4961,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="275" t="s">
+    <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="304" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="275"/>
-      <c r="C31" s="275"/>
-      <c r="D31" s="275"/>
-      <c r="E31" s="275"/>
-      <c r="F31" s="275"/>
-      <c r="G31" s="275"/>
-      <c r="H31" s="275"/>
-      <c r="I31" s="276"/>
-      <c r="J31" s="276"/>
+      <c r="B31" s="304"/>
+      <c r="C31" s="304"/>
+      <c r="D31" s="304"/>
+      <c r="E31" s="304"/>
+      <c r="F31" s="304"/>
+      <c r="G31" s="304"/>
+      <c r="H31" s="304"/>
+      <c r="I31" s="305"/>
+      <c r="J31" s="305"/>
       <c r="K31" s="130" t="s">
         <v>106</v>
       </c>
@@ -4964,19 +4982,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="275" t="s">
+    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="304" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="275"/>
-      <c r="C32" s="275"/>
-      <c r="D32" s="275"/>
-      <c r="E32" s="275"/>
-      <c r="F32" s="275"/>
-      <c r="G32" s="275"/>
-      <c r="H32" s="275"/>
-      <c r="I32" s="276"/>
-      <c r="J32" s="276"/>
+      <c r="B32" s="304"/>
+      <c r="C32" s="304"/>
+      <c r="D32" s="304"/>
+      <c r="E32" s="304"/>
+      <c r="F32" s="304"/>
+      <c r="G32" s="304"/>
+      <c r="H32" s="304"/>
+      <c r="I32" s="305"/>
+      <c r="J32" s="305"/>
       <c r="K32" s="130" t="s">
         <v>84</v>
       </c>
@@ -4985,22 +5003,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="275" t="s">
+    <row r="33" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="304" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="275"/>
-      <c r="C33" s="275"/>
-      <c r="D33" s="275"/>
-      <c r="E33" s="275"/>
-      <c r="F33" s="275"/>
-      <c r="G33" s="275"/>
-      <c r="H33" s="275"/>
-      <c r="I33" s="277">
+      <c r="B33" s="304"/>
+      <c r="C33" s="304"/>
+      <c r="D33" s="304"/>
+      <c r="E33" s="304"/>
+      <c r="F33" s="304"/>
+      <c r="G33" s="304"/>
+      <c r="H33" s="304"/>
+      <c r="I33" s="309">
         <f>L21</f>
         <v>0</v>
       </c>
-      <c r="J33" s="277"/>
+      <c r="J33" s="309"/>
       <c r="K33" s="130" t="s">
         <v>106</v>
       </c>
@@ -5009,7 +5027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F34" s="141"/>
       <c r="I34" s="109"/>
       <c r="J34" s="147"/>
@@ -5021,21 +5039,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F35" s="272" t="s">
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="306" t="s">
         <v>110</v>
       </c>
-      <c r="G35" s="273"/>
-      <c r="H35" s="273"/>
-      <c r="I35" s="273"/>
-      <c r="J35" s="273"/>
-      <c r="K35" s="274"/>
+      <c r="G35" s="307"/>
+      <c r="H35" s="307"/>
+      <c r="I35" s="307"/>
+      <c r="J35" s="307"/>
+      <c r="K35" s="308"/>
       <c r="L35" s="149">
         <f>L34/10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="F36" s="141"/>
       <c r="G36" s="141"/>
       <c r="H36" s="141"/>
@@ -5044,7 +5062,7 @@
       <c r="K36" s="141"/>
       <c r="L36" s="150"/>
     </row>
-    <row r="37" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="F37" s="141"/>
       <c r="G37" s="141"/>
       <c r="H37" s="141"/>
@@ -5053,7 +5071,7 @@
       <c r="K37" s="141"/>
       <c r="L37" s="150"/>
     </row>
-    <row r="38" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="F38" s="141"/>
       <c r="G38" s="141"/>
       <c r="H38" s="141"/>
@@ -5062,7 +5080,7 @@
       <c r="K38" s="141"/>
       <c r="L38" s="150"/>
     </row>
-    <row r="39" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
       <c r="F39" s="141"/>
       <c r="G39" s="141"/>
       <c r="H39" s="141"/>
@@ -5071,7 +5089,7 @@
       <c r="K39" s="141"/>
       <c r="L39" s="150"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F40" s="98"/>
       <c r="H40" s="97"/>
       <c r="I40" s="97"/>
@@ -5079,7 +5097,7 @@
       <c r="K40" s="95"/>
       <c r="L40" s="94"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="99" t="s">
         <v>30</v>
       </c>
@@ -5096,7 +5114,7 @@
       <c r="K42" s="99"/>
       <c r="L42" s="99"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="F43" s="98"/>
       <c r="H43" s="97"/>
       <c r="I43" s="97"/>
@@ -5104,7 +5122,7 @@
       <c r="K43" s="95"/>
       <c r="L43" s="94"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="143"/>
       <c r="B44" s="143"/>
       <c r="C44" s="143"/>
@@ -5120,18 +5138,26 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="A23:L27"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="A15:A17"/>
@@ -5148,26 +5174,18 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="A23:L27"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
   </mergeCells>
   <conditionalFormatting sqref="L15:L39 I33:J33">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
@@ -5186,21 +5204,22 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="98" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LAGKLASS</oddHeader>
+    <oddFooter>&amp;R2019-03-28</oddFooter>
   </headerFooter>
   <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5270,18 +5289,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64838F1D-7ECA-4F32-944F-43492487C498}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5304,16 +5330,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64838F1D-7ECA-4F32-944F-43492487C498}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tävling okt Jälla 2019
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll_2019_mixklass lag(mall).xlsx
+++ b/mallar/Protokoll/Protokoll_2019_mixklass lag(mall).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Protokoll 2019\Mallar 2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magnus.sandberg\Documents\Visual Studio 2015\Projects\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F7EE67-D24E-4F21-AF7F-1E5E22C4BB6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="13095"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="27" r:id="rId1"/>
@@ -54,7 +55,7 @@
     <definedName name="result" localSheetId="3">'Mixklass E grund'!$K$38</definedName>
     <definedName name="result" localSheetId="4">'Mixklass lagkür typ 2'!$L$35</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -495,16 +496,16 @@
     <t>3-6 voltigörer</t>
   </si>
   <si>
-    <t>Protokollen uppdaterades senast 2019-03-28.</t>
+    <t xml:space="preserve">Protokollen uppdaterades senast 2019-09-29. (justering information domare A mixklass E grund) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_-;\-* #,##0.00\ _k_r_-;_-* &quot;-&quot;??\ _k_r_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _k_r_-;\-* #,##0.00\ _k_r_-;_-* &quot;-&quot;??\ _k_r_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
@@ -1301,14 +1302,14 @@
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1665,7 +1666,7 @@
     <xf numFmtId="167" fontId="3" fillId="0" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1711,103 +1712,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1817,12 +1726,23 @@
     <xf numFmtId="167" fontId="8" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="169" fontId="4" fillId="2" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1838,32 +1758,253 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="21" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1878,15 +2019,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1900,217 +2032,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="2" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="2" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="12" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="33" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2119,30 +2048,102 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="3" fillId="0" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="38" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Dezimal 2" xfId="2"/>
-    <cellStyle name="Dezimal 2 2" xfId="4"/>
-    <cellStyle name="Excel Built-in Normal" xfId="6"/>
+    <cellStyle name="Dezimal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Dezimal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 3" xfId="7"/>
-    <cellStyle name="Standard 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Standard 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Tusental" xfId="1" builtinId="3"/>
-    <cellStyle name="Tusental 2" xfId="8"/>
+    <cellStyle name="Tusental 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -2295,6 +2296,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2330,6 +2348,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2505,75 +2540,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="18" width="15.7109375" customWidth="1"/>
+    <col min="1" max="18" width="15.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="84" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="84" customFormat="1" ht="20.65" x14ac:dyDescent="0.6">
       <c r="A1" s="83" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="84" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="84" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="84" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="152" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="152" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="310" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="152" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="152" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="152" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="152" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:5" s="84" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:5" s="76" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="152" customFormat="1" ht="14.25" x14ac:dyDescent="0.45"/>
+    <row r="6" spans="1:5" s="84" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:5" s="76" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A7" s="76" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="77" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="77" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="77" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="77" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="77" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="77"/>
     </row>
-    <row r="13" spans="1:5" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="78" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A13" s="78" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="79" t="s">
         <v>69</v>
       </c>
       <c r="C14" s="77"/>
     </row>
-    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="163" t="s">
         <v>70</v>
       </c>
@@ -2584,7 +2619,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="77" t="s">
         <v>112</v>
       </c>
@@ -2599,7 +2634,7 @@
       </c>
       <c r="E16" s="155"/>
     </row>
-    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="77"/>
       <c r="B17" s="80" t="s">
         <v>114</v>
@@ -2609,18 +2644,18 @@
       </c>
       <c r="D17" s="151"/>
     </row>
-    <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="77"/>
       <c r="B18" s="153"/>
       <c r="C18" s="153"/>
       <c r="D18" s="154"/>
     </row>
-    <row r="19" spans="1:8" s="152" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="152" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="165" t="s">
-        <v>72</v>
+      <c r="B19" s="166" t="s">
+        <v>111</v>
       </c>
       <c r="C19" s="166" t="s">
         <v>111</v>
@@ -2632,7 +2667,7 @@
       <c r="F19" s="154"/>
       <c r="G19" s="154"/>
     </row>
-    <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="77"/>
       <c r="B20" s="80" t="s">
         <v>114</v>
@@ -2645,7 +2680,7 @@
       <c r="F20" s="153"/>
       <c r="G20" s="153"/>
     </row>
-    <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="77"/>
       <c r="B21" s="153"/>
       <c r="C21" s="153"/>
@@ -2655,24 +2690,24 @@
       <c r="G21" s="153"/>
       <c r="H21" s="153"/>
     </row>
-    <row r="25" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N34" s="79"/>
     </row>
-    <row r="35" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="N35" s="78"/>
       <c r="O35" s="78"/>
       <c r="P35" s="78"/>
       <c r="Q35" s="78"/>
     </row>
-    <row r="36" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:17" s="84" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:17" s="84" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -2687,7 +2722,7 @@
       <c r="L40"/>
       <c r="M40"/>
     </row>
-    <row r="41" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" s="82" customFormat="1" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -2702,7 +2737,7 @@
       <c r="L41"/>
       <c r="M41"/>
     </row>
-    <row r="42" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -2717,7 +2752,7 @@
       <c r="L42"/>
       <c r="M42"/>
     </row>
-    <row r="43" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -2732,7 +2767,7 @@
       <c r="L43"/>
       <c r="M43"/>
     </row>
-    <row r="44" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" s="81" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -2754,32 +2789,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" topLeftCell="A35" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="47" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="47" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="47" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" style="47" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" style="47" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="47" customWidth="1"/>
+    <col min="2" max="2" width="10.265625" style="47" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.73046875" style="47" customWidth="1"/>
+    <col min="5" max="5" width="7.265625" style="47" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" style="47" customWidth="1"/>
     <col min="7" max="7" width="7" style="47" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" style="47" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" style="47" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" style="47" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="47" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" style="47" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="47"/>
+    <col min="8" max="8" width="9.59765625" style="47" customWidth="1"/>
+    <col min="9" max="9" width="5.73046875" style="47" customWidth="1"/>
+    <col min="10" max="10" width="5.59765625" style="47" customWidth="1"/>
+    <col min="11" max="11" width="7.1328125" style="47" customWidth="1"/>
+    <col min="12" max="12" width="7.265625" style="47" customWidth="1"/>
+    <col min="13" max="16384" width="9.1328125" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>78</v>
       </c>
@@ -2791,7 +2826,7 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -2803,7 +2838,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -2819,14 +2854,14 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="193"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
       <c r="G5" s="9"/>
       <c r="H5" s="13" t="s">
         <v>11</v>
@@ -2835,19 +2870,19 @@
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="193"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
+      <c r="E6" s="167"/>
       <c r="G6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>62</v>
       </c>
@@ -2858,79 +2893,79 @@
       <c r="G7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="192"/>
-      <c r="I7" s="201"/>
-      <c r="J7" s="201"/>
-      <c r="K7" s="202"/>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="168"/>
+      <c r="I7" s="169"/>
+      <c r="J7" s="169"/>
+      <c r="K7" s="170"/>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="192"/>
-      <c r="D8" s="192"/>
-      <c r="E8" s="192"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="168"/>
+      <c r="E8" s="168"/>
       <c r="G8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="193"/>
-      <c r="I8" s="194"/>
-      <c r="J8" s="194"/>
-      <c r="K8" s="195"/>
-    </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="167"/>
+      <c r="I8" s="173"/>
+      <c r="J8" s="173"/>
+      <c r="K8" s="174"/>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="193"/>
-      <c r="D9" s="193"/>
-      <c r="E9" s="193"/>
+      <c r="C9" s="167"/>
+      <c r="D9" s="167"/>
+      <c r="E9" s="167"/>
       <c r="G9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="193"/>
-      <c r="I9" s="194"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="195"/>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="167"/>
+      <c r="I9" s="173"/>
+      <c r="J9" s="173"/>
+      <c r="K9" s="174"/>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="193"/>
-      <c r="D10" s="193"/>
-      <c r="E10" s="193"/>
+      <c r="C10" s="167"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="167"/>
       <c r="G10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="193"/>
-      <c r="I10" s="194"/>
-      <c r="J10" s="194"/>
-      <c r="K10" s="195"/>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="167"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="173"/>
+      <c r="K10" s="174"/>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="193"/>
-      <c r="I11" s="194"/>
-      <c r="J11" s="194"/>
-      <c r="K11" s="195"/>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="167"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="173"/>
+      <c r="K11" s="174"/>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="16"/>
       <c r="G12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="193"/>
-      <c r="I12" s="194"/>
-      <c r="J12" s="194"/>
-      <c r="K12" s="195"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="167"/>
+      <c r="I12" s="173"/>
+      <c r="J12" s="173"/>
+      <c r="K12" s="174"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="16"/>
       <c r="G13" s="3"/>
       <c r="H13" s="46"/>
@@ -2938,45 +2973,45 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="196" t="s">
+    <row r="14" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="185" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="197"/>
-      <c r="I14" s="198" t="s">
+      <c r="H14" s="186"/>
+      <c r="I14" s="187" t="s">
         <v>61</v>
       </c>
-      <c r="J14" s="199"/>
-      <c r="K14" s="200"/>
-    </row>
-    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="169" t="s">
+      <c r="J14" s="188"/>
+      <c r="K14" s="189"/>
+    </row>
+    <row r="15" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="183" t="s">
+      <c r="B15" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="183" t="s">
+      <c r="C15" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="183"/>
-      <c r="E15" s="186" t="s">
+      <c r="D15" s="193"/>
+      <c r="E15" s="194" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="187"/>
+      <c r="F15" s="195"/>
       <c r="G15" s="48"/>
       <c r="H15" s="49"/>
-      <c r="I15" s="175" t="s">
+      <c r="I15" s="196" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="207"/>
-      <c r="K15" s="205">
+      <c r="J15" s="180"/>
+      <c r="K15" s="175">
         <f>ROUND(J15*0.3,3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="170"/>
+    <row r="16" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="191"/>
       <c r="B16" s="177"/>
       <c r="C16" s="177" t="s">
         <v>21</v>
@@ -2988,12 +3023,12 @@
       <c r="F16" s="179"/>
       <c r="G16" s="50"/>
       <c r="H16" s="51"/>
-      <c r="I16" s="176"/>
-      <c r="J16" s="208"/>
-      <c r="K16" s="206"/>
-    </row>
-    <row r="17" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="170"/>
+      <c r="I16" s="197"/>
+      <c r="J16" s="181"/>
+      <c r="K16" s="176"/>
+    </row>
+    <row r="17" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="191"/>
       <c r="B17" s="177"/>
       <c r="C17" s="177" t="s">
         <v>20</v>
@@ -3005,13 +3040,13 @@
       <c r="F17" s="179"/>
       <c r="G17" s="52"/>
       <c r="H17" s="53"/>
-      <c r="I17" s="176"/>
-      <c r="J17" s="208"/>
-      <c r="K17" s="206"/>
-    </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="170"/>
-      <c r="B18" s="188" t="s">
+      <c r="I17" s="197"/>
+      <c r="J17" s="181"/>
+      <c r="K17" s="176"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="191"/>
+      <c r="B18" s="198" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="177" t="s">
@@ -3024,18 +3059,18 @@
       <c r="F18" s="179"/>
       <c r="G18" s="54"/>
       <c r="H18" s="55"/>
-      <c r="I18" s="176" t="s">
+      <c r="I18" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="J18" s="208"/>
-      <c r="K18" s="206">
+      <c r="J18" s="181"/>
+      <c r="K18" s="176">
         <f>ROUND(J18*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="170"/>
-      <c r="B19" s="189"/>
+    <row r="19" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="191"/>
+      <c r="B19" s="199"/>
       <c r="C19" s="177" t="s">
         <v>22</v>
       </c>
@@ -3046,56 +3081,56 @@
       <c r="F19" s="179"/>
       <c r="G19" s="50"/>
       <c r="H19" s="51"/>
-      <c r="I19" s="176"/>
-      <c r="J19" s="208"/>
-      <c r="K19" s="206"/>
-    </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="171"/>
-      <c r="B20" s="190"/>
-      <c r="C20" s="180" t="s">
+      <c r="I19" s="197"/>
+      <c r="J19" s="181"/>
+      <c r="K19" s="176"/>
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="192"/>
+      <c r="B20" s="200"/>
+      <c r="C20" s="202" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="180"/>
-      <c r="E20" s="181" t="s">
+      <c r="D20" s="202"/>
+      <c r="E20" s="203" t="s">
         <v>42</v>
       </c>
-      <c r="F20" s="182"/>
+      <c r="F20" s="204"/>
       <c r="G20" s="56"/>
       <c r="H20" s="57"/>
-      <c r="I20" s="191"/>
-      <c r="J20" s="209"/>
-      <c r="K20" s="210"/>
-    </row>
-    <row r="21" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="169" t="s">
+      <c r="I20" s="201"/>
+      <c r="J20" s="182"/>
+      <c r="K20" s="183"/>
+    </row>
+    <row r="21" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="190" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="172" t="s">
+      <c r="B21" s="207" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="183" t="s">
+      <c r="C21" s="193" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="183"/>
-      <c r="E21" s="184" t="s">
+      <c r="D21" s="193"/>
+      <c r="E21" s="210" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="185"/>
+      <c r="F21" s="211"/>
       <c r="G21" s="58"/>
       <c r="H21" s="59"/>
-      <c r="I21" s="175" t="s">
+      <c r="I21" s="196" t="s">
         <v>65</v>
       </c>
-      <c r="J21" s="207"/>
-      <c r="K21" s="205">
+      <c r="J21" s="180"/>
+      <c r="K21" s="175">
         <f>ROUND(J21*0.25,3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="170"/>
-      <c r="B22" s="173"/>
+    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="191"/>
+      <c r="B22" s="208"/>
       <c r="C22" s="177" t="s">
         <v>25</v>
       </c>
@@ -3106,13 +3141,13 @@
       <c r="F22" s="179"/>
       <c r="G22" s="50"/>
       <c r="H22" s="51"/>
-      <c r="I22" s="176"/>
-      <c r="J22" s="208"/>
-      <c r="K22" s="206"/>
-    </row>
-    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="170"/>
-      <c r="B23" s="174"/>
+      <c r="I22" s="197"/>
+      <c r="J22" s="181"/>
+      <c r="K22" s="176"/>
+    </row>
+    <row r="23" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="191"/>
+      <c r="B23" s="209"/>
       <c r="C23" s="177" t="s">
         <v>26</v>
       </c>
@@ -3123,21 +3158,21 @@
       <c r="F23" s="179"/>
       <c r="G23" s="52"/>
       <c r="H23" s="53"/>
-      <c r="I23" s="176"/>
-      <c r="J23" s="208"/>
-      <c r="K23" s="206"/>
-    </row>
-    <row r="24" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="171"/>
+      <c r="I23" s="197"/>
+      <c r="J23" s="181"/>
+      <c r="K23" s="176"/>
+    </row>
+    <row r="24" spans="1:11" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="192"/>
       <c r="B24" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="180"/>
-      <c r="D24" s="180"/>
-      <c r="E24" s="181" t="s">
+      <c r="C24" s="202"/>
+      <c r="D24" s="202"/>
+      <c r="E24" s="203" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="182"/>
+      <c r="F24" s="204"/>
       <c r="G24" s="61"/>
       <c r="H24" s="62"/>
       <c r="I24" s="63" t="s">
@@ -3149,21 +3184,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="64" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="211" t="s">
+      <c r="C25" s="184" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="211"/>
-      <c r="E25" s="167" t="s">
+      <c r="D25" s="184"/>
+      <c r="E25" s="205" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="168"/>
+      <c r="F25" s="206"/>
       <c r="G25" s="65"/>
       <c r="H25" s="66"/>
       <c r="I25" s="67" t="s">
@@ -3175,7 +3210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="69"/>
       <c r="B26" s="69"/>
       <c r="C26" s="69"/>
@@ -3188,7 +3223,7 @@
       <c r="J26" s="69"/>
       <c r="K26" s="69"/>
     </row>
-    <row r="27" spans="1:11" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="69"/>
       <c r="B27" s="69"/>
       <c r="C27" s="69"/>
@@ -3200,13 +3235,13 @@
         <v>10</v>
       </c>
       <c r="I27" s="71"/>
-      <c r="J27" s="203">
+      <c r="J27" s="171">
         <f>SUM(K15:K25)</f>
         <v>0</v>
       </c>
-      <c r="K27" s="204"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K27" s="172"/>
+    </row>
+    <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
@@ -3225,6 +3260,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="C6:E6"/>
@@ -3241,40 +3310,6 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="J21:J23"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3289,29 +3324,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="7.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="3" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="7.265625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" customWidth="1"/>
-    <col min="9" max="11" width="7.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="11" width="7.265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>78</v>
       </c>
@@ -3323,7 +3358,7 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
     </row>
-    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>79</v>
       </c>
@@ -3335,7 +3370,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -3352,15 +3387,15 @@
       <c r="K4" s="11"/>
       <c r="L4" s="91"/>
     </row>
-    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="12"/>
-      <c r="C5" s="193"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="167"/>
+      <c r="E5" s="167"/>
+      <c r="F5" s="167"/>
       <c r="H5" s="9"/>
       <c r="I5" s="13" t="s">
         <v>11</v>
@@ -3369,20 +3404,20 @@
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
     </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="12"/>
-      <c r="C6" s="193"/>
-      <c r="D6" s="193"/>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
+      <c r="C6" s="167"/>
+      <c r="D6" s="167"/>
+      <c r="E6" s="167"/>
+      <c r="F6" s="167"/>
       <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>62</v>
       </c>
@@ -3394,89 +3429,89 @@
       <c r="H7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="192"/>
-      <c r="J7" s="201"/>
-      <c r="K7" s="201"/>
-      <c r="L7" s="201"/>
-    </row>
-    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="168"/>
+      <c r="J7" s="169"/>
+      <c r="K7" s="169"/>
+      <c r="L7" s="169"/>
+    </row>
+    <row r="8" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="192"/>
-      <c r="D8" s="192"/>
-      <c r="E8" s="192"/>
-      <c r="F8" s="192"/>
+      <c r="C8" s="168"/>
+      <c r="D8" s="168"/>
+      <c r="E8" s="168"/>
+      <c r="F8" s="168"/>
       <c r="H8" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="193"/>
-      <c r="J8" s="194"/>
-      <c r="K8" s="194"/>
-      <c r="L8" s="194"/>
-    </row>
-    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="167"/>
+      <c r="J8" s="173"/>
+      <c r="K8" s="173"/>
+      <c r="L8" s="173"/>
+    </row>
+    <row r="9" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="193"/>
-      <c r="D9" s="193"/>
-      <c r="E9" s="193"/>
-      <c r="F9" s="193"/>
+      <c r="C9" s="167"/>
+      <c r="D9" s="167"/>
+      <c r="E9" s="167"/>
+      <c r="F9" s="167"/>
       <c r="H9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="193"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="194"/>
-      <c r="L9" s="194"/>
-    </row>
-    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="167"/>
+      <c r="J9" s="173"/>
+      <c r="K9" s="173"/>
+      <c r="L9" s="173"/>
+    </row>
+    <row r="10" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="193"/>
-      <c r="D10" s="193"/>
-      <c r="E10" s="193"/>
-      <c r="F10" s="193"/>
+      <c r="C10" s="167"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="167"/>
+      <c r="F10" s="167"/>
       <c r="H10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="193"/>
-      <c r="J10" s="194"/>
-      <c r="K10" s="194"/>
-      <c r="L10" s="194"/>
-    </row>
-    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="167"/>
+      <c r="J10" s="173"/>
+      <c r="K10" s="173"/>
+      <c r="L10" s="173"/>
+    </row>
+    <row r="11" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="193"/>
-      <c r="J11" s="194"/>
-      <c r="K11" s="194"/>
-      <c r="L11" s="194"/>
-    </row>
-    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="167"/>
+      <c r="J11" s="173"/>
+      <c r="K11" s="173"/>
+      <c r="L11" s="173"/>
+    </row>
+    <row r="12" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="16"/>
       <c r="H12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="193"/>
-      <c r="J12" s="194"/>
-      <c r="K12" s="194"/>
-      <c r="L12" s="194"/>
-    </row>
-    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="167"/>
+      <c r="J12" s="173"/>
+      <c r="K12" s="173"/>
+      <c r="L12" s="173"/>
+    </row>
+    <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
@@ -3491,7 +3526,7 @@
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F15" s="20">
         <v>1</v>
       </c>
@@ -3514,13 +3549,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="212"/>
-      <c r="B16" s="213" t="s">
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="219"/>
+      <c r="B16" s="220" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="214"/>
-      <c r="D16" s="214"/>
+      <c r="C16" s="213"/>
+      <c r="D16" s="213"/>
       <c r="E16" s="21"/>
       <c r="F16" s="90"/>
       <c r="G16" s="90"/>
@@ -3533,13 +3568,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="212"/>
-      <c r="B17" s="215" t="s">
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="219"/>
+      <c r="B17" s="212" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="214"/>
-      <c r="D17" s="214"/>
+      <c r="C17" s="213"/>
+      <c r="D17" s="213"/>
       <c r="E17" s="21"/>
       <c r="F17" s="90"/>
       <c r="G17" s="90"/>
@@ -3552,12 +3587,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="215" t="s">
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="212" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="214"/>
-      <c r="D18" s="214"/>
+      <c r="C18" s="213"/>
+      <c r="D18" s="213"/>
       <c r="E18" s="21"/>
       <c r="F18" s="90"/>
       <c r="G18" s="90"/>
@@ -3570,12 +3605,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="219" t="s">
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="217" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="214"/>
-      <c r="D19" s="214"/>
+      <c r="C19" s="213"/>
+      <c r="D19" s="213"/>
       <c r="E19" s="21"/>
       <c r="F19" s="90"/>
       <c r="G19" s="90"/>
@@ -3588,13 +3623,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="215" t="s">
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="212" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="214"/>
-      <c r="D20" s="214"/>
-      <c r="E20" s="220"/>
+      <c r="C20" s="213"/>
+      <c r="D20" s="213"/>
+      <c r="E20" s="218"/>
       <c r="F20" s="90"/>
       <c r="G20" s="90"/>
       <c r="H20" s="90"/>
@@ -3606,12 +3641,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="215" t="s">
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="212" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="214"/>
-      <c r="D21" s="214"/>
+      <c r="C21" s="213"/>
+      <c r="D21" s="213"/>
       <c r="E21" s="21"/>
       <c r="F21" s="90"/>
       <c r="G21" s="90"/>
@@ -3624,13 +3659,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="216" t="s">
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="214" t="s">
         <v>77</v>
       </c>
-      <c r="C22" s="217"/>
-      <c r="D22" s="217"/>
-      <c r="E22" s="218"/>
+      <c r="C22" s="215"/>
+      <c r="D22" s="215"/>
+      <c r="E22" s="216"/>
       <c r="F22" s="90"/>
       <c r="G22" s="90"/>
       <c r="H22" s="90"/>
@@ -3642,10 +3677,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L23" s="23"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="24" t="s">
         <v>53</v>
       </c>
@@ -3663,7 +3698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="28"/>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -3680,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26" s="28"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -3692,7 +3727,7 @@
       <c r="J26" s="33"/>
       <c r="L26" s="34"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" s="35"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3706,8 +3741,8 @@
       </c>
       <c r="L27" s="33"/>
     </row>
-    <row r="28" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:12" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H29" s="37"/>
       <c r="I29" s="38" t="s">
         <v>57</v>
@@ -3719,7 +3754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -3731,7 +3766,7 @@
       <c r="K30" s="27"/>
       <c r="L30" s="6"/>
     </row>
-    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -3743,8 +3778,8 @@
       <c r="K31" s="27"/>
       <c r="L31" s="6"/>
     </row>
-    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -3761,7 +3796,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
@@ -3773,7 +3808,7 @@
       <c r="K34" s="27"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="45"/>
       <c r="B35" s="45"/>
       <c r="C35" s="45"/>
@@ -3788,31 +3823,24 @@
       <c r="L35" s="45"/>
       <c r="M35" s="45"/>
     </row>
-    <row r="36" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:E20"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="I8:L8"/>
@@ -3825,6 +3853,13 @@
     <mergeCell ref="I10:L10"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3841,27 +3876,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A10" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" style="93" customWidth="1"/>
-    <col min="3" max="10" width="7.5703125" style="93" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" style="93" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="93" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="8.73046875" style="93" customWidth="1"/>
+    <col min="3" max="10" width="7.59765625" style="93" customWidth="1"/>
+    <col min="11" max="11" width="7.3984375" style="93" customWidth="1"/>
+    <col min="12" max="12" width="7.73046875" style="93" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="93"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="142" t="s">
         <v>80</v>
       </c>
@@ -3873,7 +3908,7 @@
       <c r="J2" s="135"/>
       <c r="K2" s="135"/>
     </row>
-    <row r="3" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="141" t="s">
         <v>75</v>
       </c>
@@ -3885,13 +3920,13 @@
       <c r="J3" s="135"/>
       <c r="K3" s="135"/>
     </row>
-    <row r="4" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="99"/>
-      <c r="C4" s="229"/>
-      <c r="D4" s="229"/>
+      <c r="C4" s="272"/>
+      <c r="D4" s="272"/>
       <c r="E4" s="140"/>
       <c r="G4" s="138"/>
       <c r="H4" s="137" t="s">
@@ -3901,14 +3936,14 @@
       <c r="J4" s="135"/>
       <c r="K4" s="135"/>
     </row>
-    <row r="5" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="133" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="133"/>
-      <c r="C5" s="230"/>
-      <c r="D5" s="230"/>
-      <c r="E5" s="230"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
       <c r="G5" s="138"/>
       <c r="H5" s="137" t="s">
         <v>11</v>
@@ -3917,7 +3952,7 @@
       <c r="J5" s="135"/>
       <c r="K5" s="135"/>
     </row>
-    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="93" t="s">
         <v>62</v>
       </c>
@@ -3925,94 +3960,94 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="133" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="133"/>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
+      <c r="C7" s="273"/>
+      <c r="D7" s="273"/>
+      <c r="E7" s="273"/>
       <c r="G7" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="231"/>
-      <c r="I7" s="232"/>
-      <c r="J7" s="232"/>
-      <c r="K7" s="232"/>
-    </row>
-    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="274"/>
+      <c r="I7" s="275"/>
+      <c r="J7" s="275"/>
+      <c r="K7" s="275"/>
+    </row>
+    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="99" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="99"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
+      <c r="C8" s="276"/>
+      <c r="D8" s="276"/>
+      <c r="E8" s="276"/>
       <c r="G8" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="221"/>
-      <c r="I8" s="222"/>
-      <c r="J8" s="222"/>
-      <c r="K8" s="222"/>
-    </row>
-    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="267"/>
+      <c r="I8" s="268"/>
+      <c r="J8" s="268"/>
+      <c r="K8" s="268"/>
+    </row>
+    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="133" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="133"/>
-      <c r="C9" s="230"/>
-      <c r="D9" s="230"/>
-      <c r="E9" s="230"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
       <c r="G9" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="221"/>
-      <c r="I9" s="222"/>
-      <c r="J9" s="222"/>
-      <c r="K9" s="222"/>
-    </row>
-    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="267"/>
+      <c r="I9" s="268"/>
+      <c r="J9" s="268"/>
+      <c r="K9" s="268"/>
+    </row>
+    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="133" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="133"/>
-      <c r="C10" s="230"/>
-      <c r="D10" s="230"/>
-      <c r="E10" s="230"/>
+      <c r="C10" s="273"/>
+      <c r="D10" s="273"/>
+      <c r="E10" s="273"/>
       <c r="G10" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="221"/>
-      <c r="I10" s="222"/>
-      <c r="J10" s="222"/>
-      <c r="K10" s="222"/>
-    </row>
-    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="267"/>
+      <c r="I10" s="268"/>
+      <c r="J10" s="268"/>
+      <c r="K10" s="268"/>
+    </row>
+    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="221"/>
-      <c r="I11" s="222"/>
-      <c r="J11" s="222"/>
-      <c r="K11" s="222"/>
-    </row>
-    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="267"/>
+      <c r="I11" s="268"/>
+      <c r="J11" s="268"/>
+      <c r="K11" s="268"/>
+    </row>
+    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="134"/>
       <c r="G12" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="221"/>
-      <c r="I12" s="222"/>
-      <c r="J12" s="222"/>
-      <c r="K12" s="222"/>
-    </row>
-    <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="267"/>
+      <c r="I12" s="268"/>
+      <c r="J12" s="268"/>
+      <c r="K12" s="268"/>
+    </row>
+    <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="132"/>
       <c r="B13" s="131"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="130">
         <v>1</v>
       </c>
@@ -4035,12 +4070,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="223" t="s">
+    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="269" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="224"/>
-      <c r="C15" s="225"/>
+      <c r="B15" s="270"/>
+      <c r="C15" s="271"/>
       <c r="D15" s="156"/>
       <c r="E15" s="156"/>
       <c r="F15" s="156"/>
@@ -4052,12 +4087,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="226" t="s">
+    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="246" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="227"/>
-      <c r="C16" s="228"/>
+      <c r="B16" s="247"/>
+      <c r="C16" s="248"/>
       <c r="D16" s="156"/>
       <c r="E16" s="156"/>
       <c r="F16" s="156"/>
@@ -4069,12 +4104,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="226" t="s">
+    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="246" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="227"/>
-      <c r="C17" s="228"/>
+      <c r="B17" s="247"/>
+      <c r="C17" s="248"/>
       <c r="D17" s="156"/>
       <c r="E17" s="156"/>
       <c r="F17" s="156"/>
@@ -4086,12 +4121,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="234" t="s">
+    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="243" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="235"/>
-      <c r="C18" s="236"/>
+      <c r="B18" s="244"/>
+      <c r="C18" s="245"/>
       <c r="D18" s="156"/>
       <c r="E18" s="156"/>
       <c r="F18" s="156"/>
@@ -4103,12 +4138,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="226" t="s">
+    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="246" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="227"/>
-      <c r="C19" s="228"/>
+      <c r="B19" s="247"/>
+      <c r="C19" s="248"/>
       <c r="D19" s="156"/>
       <c r="E19" s="156"/>
       <c r="F19" s="156"/>
@@ -4120,12 +4155,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="226" t="s">
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="246" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="227"/>
-      <c r="C20" s="228"/>
+      <c r="B20" s="247"/>
+      <c r="C20" s="248"/>
       <c r="D20" s="156"/>
       <c r="E20" s="156"/>
       <c r="F20" s="156"/>
@@ -4137,10 +4172,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="J21" s="129"/>
     </row>
-    <row r="22" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="128" t="s">
         <v>53</v>
       </c>
@@ -4157,7 +4192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="122"/>
       <c r="E23" s="125"/>
       <c r="G23" s="95" t="s">
@@ -4170,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="123"/>
       <c r="B24" s="99"/>
       <c r="C24" s="99"/>
@@ -4179,12 +4214,12 @@
       <c r="F24" s="122"/>
       <c r="J24" s="121"/>
     </row>
-    <row r="25" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J25" s="95" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G26" s="120" t="s">
         <v>57</v>
       </c>
@@ -4195,7 +4230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E27" s="98"/>
       <c r="G27" s="97"/>
       <c r="H27" s="97"/>
@@ -4203,7 +4238,7 @@
       <c r="J27" s="95"/>
       <c r="K27" s="94"/>
     </row>
-    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A28" s="116" t="s">
         <v>91</v>
       </c>
@@ -4212,91 +4247,91 @@
       <c r="D28" s="115"/>
       <c r="E28" s="115"/>
       <c r="F28" s="115"/>
-      <c r="G28" s="237" t="s">
+      <c r="G28" s="249" t="s">
         <v>53</v>
       </c>
-      <c r="H28" s="238"/>
-      <c r="I28" s="239" t="s">
+      <c r="H28" s="250"/>
+      <c r="I28" s="251" t="s">
         <v>61</v>
       </c>
-      <c r="J28" s="240"/>
-      <c r="K28" s="241"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="242" t="s">
+      <c r="J28" s="252"/>
+      <c r="K28" s="253"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="229" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="245" t="s">
+      <c r="B29" s="255" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="245" t="s">
+      <c r="C29" s="255" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="245"/>
-      <c r="E29" s="247" t="s">
+      <c r="D29" s="255"/>
+      <c r="E29" s="256" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="248"/>
-      <c r="G29" s="249"/>
-      <c r="H29" s="250"/>
-      <c r="I29" s="251">
+      <c r="F29" s="257"/>
+      <c r="G29" s="258"/>
+      <c r="H29" s="259"/>
+      <c r="I29" s="260">
         <v>0.2</v>
       </c>
-      <c r="J29" s="254"/>
-      <c r="K29" s="256">
+      <c r="J29" s="263"/>
+      <c r="K29" s="265">
         <f>J29*0.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="243"/>
-      <c r="B30" s="245"/>
-      <c r="C30" s="245" t="s">
+    <row r="30" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="254"/>
+      <c r="B30" s="255"/>
+      <c r="C30" s="255" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="245"/>
-      <c r="E30" s="258" t="s">
+      <c r="D30" s="255"/>
+      <c r="E30" s="222" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="259"/>
-      <c r="G30" s="260"/>
-      <c r="H30" s="261"/>
-      <c r="I30" s="252"/>
-      <c r="J30" s="254"/>
-      <c r="K30" s="256"/>
-    </row>
-    <row r="31" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="244"/>
-      <c r="B31" s="246"/>
-      <c r="C31" s="246" t="s">
+      <c r="F30" s="223"/>
+      <c r="G30" s="236"/>
+      <c r="H30" s="237"/>
+      <c r="I30" s="261"/>
+      <c r="J30" s="263"/>
+      <c r="K30" s="265"/>
+    </row>
+    <row r="31" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="230"/>
+      <c r="B31" s="221"/>
+      <c r="C31" s="221" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="246"/>
-      <c r="E31" s="258" t="s">
+      <c r="D31" s="221"/>
+      <c r="E31" s="222" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="259"/>
-      <c r="G31" s="262"/>
-      <c r="H31" s="263"/>
-      <c r="I31" s="253"/>
-      <c r="J31" s="255"/>
-      <c r="K31" s="257"/>
-    </row>
-    <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="242" t="s">
+      <c r="F31" s="223"/>
+      <c r="G31" s="224"/>
+      <c r="H31" s="225"/>
+      <c r="I31" s="262"/>
+      <c r="J31" s="264"/>
+      <c r="K31" s="266"/>
+    </row>
+    <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="229" t="s">
         <v>88</v>
       </c>
-      <c r="B32" s="267" t="s">
+      <c r="B32" s="231" t="s">
         <v>87</v>
       </c>
-      <c r="C32" s="268"/>
-      <c r="D32" s="269"/>
-      <c r="E32" s="270" t="s">
+      <c r="C32" s="232"/>
+      <c r="D32" s="233"/>
+      <c r="E32" s="234" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="271"/>
-      <c r="G32" s="260"/>
-      <c r="H32" s="261"/>
+      <c r="F32" s="235"/>
+      <c r="G32" s="236"/>
+      <c r="H32" s="237"/>
       <c r="I32" s="114">
         <v>0.4</v>
       </c>
@@ -4306,19 +4341,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="244"/>
-      <c r="B33" s="272" t="s">
+    <row r="33" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="230"/>
+      <c r="B33" s="238" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="273"/>
-      <c r="D33" s="274"/>
-      <c r="E33" s="275" t="s">
+      <c r="C33" s="239"/>
+      <c r="D33" s="240"/>
+      <c r="E33" s="241" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="276"/>
-      <c r="G33" s="260"/>
-      <c r="H33" s="261"/>
+      <c r="F33" s="242"/>
+      <c r="G33" s="236"/>
+      <c r="H33" s="237"/>
       <c r="I33" s="114">
         <v>0.4</v>
       </c>
@@ -4328,24 +4363,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="264" t="s">
+      <c r="B34" s="226" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="265"/>
-      <c r="D34" s="265"/>
-      <c r="E34" s="265"/>
-      <c r="F34" s="265"/>
-      <c r="G34" s="265"/>
-      <c r="H34" s="265"/>
-      <c r="I34" s="266"/>
+      <c r="C34" s="227"/>
+      <c r="D34" s="227"/>
+      <c r="E34" s="227"/>
+      <c r="F34" s="227"/>
+      <c r="G34" s="227"/>
+      <c r="H34" s="227"/>
+      <c r="I34" s="228"/>
       <c r="J34" s="160"/>
       <c r="K34" s="159"/>
     </row>
-    <row r="35" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G35" s="109"/>
       <c r="H35" s="109"/>
       <c r="I35" s="110"/>
@@ -4357,7 +4392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G36" s="109"/>
       <c r="H36" s="109"/>
       <c r="I36" s="108"/>
@@ -4369,7 +4404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G37" s="109"/>
       <c r="H37" s="109"/>
       <c r="I37" s="108" t="s">
@@ -4381,7 +4416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E38" s="98"/>
       <c r="G38" s="97"/>
       <c r="H38" s="105"/>
@@ -4396,8 +4431,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="99" t="s">
         <v>30</v>
       </c>
@@ -4413,7 +4448,7 @@
       <c r="J40" s="99"/>
       <c r="K40" s="99"/>
     </row>
-    <row r="41" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E41" s="98"/>
       <c r="G41" s="97"/>
       <c r="H41" s="97"/>
@@ -4421,21 +4456,25 @@
       <c r="J41" s="95"/>
       <c r="K41" s="94"/>
     </row>
-    <row r="46" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:11" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="G28:H28"/>
@@ -4452,21 +4491,17 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="G30:H30"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
   </mergeCells>
   <conditionalFormatting sqref="K29:K37">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
@@ -4495,33 +4530,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="93" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="93"/>
-    <col min="4" max="4" width="2.7109375" style="93" customWidth="1"/>
-    <col min="5" max="6" width="7.28515625" style="93" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" style="93" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="93" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="93" customWidth="1"/>
-    <col min="10" max="11" width="7.28515625" style="93" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="93" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="93" hidden="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="93"/>
+    <col min="1" max="1" width="8.265625" style="93" customWidth="1"/>
+    <col min="2" max="3" width="9.1328125" style="93"/>
+    <col min="4" max="4" width="2.73046875" style="93" customWidth="1"/>
+    <col min="5" max="6" width="7.265625" style="93" customWidth="1"/>
+    <col min="7" max="7" width="6.86328125" style="93" customWidth="1"/>
+    <col min="8" max="8" width="6.59765625" style="93" customWidth="1"/>
+    <col min="9" max="9" width="6.1328125" style="93" customWidth="1"/>
+    <col min="10" max="11" width="7.265625" style="93" customWidth="1"/>
+    <col min="12" max="12" width="8.73046875" style="93" customWidth="1"/>
+    <col min="13" max="13" width="7.265625" style="93" hidden="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1328125" style="93"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="142" t="s">
         <v>116</v>
       </c>
@@ -4533,7 +4568,7 @@
       <c r="K2" s="135"/>
       <c r="L2" s="135"/>
     </row>
-    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="141" t="s">
         <v>98</v>
       </c>
@@ -4545,14 +4580,14 @@
       <c r="K3" s="135"/>
       <c r="L3" s="135"/>
     </row>
-    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="99" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="99"/>
-      <c r="C4" s="233"/>
-      <c r="D4" s="233"/>
-      <c r="E4" s="233"/>
+      <c r="C4" s="276"/>
+      <c r="D4" s="276"/>
+      <c r="E4" s="276"/>
       <c r="F4" s="140"/>
       <c r="H4" s="138"/>
       <c r="I4" s="137" t="s">
@@ -4562,15 +4597,15 @@
       <c r="K4" s="135"/>
       <c r="L4" s="135"/>
     </row>
-    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="133" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="133"/>
-      <c r="C5" s="230"/>
-      <c r="D5" s="230"/>
-      <c r="E5" s="230"/>
-      <c r="F5" s="230"/>
+      <c r="C5" s="273"/>
+      <c r="D5" s="273"/>
+      <c r="E5" s="273"/>
+      <c r="F5" s="273"/>
       <c r="H5" s="138"/>
       <c r="I5" s="137" t="s">
         <v>11</v>
@@ -4579,7 +4614,7 @@
       <c r="K5" s="135"/>
       <c r="L5" s="135"/>
     </row>
-    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="93" t="s">
         <v>62</v>
       </c>
@@ -4587,98 +4622,98 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="133" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="133"/>
-      <c r="C7" s="230"/>
-      <c r="D7" s="230"/>
-      <c r="E7" s="230"/>
-      <c r="F7" s="230"/>
+      <c r="C7" s="273"/>
+      <c r="D7" s="273"/>
+      <c r="E7" s="273"/>
+      <c r="F7" s="273"/>
       <c r="H7" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="231"/>
-      <c r="J7" s="232"/>
-      <c r="K7" s="232"/>
-      <c r="L7" s="232"/>
-    </row>
-    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I7" s="274"/>
+      <c r="J7" s="275"/>
+      <c r="K7" s="275"/>
+      <c r="L7" s="275"/>
+    </row>
+    <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="99" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="99"/>
-      <c r="C8" s="233"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="233"/>
-      <c r="F8" s="233"/>
+      <c r="C8" s="276"/>
+      <c r="D8" s="276"/>
+      <c r="E8" s="276"/>
+      <c r="F8" s="276"/>
       <c r="H8" s="133" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="221"/>
-      <c r="J8" s="222"/>
-      <c r="K8" s="222"/>
-      <c r="L8" s="222"/>
-    </row>
-    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="267"/>
+      <c r="J8" s="268"/>
+      <c r="K8" s="268"/>
+      <c r="L8" s="268"/>
+    </row>
+    <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="133" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="133"/>
-      <c r="C9" s="230"/>
-      <c r="D9" s="230"/>
-      <c r="E9" s="230"/>
-      <c r="F9" s="230"/>
+      <c r="C9" s="273"/>
+      <c r="D9" s="273"/>
+      <c r="E9" s="273"/>
+      <c r="F9" s="273"/>
       <c r="H9" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="221"/>
-      <c r="J9" s="222"/>
-      <c r="K9" s="222"/>
-      <c r="L9" s="222"/>
-    </row>
-    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I9" s="267"/>
+      <c r="J9" s="268"/>
+      <c r="K9" s="268"/>
+      <c r="L9" s="268"/>
+    </row>
+    <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="133" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="133"/>
-      <c r="C10" s="230"/>
-      <c r="D10" s="230"/>
-      <c r="E10" s="230"/>
-      <c r="F10" s="230"/>
+      <c r="C10" s="273"/>
+      <c r="D10" s="273"/>
+      <c r="E10" s="273"/>
+      <c r="F10" s="273"/>
       <c r="H10" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="221"/>
-      <c r="J10" s="222"/>
-      <c r="K10" s="222"/>
-      <c r="L10" s="222"/>
-    </row>
-    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="267"/>
+      <c r="J10" s="268"/>
+      <c r="K10" s="268"/>
+      <c r="L10" s="268"/>
+    </row>
+    <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="221"/>
-      <c r="J11" s="222"/>
-      <c r="K11" s="222"/>
-      <c r="L11" s="222"/>
-    </row>
-    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="267"/>
+      <c r="J11" s="268"/>
+      <c r="K11" s="268"/>
+      <c r="L11" s="268"/>
+    </row>
+    <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="134"/>
       <c r="H12" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="221"/>
-      <c r="J12" s="222"/>
-      <c r="K12" s="222"/>
-      <c r="L12" s="222"/>
-    </row>
-    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="267"/>
+      <c r="J12" s="268"/>
+      <c r="K12" s="268"/>
+      <c r="L12" s="268"/>
+    </row>
+    <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="132"/>
       <c r="B13" s="131"/>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="13.9" x14ac:dyDescent="0.3">
       <c r="A14" s="116" t="s">
         <v>91</v>
       </c>
@@ -4688,97 +4723,97 @@
       <c r="E14" s="115"/>
       <c r="F14" s="115"/>
       <c r="G14" s="115"/>
-      <c r="H14" s="237" t="s">
+      <c r="H14" s="249" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="238"/>
-      <c r="J14" s="239" t="s">
+      <c r="I14" s="250"/>
+      <c r="J14" s="251" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="240"/>
-      <c r="L14" s="241"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="277" t="s">
+      <c r="K14" s="252"/>
+      <c r="L14" s="253"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="292" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="280" t="s">
+      <c r="B15" s="305" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="280" t="s">
+      <c r="C15" s="305" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="280"/>
-      <c r="E15" s="280"/>
-      <c r="F15" s="282" t="s">
+      <c r="D15" s="305"/>
+      <c r="E15" s="305"/>
+      <c r="F15" s="297" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="283"/>
-      <c r="H15" s="249"/>
-      <c r="I15" s="250"/>
-      <c r="J15" s="251">
+      <c r="G15" s="307"/>
+      <c r="H15" s="258"/>
+      <c r="I15" s="259"/>
+      <c r="J15" s="260">
         <v>0.2</v>
       </c>
-      <c r="K15" s="254">
+      <c r="K15" s="263">
         <v>0</v>
       </c>
-      <c r="L15" s="256">
+      <c r="L15" s="265">
         <f>K15*0.2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="278"/>
-      <c r="B16" s="280"/>
-      <c r="C16" s="280" t="s">
+    <row r="16" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="304"/>
+      <c r="B16" s="305"/>
+      <c r="C16" s="305" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="280"/>
-      <c r="E16" s="280"/>
-      <c r="F16" s="284" t="s">
+      <c r="D16" s="305"/>
+      <c r="E16" s="305"/>
+      <c r="F16" s="308" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="285"/>
-      <c r="H16" s="260"/>
-      <c r="I16" s="261"/>
-      <c r="J16" s="252"/>
-      <c r="K16" s="254"/>
-      <c r="L16" s="256"/>
-    </row>
-    <row r="17" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="279"/>
-      <c r="B17" s="281"/>
-      <c r="C17" s="281" t="s">
+      <c r="G16" s="309"/>
+      <c r="H16" s="236"/>
+      <c r="I16" s="237"/>
+      <c r="J16" s="261"/>
+      <c r="K16" s="263"/>
+      <c r="L16" s="265"/>
+    </row>
+    <row r="17" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="293"/>
+      <c r="B17" s="306"/>
+      <c r="C17" s="306" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="281"/>
-      <c r="E17" s="281"/>
-      <c r="F17" s="284" t="s">
+      <c r="D17" s="306"/>
+      <c r="E17" s="306"/>
+      <c r="F17" s="308" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="285"/>
-      <c r="H17" s="262"/>
-      <c r="I17" s="263"/>
-      <c r="J17" s="253"/>
-      <c r="K17" s="255"/>
-      <c r="L17" s="257"/>
-    </row>
-    <row r="18" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="277" t="s">
+      <c r="G17" s="309"/>
+      <c r="H17" s="224"/>
+      <c r="I17" s="225"/>
+      <c r="J17" s="262"/>
+      <c r="K17" s="264"/>
+      <c r="L17" s="266"/>
+    </row>
+    <row r="18" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="292" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="286" t="s">
+      <c r="B18" s="294" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="287"/>
-      <c r="D18" s="287"/>
-      <c r="E18" s="288"/>
-      <c r="F18" s="282" t="s">
+      <c r="C18" s="295"/>
+      <c r="D18" s="295"/>
+      <c r="E18" s="296"/>
+      <c r="F18" s="297" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="289"/>
-      <c r="H18" s="260"/>
-      <c r="I18" s="261"/>
+      <c r="G18" s="298"/>
+      <c r="H18" s="236"/>
+      <c r="I18" s="237"/>
       <c r="J18" s="114">
         <v>0.4</v>
       </c>
@@ -4791,20 +4826,20 @@
       </c>
       <c r="M18" s="143"/>
     </row>
-    <row r="19" spans="1:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="279"/>
-      <c r="B19" s="290" t="s">
+    <row r="19" spans="1:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="293"/>
+      <c r="B19" s="299" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="291"/>
-      <c r="D19" s="291"/>
-      <c r="E19" s="292"/>
-      <c r="F19" s="293" t="s">
+      <c r="C19" s="300"/>
+      <c r="D19" s="300"/>
+      <c r="E19" s="301"/>
+      <c r="F19" s="302" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="294"/>
-      <c r="H19" s="260"/>
-      <c r="I19" s="261"/>
+      <c r="G19" s="303"/>
+      <c r="H19" s="236"/>
+      <c r="I19" s="237"/>
       <c r="J19" s="114">
         <v>0.4</v>
       </c>
@@ -4816,25 +4851,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="13.15" x14ac:dyDescent="0.3">
       <c r="A20" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="264" t="s">
+      <c r="B20" s="226" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="265"/>
-      <c r="D20" s="265"/>
-      <c r="E20" s="265"/>
-      <c r="F20" s="265"/>
-      <c r="G20" s="265"/>
-      <c r="H20" s="265"/>
-      <c r="I20" s="265"/>
-      <c r="J20" s="266"/>
+      <c r="C20" s="227"/>
+      <c r="D20" s="227"/>
+      <c r="E20" s="227"/>
+      <c r="F20" s="227"/>
+      <c r="G20" s="227"/>
+      <c r="H20" s="227"/>
+      <c r="I20" s="227"/>
+      <c r="J20" s="228"/>
       <c r="K20" s="113"/>
       <c r="L20" s="161"/>
     </row>
-    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H21" s="109"/>
       <c r="I21" s="109"/>
       <c r="L21" s="144">
@@ -4842,96 +4877,96 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="142" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="295" t="s">
+    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="283" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="296"/>
-      <c r="C23" s="296"/>
-      <c r="D23" s="296"/>
-      <c r="E23" s="296"/>
-      <c r="F23" s="296"/>
-      <c r="G23" s="296"/>
-      <c r="H23" s="296"/>
-      <c r="I23" s="296"/>
-      <c r="J23" s="296"/>
-      <c r="K23" s="296"/>
-      <c r="L23" s="297"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="298"/>
-      <c r="B24" s="299"/>
-      <c r="C24" s="299"/>
-      <c r="D24" s="299"/>
-      <c r="E24" s="299"/>
-      <c r="F24" s="299"/>
-      <c r="G24" s="299"/>
-      <c r="H24" s="299"/>
-      <c r="I24" s="299"/>
-      <c r="J24" s="299"/>
-      <c r="K24" s="299"/>
-      <c r="L24" s="300"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="298"/>
-      <c r="B25" s="299"/>
-      <c r="C25" s="299"/>
-      <c r="D25" s="299"/>
-      <c r="E25" s="299"/>
-      <c r="F25" s="299"/>
-      <c r="G25" s="299"/>
-      <c r="H25" s="299"/>
-      <c r="I25" s="299"/>
-      <c r="J25" s="299"/>
-      <c r="K25" s="299"/>
-      <c r="L25" s="300"/>
-    </row>
-    <row r="26" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="298"/>
-      <c r="B26" s="299"/>
-      <c r="C26" s="299"/>
-      <c r="D26" s="299"/>
-      <c r="E26" s="299"/>
-      <c r="F26" s="299"/>
-      <c r="G26" s="299"/>
-      <c r="H26" s="299"/>
-      <c r="I26" s="299"/>
-      <c r="J26" s="299"/>
-      <c r="K26" s="299"/>
-      <c r="L26" s="300"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="301"/>
-      <c r="B27" s="302"/>
-      <c r="C27" s="302"/>
-      <c r="D27" s="302"/>
-      <c r="E27" s="302"/>
-      <c r="F27" s="302"/>
-      <c r="G27" s="302"/>
-      <c r="H27" s="302"/>
-      <c r="I27" s="302"/>
-      <c r="J27" s="302"/>
-      <c r="K27" s="302"/>
-      <c r="L27" s="303"/>
-    </row>
-    <row r="29" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="304" t="s">
+      <c r="B23" s="284"/>
+      <c r="C23" s="284"/>
+      <c r="D23" s="284"/>
+      <c r="E23" s="284"/>
+      <c r="F23" s="284"/>
+      <c r="G23" s="284"/>
+      <c r="H23" s="284"/>
+      <c r="I23" s="284"/>
+      <c r="J23" s="284"/>
+      <c r="K23" s="284"/>
+      <c r="L23" s="285"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="286"/>
+      <c r="B24" s="287"/>
+      <c r="C24" s="287"/>
+      <c r="D24" s="287"/>
+      <c r="E24" s="287"/>
+      <c r="F24" s="287"/>
+      <c r="G24" s="287"/>
+      <c r="H24" s="287"/>
+      <c r="I24" s="287"/>
+      <c r="J24" s="287"/>
+      <c r="K24" s="287"/>
+      <c r="L24" s="288"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="286"/>
+      <c r="B25" s="287"/>
+      <c r="C25" s="287"/>
+      <c r="D25" s="287"/>
+      <c r="E25" s="287"/>
+      <c r="F25" s="287"/>
+      <c r="G25" s="287"/>
+      <c r="H25" s="287"/>
+      <c r="I25" s="287"/>
+      <c r="J25" s="287"/>
+      <c r="K25" s="287"/>
+      <c r="L25" s="288"/>
+    </row>
+    <row r="26" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="286"/>
+      <c r="B26" s="287"/>
+      <c r="C26" s="287"/>
+      <c r="D26" s="287"/>
+      <c r="E26" s="287"/>
+      <c r="F26" s="287"/>
+      <c r="G26" s="287"/>
+      <c r="H26" s="287"/>
+      <c r="I26" s="287"/>
+      <c r="J26" s="287"/>
+      <c r="K26" s="287"/>
+      <c r="L26" s="288"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="289"/>
+      <c r="B27" s="290"/>
+      <c r="C27" s="290"/>
+      <c r="D27" s="290"/>
+      <c r="E27" s="290"/>
+      <c r="F27" s="290"/>
+      <c r="G27" s="290"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
+      <c r="K27" s="290"/>
+      <c r="L27" s="291"/>
+    </row>
+    <row r="29" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A29" s="280" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="304"/>
-      <c r="C29" s="304"/>
-      <c r="D29" s="304"/>
-      <c r="E29" s="304"/>
-      <c r="F29" s="304"/>
-      <c r="G29" s="304"/>
-      <c r="H29" s="304"/>
-      <c r="I29" s="305"/>
-      <c r="J29" s="305"/>
+      <c r="B29" s="280"/>
+      <c r="C29" s="280"/>
+      <c r="D29" s="280"/>
+      <c r="E29" s="280"/>
+      <c r="F29" s="280"/>
+      <c r="G29" s="280"/>
+      <c r="H29" s="280"/>
+      <c r="I29" s="281"/>
+      <c r="J29" s="281"/>
       <c r="K29" s="145" t="s">
         <v>103</v>
       </c>
@@ -4940,19 +4975,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="304" t="s">
+    <row r="30" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="280" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="304"/>
-      <c r="C30" s="304"/>
-      <c r="D30" s="304"/>
-      <c r="E30" s="304"/>
-      <c r="F30" s="304"/>
-      <c r="G30" s="304"/>
-      <c r="H30" s="304"/>
-      <c r="I30" s="305"/>
-      <c r="J30" s="305"/>
+      <c r="B30" s="280"/>
+      <c r="C30" s="280"/>
+      <c r="D30" s="280"/>
+      <c r="E30" s="280"/>
+      <c r="F30" s="280"/>
+      <c r="G30" s="280"/>
+      <c r="H30" s="280"/>
+      <c r="I30" s="281"/>
+      <c r="J30" s="281"/>
       <c r="K30" s="130" t="s">
         <v>103</v>
       </c>
@@ -4961,19 +4996,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="304" t="s">
+    <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="280" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="304"/>
-      <c r="C31" s="304"/>
-      <c r="D31" s="304"/>
-      <c r="E31" s="304"/>
-      <c r="F31" s="304"/>
-      <c r="G31" s="304"/>
-      <c r="H31" s="304"/>
-      <c r="I31" s="305"/>
-      <c r="J31" s="305"/>
+      <c r="B31" s="280"/>
+      <c r="C31" s="280"/>
+      <c r="D31" s="280"/>
+      <c r="E31" s="280"/>
+      <c r="F31" s="280"/>
+      <c r="G31" s="280"/>
+      <c r="H31" s="280"/>
+      <c r="I31" s="281"/>
+      <c r="J31" s="281"/>
       <c r="K31" s="130" t="s">
         <v>106</v>
       </c>
@@ -4982,19 +5017,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="304" t="s">
+    <row r="32" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="280" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="304"/>
-      <c r="C32" s="304"/>
-      <c r="D32" s="304"/>
-      <c r="E32" s="304"/>
-      <c r="F32" s="304"/>
-      <c r="G32" s="304"/>
-      <c r="H32" s="304"/>
-      <c r="I32" s="305"/>
-      <c r="J32" s="305"/>
+      <c r="B32" s="280"/>
+      <c r="C32" s="280"/>
+      <c r="D32" s="280"/>
+      <c r="E32" s="280"/>
+      <c r="F32" s="280"/>
+      <c r="G32" s="280"/>
+      <c r="H32" s="280"/>
+      <c r="I32" s="281"/>
+      <c r="J32" s="281"/>
       <c r="K32" s="130" t="s">
         <v>84</v>
       </c>
@@ -5003,22 +5038,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="304" t="s">
+    <row r="33" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="280" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="304"/>
-      <c r="C33" s="304"/>
-      <c r="D33" s="304"/>
-      <c r="E33" s="304"/>
-      <c r="F33" s="304"/>
-      <c r="G33" s="304"/>
-      <c r="H33" s="304"/>
-      <c r="I33" s="309">
+      <c r="B33" s="280"/>
+      <c r="C33" s="280"/>
+      <c r="D33" s="280"/>
+      <c r="E33" s="280"/>
+      <c r="F33" s="280"/>
+      <c r="G33" s="280"/>
+      <c r="H33" s="280"/>
+      <c r="I33" s="282">
         <f>L21</f>
         <v>0</v>
       </c>
-      <c r="J33" s="309"/>
+      <c r="J33" s="282"/>
       <c r="K33" s="130" t="s">
         <v>106</v>
       </c>
@@ -5027,7 +5062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F34" s="141"/>
       <c r="I34" s="109"/>
       <c r="J34" s="147"/>
@@ -5039,21 +5074,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F35" s="306" t="s">
+    <row r="35" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F35" s="277" t="s">
         <v>110</v>
       </c>
-      <c r="G35" s="307"/>
-      <c r="H35" s="307"/>
-      <c r="I35" s="307"/>
-      <c r="J35" s="307"/>
-      <c r="K35" s="308"/>
+      <c r="G35" s="278"/>
+      <c r="H35" s="278"/>
+      <c r="I35" s="278"/>
+      <c r="J35" s="278"/>
+      <c r="K35" s="279"/>
       <c r="L35" s="149">
         <f>L34/10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
       <c r="F36" s="141"/>
       <c r="G36" s="141"/>
       <c r="H36" s="141"/>
@@ -5062,7 +5097,7 @@
       <c r="K36" s="141"/>
       <c r="L36" s="150"/>
     </row>
-    <row r="37" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
       <c r="F37" s="141"/>
       <c r="G37" s="141"/>
       <c r="H37" s="141"/>
@@ -5071,7 +5106,7 @@
       <c r="K37" s="141"/>
       <c r="L37" s="150"/>
     </row>
-    <row r="38" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
       <c r="F38" s="141"/>
       <c r="G38" s="141"/>
       <c r="H38" s="141"/>
@@ -5080,7 +5115,7 @@
       <c r="K38" s="141"/>
       <c r="L38" s="150"/>
     </row>
-    <row r="39" spans="1:12" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
       <c r="F39" s="141"/>
       <c r="G39" s="141"/>
       <c r="H39" s="141"/>
@@ -5089,7 +5124,7 @@
       <c r="K39" s="141"/>
       <c r="L39" s="150"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F40" s="98"/>
       <c r="H40" s="97"/>
       <c r="I40" s="97"/>
@@ -5097,7 +5132,7 @@
       <c r="K40" s="95"/>
       <c r="L40" s="94"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="99" t="s">
         <v>30</v>
       </c>
@@ -5114,7 +5149,7 @@
       <c r="K42" s="99"/>
       <c r="L42" s="99"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F43" s="98"/>
       <c r="H43" s="97"/>
       <c r="I43" s="97"/>
@@ -5122,7 +5157,7 @@
       <c r="K43" s="95"/>
       <c r="L43" s="94"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="143"/>
       <c r="B44" s="143"/>
       <c r="C44" s="143"/>
@@ -5138,26 +5173,18 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="A23:L27"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="A15:A17"/>
@@ -5174,18 +5201,26 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="A23:L27"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="I33:J33"/>
   </mergeCells>
   <conditionalFormatting sqref="L15:L39 I33:J33">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
@@ -5204,7 +5239,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="98" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR LAGKLASS</oddHeader>
     <oddFooter>&amp;R2019-03-28</oddFooter>
@@ -5214,15 +5249,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5288,6 +5314,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5298,21 +5333,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64838F1D-7ECA-4F32-944F-43492487C498}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5329,6 +5349,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64838F1D-7ECA-4F32-944F-43492487C498}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Ändrade felaktig ordning mellan lag och klubb i protokollet
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll_2019_mixklass lag(mall).xlsx
+++ b/mallar/Protokoll/Protokoll_2019_mixklass lag(mall).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85623E2F-BE69-4B91-9C47-086B9832609D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7E7746-886C-47BE-84DA-DB45B4C1CCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="27" r:id="rId1"/>
@@ -943,7 +943,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="268">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1290,34 +1290,149 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="30" fillId="0" borderId="17" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="17" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="0" borderId="17" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="12" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="21" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="12" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="21" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1328,39 +1443,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="12" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="21" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1369,128 +1451,79 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="12" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="21" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
@@ -1500,15 +1533,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1530,40 +1554,98 @@
     <xf numFmtId="167" fontId="4" fillId="0" borderId="21" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1572,97 +1654,16 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="17" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="17" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="30" fillId="0" borderId="17" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2489,7 +2490,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -2536,8 +2537,8 @@
         <v>9</v>
       </c>
       <c r="B4" s="139"/>
-      <c r="C4" s="201"/>
-      <c r="D4" s="201"/>
+      <c r="C4" s="150"/>
+      <c r="D4" s="150"/>
       <c r="E4" s="140"/>
       <c r="G4" s="98"/>
       <c r="H4" s="99" t="s">
@@ -2552,9 +2553,9 @@
         <v>10</v>
       </c>
       <c r="B5" s="141"/>
-      <c r="C5" s="198"/>
-      <c r="D5" s="198"/>
-      <c r="E5" s="198"/>
+      <c r="C5" s="151"/>
+      <c r="D5" s="151"/>
+      <c r="E5" s="151"/>
       <c r="G5" s="98"/>
       <c r="H5" s="99" t="s">
         <v>8</v>
@@ -2565,7 +2566,7 @@
     </row>
     <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="96" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B6" s="138"/>
       <c r="C6" s="138"/>
@@ -2577,86 +2578,86 @@
     </row>
     <row r="7" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="104" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B7" s="141"/>
-      <c r="C7" s="198"/>
-      <c r="D7" s="198"/>
-      <c r="E7" s="198"/>
+      <c r="C7" s="151"/>
+      <c r="D7" s="151"/>
+      <c r="E7" s="151"/>
       <c r="G7" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="202"/>
-      <c r="I7" s="203"/>
-      <c r="J7" s="203"/>
-      <c r="K7" s="203"/>
+      <c r="H7" s="152"/>
+      <c r="I7" s="153"/>
+      <c r="J7" s="153"/>
+      <c r="K7" s="153"/>
     </row>
     <row r="8" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="103" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="139"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="204"/>
-      <c r="E8" s="204"/>
+      <c r="C8" s="154"/>
+      <c r="D8" s="154"/>
+      <c r="E8" s="154"/>
       <c r="G8" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="199"/>
-      <c r="I8" s="200"/>
-      <c r="J8" s="200"/>
-      <c r="K8" s="200"/>
+      <c r="H8" s="155"/>
+      <c r="I8" s="156"/>
+      <c r="J8" s="156"/>
+      <c r="K8" s="156"/>
     </row>
     <row r="9" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="104" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="141"/>
-      <c r="C9" s="198"/>
-      <c r="D9" s="198"/>
-      <c r="E9" s="198"/>
+      <c r="C9" s="151"/>
+      <c r="D9" s="151"/>
+      <c r="E9" s="151"/>
       <c r="G9" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="199"/>
-      <c r="I9" s="200"/>
-      <c r="J9" s="200"/>
-      <c r="K9" s="200"/>
+      <c r="H9" s="155"/>
+      <c r="I9" s="156"/>
+      <c r="J9" s="156"/>
+      <c r="K9" s="156"/>
     </row>
     <row r="10" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="104" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="141"/>
-      <c r="C10" s="198"/>
-      <c r="D10" s="198"/>
-      <c r="E10" s="198"/>
+      <c r="C10" s="151"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="151"/>
       <c r="G10" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="199"/>
-      <c r="I10" s="200"/>
-      <c r="J10" s="200"/>
-      <c r="K10" s="200"/>
+      <c r="H10" s="155"/>
+      <c r="I10" s="156"/>
+      <c r="J10" s="156"/>
+      <c r="K10" s="156"/>
     </row>
     <row r="11" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="199"/>
-      <c r="I11" s="200"/>
-      <c r="J11" s="200"/>
-      <c r="K11" s="200"/>
+      <c r="H11" s="155"/>
+      <c r="I11" s="156"/>
+      <c r="J11" s="156"/>
+      <c r="K11" s="156"/>
     </row>
     <row r="12" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="106"/>
       <c r="G12" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="199"/>
-      <c r="I12" s="200"/>
-      <c r="J12" s="200"/>
-      <c r="K12" s="200"/>
+      <c r="H12" s="155"/>
+      <c r="I12" s="156"/>
+      <c r="J12" s="156"/>
+      <c r="K12" s="156"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="107"/>
@@ -2686,11 +2687,11 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="189" t="s">
+      <c r="A15" s="160" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="190"/>
-      <c r="C15" s="191"/>
+      <c r="B15" s="161"/>
+      <c r="C15" s="162"/>
       <c r="D15" s="143"/>
       <c r="E15" s="143"/>
       <c r="F15" s="143"/>
@@ -2703,11 +2704,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="189" t="s">
+      <c r="A16" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="190"/>
-      <c r="C16" s="191"/>
+      <c r="B16" s="161"/>
+      <c r="C16" s="162"/>
       <c r="D16" s="143"/>
       <c r="E16" s="143"/>
       <c r="F16" s="143"/>
@@ -2720,11 +2721,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="192" t="s">
+      <c r="A17" s="157" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="193"/>
-      <c r="C17" s="194"/>
+      <c r="B17" s="158"/>
+      <c r="C17" s="159"/>
       <c r="D17" s="143"/>
       <c r="E17" s="143"/>
       <c r="F17" s="143"/>
@@ -2737,11 +2738,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="192" t="s">
+      <c r="A18" s="157" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="193"/>
-      <c r="C18" s="194"/>
+      <c r="B18" s="158"/>
+      <c r="C18" s="159"/>
       <c r="D18" s="143"/>
       <c r="E18" s="143"/>
       <c r="F18" s="143"/>
@@ -2754,11 +2755,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="195" t="s">
+      <c r="A19" s="163" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="196"/>
-      <c r="C19" s="197"/>
+      <c r="B19" s="164"/>
+      <c r="C19" s="165"/>
       <c r="D19" s="143"/>
       <c r="E19" s="143"/>
       <c r="F19" s="143"/>
@@ -2771,11 +2772,11 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="20.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="192" t="s">
+      <c r="A20" s="157" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="193"/>
-      <c r="C20" s="194"/>
+      <c r="B20" s="158"/>
+      <c r="C20" s="159"/>
       <c r="D20" s="143"/>
       <c r="E20" s="143"/>
       <c r="F20" s="143"/>
@@ -2788,11 +2789,11 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="171" t="s">
+      <c r="A21" s="166" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="172"/>
-      <c r="C21" s="173"/>
+      <c r="B21" s="167"/>
+      <c r="C21" s="168"/>
       <c r="D21" s="143"/>
       <c r="E21" s="143"/>
       <c r="F21" s="143"/>
@@ -2859,7 +2860,7 @@
       </c>
       <c r="H27" s="122"/>
       <c r="I27" s="123"/>
-      <c r="J27" s="264">
+      <c r="J27" s="147">
         <f>IFERROR(+J24/7,3)</f>
         <v>0</v>
       </c>
@@ -2881,91 +2882,91 @@
       <c r="D29" s="89"/>
       <c r="E29" s="89"/>
       <c r="F29" s="89"/>
-      <c r="G29" s="174" t="s">
+      <c r="G29" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="H29" s="175"/>
-      <c r="I29" s="176" t="s">
+      <c r="H29" s="170"/>
+      <c r="I29" s="171" t="s">
         <v>38</v>
       </c>
-      <c r="J29" s="177"/>
-      <c r="K29" s="178"/>
+      <c r="J29" s="172"/>
+      <c r="K29" s="173"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="149" t="s">
+      <c r="A30" s="174" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="165" t="s">
+      <c r="B30" s="177" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="165" t="s">
+      <c r="C30" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="165"/>
-      <c r="E30" s="180" t="s">
+      <c r="D30" s="177"/>
+      <c r="E30" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="181"/>
-      <c r="G30" s="182"/>
-      <c r="H30" s="183"/>
-      <c r="I30" s="184">
+      <c r="F30" s="180"/>
+      <c r="G30" s="181"/>
+      <c r="H30" s="182"/>
+      <c r="I30" s="183">
         <v>0.2</v>
       </c>
-      <c r="J30" s="187"/>
-      <c r="K30" s="163">
+      <c r="J30" s="186"/>
+      <c r="K30" s="188">
         <f>J30*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="179"/>
-      <c r="B31" s="165"/>
-      <c r="C31" s="165" t="s">
+      <c r="A31" s="175"/>
+      <c r="B31" s="177"/>
+      <c r="C31" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="165"/>
-      <c r="E31" s="166" t="s">
+      <c r="D31" s="177"/>
+      <c r="E31" s="190" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="167"/>
-      <c r="G31" s="156"/>
-      <c r="H31" s="157"/>
-      <c r="I31" s="185"/>
-      <c r="J31" s="187"/>
-      <c r="K31" s="163"/>
+      <c r="F31" s="191"/>
+      <c r="G31" s="192"/>
+      <c r="H31" s="193"/>
+      <c r="I31" s="184"/>
+      <c r="J31" s="186"/>
+      <c r="K31" s="188"/>
     </row>
     <row r="32" spans="1:11" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="150"/>
-      <c r="B32" s="168"/>
-      <c r="C32" s="168" t="s">
+      <c r="A32" s="176"/>
+      <c r="B32" s="178"/>
+      <c r="C32" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="168"/>
-      <c r="E32" s="166" t="s">
+      <c r="D32" s="178"/>
+      <c r="E32" s="190" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="167"/>
-      <c r="G32" s="169"/>
-      <c r="H32" s="170"/>
-      <c r="I32" s="186"/>
-      <c r="J32" s="188"/>
-      <c r="K32" s="164"/>
+      <c r="F32" s="191"/>
+      <c r="G32" s="194"/>
+      <c r="H32" s="195"/>
+      <c r="I32" s="185"/>
+      <c r="J32" s="187"/>
+      <c r="K32" s="189"/>
     </row>
     <row r="33" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="149" t="s">
+      <c r="A33" s="174" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="151" t="s">
+      <c r="B33" s="199" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="152"/>
-      <c r="D33" s="153"/>
-      <c r="E33" s="154" t="s">
+      <c r="C33" s="200"/>
+      <c r="D33" s="201"/>
+      <c r="E33" s="202" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="155"/>
-      <c r="G33" s="156"/>
-      <c r="H33" s="157"/>
+      <c r="F33" s="203"/>
+      <c r="G33" s="192"/>
+      <c r="H33" s="193"/>
       <c r="I33" s="88">
         <v>0.4</v>
       </c>
@@ -2976,18 +2977,18 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="150"/>
-      <c r="B34" s="158" t="s">
+      <c r="A34" s="176"/>
+      <c r="B34" s="204" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="159"/>
-      <c r="D34" s="160"/>
-      <c r="E34" s="161" t="s">
+      <c r="C34" s="205"/>
+      <c r="D34" s="206"/>
+      <c r="E34" s="207" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="162"/>
-      <c r="G34" s="156"/>
-      <c r="H34" s="157"/>
+      <c r="F34" s="208"/>
+      <c r="G34" s="192"/>
+      <c r="H34" s="193"/>
       <c r="I34" s="88">
         <v>0.4</v>
       </c>
@@ -3001,16 +3002,16 @@
       <c r="A35" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="146" t="s">
+      <c r="B35" s="196" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="147"/>
-      <c r="D35" s="147"/>
-      <c r="E35" s="147"/>
-      <c r="F35" s="147"/>
-      <c r="G35" s="147"/>
-      <c r="H35" s="147"/>
-      <c r="I35" s="148"/>
+      <c r="C35" s="197"/>
+      <c r="D35" s="197"/>
+      <c r="E35" s="197"/>
+      <c r="F35" s="197"/>
+      <c r="G35" s="197"/>
+      <c r="H35" s="197"/>
+      <c r="I35" s="198"/>
       <c r="J35" s="130"/>
       <c r="K35" s="145"/>
     </row>
@@ -3060,7 +3061,7 @@
       <c r="J39" s="137" t="s">
         <v>50</v>
       </c>
-      <c r="K39" s="265">
+      <c r="K39" s="148">
         <f>K38/8</f>
         <v>0</v>
       </c>
@@ -3094,24 +3095,15 @@
     <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="I29:K29"/>
@@ -3128,15 +3120,24 @@
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
   </mergeCells>
   <conditionalFormatting sqref="K30:K38">
     <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
@@ -3171,8 +3172,8 @@
   </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -3214,8 +3215,8 @@
         <v>9</v>
       </c>
       <c r="B4" s="18"/>
-      <c r="C4" s="226"/>
-      <c r="D4" s="226"/>
+      <c r="C4" s="217"/>
+      <c r="D4" s="217"/>
       <c r="E4" s="58"/>
       <c r="G4" s="56"/>
       <c r="H4" s="55" t="s">
@@ -3230,9 +3231,9 @@
         <v>10</v>
       </c>
       <c r="B5" s="51"/>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="227"/>
+      <c r="C5" s="218"/>
+      <c r="D5" s="218"/>
+      <c r="E5" s="218"/>
       <c r="G5" s="56"/>
       <c r="H5" s="55" t="s">
         <v>8</v>
@@ -3242,8 +3243,8 @@
       <c r="K5" s="53"/>
     </row>
     <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>39</v>
+      <c r="A6" s="146" t="s">
+        <v>11</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>13</v>
@@ -3251,86 +3252,86 @@
     </row>
     <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B7" s="51"/>
-      <c r="C7" s="227"/>
-      <c r="D7" s="227"/>
-      <c r="E7" s="227"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="218"/>
+      <c r="E7" s="218"/>
       <c r="G7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="228"/>
-      <c r="I7" s="229"/>
-      <c r="J7" s="229"/>
-      <c r="K7" s="229"/>
+      <c r="H7" s="219"/>
+      <c r="I7" s="220"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="220"/>
     </row>
     <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="18"/>
-      <c r="C8" s="230"/>
-      <c r="D8" s="230"/>
-      <c r="E8" s="230"/>
+      <c r="C8" s="221"/>
+      <c r="D8" s="221"/>
+      <c r="E8" s="221"/>
       <c r="G8" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="221"/>
-      <c r="I8" s="222"/>
-      <c r="J8" s="222"/>
-      <c r="K8" s="222"/>
+      <c r="H8" s="209"/>
+      <c r="I8" s="210"/>
+      <c r="J8" s="210"/>
+      <c r="K8" s="210"/>
     </row>
     <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="51"/>
-      <c r="C9" s="227"/>
-      <c r="D9" s="227"/>
-      <c r="E9" s="227"/>
+      <c r="C9" s="218"/>
+      <c r="D9" s="218"/>
+      <c r="E9" s="218"/>
       <c r="G9" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="221"/>
-      <c r="I9" s="222"/>
-      <c r="J9" s="222"/>
-      <c r="K9" s="222"/>
+      <c r="H9" s="209"/>
+      <c r="I9" s="210"/>
+      <c r="J9" s="210"/>
+      <c r="K9" s="210"/>
     </row>
     <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="51" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="51"/>
-      <c r="C10" s="227"/>
-      <c r="D10" s="227"/>
-      <c r="E10" s="227"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
       <c r="G10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="221"/>
-      <c r="I10" s="222"/>
-      <c r="J10" s="222"/>
-      <c r="K10" s="222"/>
+      <c r="H10" s="209"/>
+      <c r="I10" s="210"/>
+      <c r="J10" s="210"/>
+      <c r="K10" s="210"/>
     </row>
     <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="221"/>
-      <c r="I11" s="222"/>
-      <c r="J11" s="222"/>
-      <c r="K11" s="222"/>
+      <c r="H11" s="209"/>
+      <c r="I11" s="210"/>
+      <c r="J11" s="210"/>
+      <c r="K11" s="210"/>
     </row>
     <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="52"/>
       <c r="G12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="221"/>
-      <c r="I12" s="222"/>
-      <c r="J12" s="222"/>
-      <c r="K12" s="222"/>
+      <c r="H12" s="209"/>
+      <c r="I12" s="210"/>
+      <c r="J12" s="210"/>
+      <c r="K12" s="210"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="50"/>
@@ -3360,11 +3361,11 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="223" t="s">
+      <c r="A15" s="211" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="224"/>
-      <c r="C15" s="225"/>
+      <c r="B15" s="212"/>
+      <c r="C15" s="213"/>
       <c r="D15" s="74">
         <v>0</v>
       </c>
@@ -3381,11 +3382,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="212" t="s">
+      <c r="A16" s="214" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="213"/>
-      <c r="C16" s="214"/>
+      <c r="B16" s="215"/>
+      <c r="C16" s="216"/>
       <c r="D16" s="74">
         <v>0</v>
       </c>
@@ -3402,11 +3403,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="212" t="s">
+      <c r="A17" s="214" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="213"/>
-      <c r="C17" s="214"/>
+      <c r="B17" s="215"/>
+      <c r="C17" s="216"/>
       <c r="D17" s="74">
         <v>0</v>
       </c>
@@ -3423,11 +3424,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="209" t="s">
+      <c r="A18" s="222" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="210"/>
-      <c r="C18" s="211"/>
+      <c r="B18" s="223"/>
+      <c r="C18" s="224"/>
       <c r="D18" s="74">
         <v>0</v>
       </c>
@@ -3444,11 +3445,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="212" t="s">
+      <c r="A19" s="214" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="213"/>
-      <c r="C19" s="214"/>
+      <c r="B19" s="215"/>
+      <c r="C19" s="216"/>
       <c r="D19" s="74">
         <v>0</v>
       </c>
@@ -3465,11 +3466,11 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="212" t="s">
+      <c r="A20" s="214" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="213"/>
-      <c r="C20" s="214"/>
+      <c r="B20" s="215"/>
+      <c r="C20" s="216"/>
       <c r="D20" s="74">
         <v>0</v>
       </c>
@@ -3540,7 +3541,7 @@
       </c>
       <c r="H26" s="37"/>
       <c r="I26" s="36"/>
-      <c r="J26" s="266">
+      <c r="J26" s="149">
         <f>IFERROR(+J23/6,3)</f>
         <v>0</v>
       </c>
@@ -3562,91 +3563,91 @@
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
-      <c r="G28" s="174" t="s">
+      <c r="G28" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="H28" s="175"/>
-      <c r="I28" s="176" t="s">
+      <c r="H28" s="170"/>
+      <c r="I28" s="171" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="177"/>
-      <c r="K28" s="178"/>
+      <c r="J28" s="172"/>
+      <c r="K28" s="173"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="149" t="s">
+      <c r="A29" s="174" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="165" t="s">
+      <c r="B29" s="177" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="165" t="s">
+      <c r="C29" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="165"/>
-      <c r="E29" s="180" t="s">
+      <c r="D29" s="177"/>
+      <c r="E29" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="181"/>
-      <c r="G29" s="215"/>
-      <c r="H29" s="216"/>
-      <c r="I29" s="184">
+      <c r="F29" s="180"/>
+      <c r="G29" s="225"/>
+      <c r="H29" s="226"/>
+      <c r="I29" s="183">
         <v>0.2</v>
       </c>
-      <c r="J29" s="217"/>
-      <c r="K29" s="219">
+      <c r="J29" s="227"/>
+      <c r="K29" s="229">
         <f>J29*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="179"/>
-      <c r="B30" s="165"/>
-      <c r="C30" s="165" t="s">
+      <c r="A30" s="175"/>
+      <c r="B30" s="177"/>
+      <c r="C30" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="165"/>
-      <c r="E30" s="166" t="s">
+      <c r="D30" s="177"/>
+      <c r="E30" s="190" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="167"/>
-      <c r="G30" s="207"/>
-      <c r="H30" s="208"/>
-      <c r="I30" s="185"/>
-      <c r="J30" s="217"/>
-      <c r="K30" s="219"/>
+      <c r="F30" s="191"/>
+      <c r="G30" s="231"/>
+      <c r="H30" s="232"/>
+      <c r="I30" s="184"/>
+      <c r="J30" s="227"/>
+      <c r="K30" s="229"/>
     </row>
     <row r="31" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="150"/>
-      <c r="B31" s="168"/>
-      <c r="C31" s="168" t="s">
+      <c r="A31" s="176"/>
+      <c r="B31" s="178"/>
+      <c r="C31" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="168"/>
-      <c r="E31" s="166" t="s">
+      <c r="D31" s="178"/>
+      <c r="E31" s="190" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="167"/>
-      <c r="G31" s="205"/>
-      <c r="H31" s="206"/>
-      <c r="I31" s="186"/>
-      <c r="J31" s="218"/>
-      <c r="K31" s="220"/>
+      <c r="F31" s="191"/>
+      <c r="G31" s="233"/>
+      <c r="H31" s="234"/>
+      <c r="I31" s="185"/>
+      <c r="J31" s="228"/>
+      <c r="K31" s="230"/>
     </row>
     <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="149" t="s">
+      <c r="A32" s="174" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="151" t="s">
+      <c r="B32" s="199" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="152"/>
-      <c r="D32" s="153"/>
-      <c r="E32" s="154" t="s">
+      <c r="C32" s="200"/>
+      <c r="D32" s="201"/>
+      <c r="E32" s="202" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="155"/>
-      <c r="G32" s="207"/>
-      <c r="H32" s="208"/>
+      <c r="F32" s="203"/>
+      <c r="G32" s="231"/>
+      <c r="H32" s="232"/>
       <c r="I32" s="33">
         <v>0.4</v>
       </c>
@@ -3657,18 +3658,18 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="150"/>
-      <c r="B33" s="158" t="s">
+      <c r="A33" s="176"/>
+      <c r="B33" s="204" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="159"/>
-      <c r="D33" s="160"/>
-      <c r="E33" s="161" t="s">
+      <c r="C33" s="205"/>
+      <c r="D33" s="206"/>
+      <c r="E33" s="207" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="162"/>
-      <c r="G33" s="207"/>
-      <c r="H33" s="208"/>
+      <c r="F33" s="208"/>
+      <c r="G33" s="231"/>
+      <c r="H33" s="232"/>
       <c r="I33" s="33">
         <v>0.4</v>
       </c>
@@ -3682,16 +3683,16 @@
       <c r="A34" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="146" t="s">
+      <c r="B34" s="196" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="147"/>
-      <c r="D34" s="147"/>
-      <c r="E34" s="147"/>
-      <c r="F34" s="147"/>
-      <c r="G34" s="147"/>
-      <c r="H34" s="147"/>
-      <c r="I34" s="148"/>
+      <c r="C34" s="197"/>
+      <c r="D34" s="197"/>
+      <c r="E34" s="197"/>
+      <c r="F34" s="197"/>
+      <c r="G34" s="197"/>
+      <c r="H34" s="197"/>
+      <c r="I34" s="198"/>
       <c r="J34" s="78"/>
       <c r="K34" s="77"/>
     </row>
@@ -3775,21 +3776,17 @@
     <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="G28:H28"/>
@@ -3806,17 +3803,21 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
   </mergeCells>
   <conditionalFormatting sqref="K29:K37">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
@@ -3851,8 +3852,8 @@
   </sheetPr>
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -3900,9 +3901,9 @@
         <v>9</v>
       </c>
       <c r="B4" s="18"/>
-      <c r="C4" s="230"/>
-      <c r="D4" s="230"/>
-      <c r="E4" s="230"/>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
       <c r="F4" s="58"/>
       <c r="H4" s="56"/>
       <c r="I4" s="55" t="s">
@@ -3917,10 +3918,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="51"/>
-      <c r="C5" s="227"/>
-      <c r="D5" s="227"/>
-      <c r="E5" s="227"/>
-      <c r="F5" s="227"/>
+      <c r="C5" s="218"/>
+      <c r="D5" s="218"/>
+      <c r="E5" s="218"/>
+      <c r="F5" s="218"/>
       <c r="H5" s="56"/>
       <c r="I5" s="55" t="s">
         <v>8</v>
@@ -3931,7 +3932,7 @@
     </row>
     <row r="6" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>13</v>
@@ -3939,90 +3940,90 @@
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="51" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B7" s="51"/>
-      <c r="C7" s="227"/>
-      <c r="D7" s="227"/>
-      <c r="E7" s="227"/>
-      <c r="F7" s="227"/>
+      <c r="C7" s="218"/>
+      <c r="D7" s="218"/>
+      <c r="E7" s="218"/>
+      <c r="F7" s="218"/>
       <c r="H7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="228"/>
-      <c r="J7" s="229"/>
-      <c r="K7" s="229"/>
-      <c r="L7" s="229"/>
+      <c r="I7" s="219"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="220"/>
+      <c r="L7" s="220"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="18"/>
-      <c r="C8" s="230"/>
-      <c r="D8" s="230"/>
-      <c r="E8" s="230"/>
-      <c r="F8" s="230"/>
+      <c r="C8" s="221"/>
+      <c r="D8" s="221"/>
+      <c r="E8" s="221"/>
+      <c r="F8" s="221"/>
       <c r="H8" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="221"/>
-      <c r="J8" s="222"/>
-      <c r="K8" s="222"/>
-      <c r="L8" s="222"/>
+      <c r="I8" s="209"/>
+      <c r="J8" s="210"/>
+      <c r="K8" s="210"/>
+      <c r="L8" s="210"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="51"/>
-      <c r="C9" s="227"/>
-      <c r="D9" s="227"/>
-      <c r="E9" s="227"/>
-      <c r="F9" s="227"/>
+      <c r="C9" s="218"/>
+      <c r="D9" s="218"/>
+      <c r="E9" s="218"/>
+      <c r="F9" s="218"/>
       <c r="H9" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="221"/>
-      <c r="J9" s="222"/>
-      <c r="K9" s="222"/>
-      <c r="L9" s="222"/>
+      <c r="I9" s="209"/>
+      <c r="J9" s="210"/>
+      <c r="K9" s="210"/>
+      <c r="L9" s="210"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="51" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="51"/>
-      <c r="C10" s="227"/>
-      <c r="D10" s="227"/>
-      <c r="E10" s="227"/>
-      <c r="F10" s="227"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="218"/>
+      <c r="E10" s="218"/>
+      <c r="F10" s="218"/>
       <c r="H10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="221"/>
-      <c r="J10" s="222"/>
-      <c r="K10" s="222"/>
-      <c r="L10" s="222"/>
+      <c r="I10" s="209"/>
+      <c r="J10" s="210"/>
+      <c r="K10" s="210"/>
+      <c r="L10" s="210"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="221"/>
-      <c r="J11" s="222"/>
-      <c r="K11" s="222"/>
-      <c r="L11" s="222"/>
+      <c r="I11" s="209"/>
+      <c r="J11" s="210"/>
+      <c r="K11" s="210"/>
+      <c r="L11" s="210"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="52"/>
       <c r="H12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="221"/>
-      <c r="J12" s="222"/>
-      <c r="K12" s="222"/>
-      <c r="L12" s="222"/>
+      <c r="I12" s="209"/>
+      <c r="J12" s="210"/>
+      <c r="K12" s="210"/>
+      <c r="L12" s="210"/>
     </row>
     <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="50"/>
@@ -4038,97 +4039,97 @@
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
-      <c r="H14" s="174" t="s">
+      <c r="H14" s="169" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="175"/>
-      <c r="J14" s="176" t="s">
+      <c r="I14" s="170"/>
+      <c r="J14" s="171" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="177"/>
-      <c r="L14" s="178"/>
+      <c r="K14" s="172"/>
+      <c r="L14" s="173"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="246" t="s">
+      <c r="A15" s="235" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="259" t="s">
+      <c r="B15" s="238" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="259" t="s">
+      <c r="C15" s="238" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="259"/>
-      <c r="E15" s="259"/>
-      <c r="F15" s="251" t="s">
+      <c r="D15" s="238"/>
+      <c r="E15" s="238"/>
+      <c r="F15" s="240" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="261"/>
-      <c r="H15" s="215"/>
-      <c r="I15" s="216"/>
-      <c r="J15" s="184">
+      <c r="G15" s="241"/>
+      <c r="H15" s="225"/>
+      <c r="I15" s="226"/>
+      <c r="J15" s="183">
         <v>0.2</v>
       </c>
-      <c r="K15" s="217">
-        <v>0</v>
-      </c>
-      <c r="L15" s="219">
+      <c r="K15" s="227">
+        <v>0</v>
+      </c>
+      <c r="L15" s="229">
         <f>K15*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="258"/>
-      <c r="B16" s="259"/>
-      <c r="C16" s="259" t="s">
+      <c r="A16" s="236"/>
+      <c r="B16" s="238"/>
+      <c r="C16" s="238" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="259"/>
-      <c r="E16" s="259"/>
-      <c r="F16" s="262" t="s">
+      <c r="D16" s="238"/>
+      <c r="E16" s="238"/>
+      <c r="F16" s="242" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="263"/>
-      <c r="H16" s="207"/>
-      <c r="I16" s="208"/>
-      <c r="J16" s="185"/>
-      <c r="K16" s="217"/>
-      <c r="L16" s="219"/>
+      <c r="G16" s="243"/>
+      <c r="H16" s="231"/>
+      <c r="I16" s="232"/>
+      <c r="J16" s="184"/>
+      <c r="K16" s="227"/>
+      <c r="L16" s="229"/>
     </row>
     <row r="17" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="247"/>
-      <c r="B17" s="260"/>
-      <c r="C17" s="260" t="s">
+      <c r="A17" s="237"/>
+      <c r="B17" s="239"/>
+      <c r="C17" s="239" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="260"/>
-      <c r="E17" s="260"/>
-      <c r="F17" s="262" t="s">
+      <c r="D17" s="239"/>
+      <c r="E17" s="239"/>
+      <c r="F17" s="242" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="263"/>
-      <c r="H17" s="205"/>
-      <c r="I17" s="206"/>
-      <c r="J17" s="186"/>
-      <c r="K17" s="218"/>
-      <c r="L17" s="220"/>
+      <c r="G17" s="243"/>
+      <c r="H17" s="233"/>
+      <c r="I17" s="234"/>
+      <c r="J17" s="185"/>
+      <c r="K17" s="228"/>
+      <c r="L17" s="230"/>
     </row>
     <row r="18" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="246" t="s">
+      <c r="A18" s="235" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="248" t="s">
+      <c r="B18" s="244" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="249"/>
-      <c r="D18" s="249"/>
-      <c r="E18" s="250"/>
-      <c r="F18" s="251" t="s">
+      <c r="C18" s="245"/>
+      <c r="D18" s="245"/>
+      <c r="E18" s="246"/>
+      <c r="F18" s="240" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="252"/>
-      <c r="H18" s="207"/>
-      <c r="I18" s="208"/>
+      <c r="G18" s="247"/>
+      <c r="H18" s="231"/>
+      <c r="I18" s="232"/>
       <c r="J18" s="33">
         <v>0.4</v>
       </c>
@@ -4142,19 +4143,19 @@
       <c r="M18" s="61"/>
     </row>
     <row r="19" spans="1:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="247"/>
-      <c r="B19" s="253" t="s">
+      <c r="A19" s="237"/>
+      <c r="B19" s="248" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="254"/>
-      <c r="D19" s="254"/>
-      <c r="E19" s="255"/>
-      <c r="F19" s="256" t="s">
+      <c r="C19" s="249"/>
+      <c r="D19" s="249"/>
+      <c r="E19" s="250"/>
+      <c r="F19" s="251" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="257"/>
-      <c r="H19" s="207"/>
-      <c r="I19" s="208"/>
+      <c r="G19" s="252"/>
+      <c r="H19" s="231"/>
+      <c r="I19" s="232"/>
       <c r="J19" s="33">
         <v>0.4</v>
       </c>
@@ -4170,17 +4171,17 @@
       <c r="A20" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="146" t="s">
+      <c r="B20" s="196" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="147"/>
-      <c r="D20" s="147"/>
-      <c r="E20" s="147"/>
-      <c r="F20" s="147"/>
-      <c r="G20" s="147"/>
-      <c r="H20" s="147"/>
-      <c r="I20" s="147"/>
-      <c r="J20" s="148"/>
+      <c r="C20" s="197"/>
+      <c r="D20" s="197"/>
+      <c r="E20" s="197"/>
+      <c r="F20" s="197"/>
+      <c r="G20" s="197"/>
+      <c r="H20" s="197"/>
+      <c r="I20" s="197"/>
+      <c r="J20" s="198"/>
       <c r="K20" s="32"/>
       <c r="L20" s="79"/>
     </row>
@@ -4198,90 +4199,90 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="237" t="s">
+      <c r="A23" s="253" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="238"/>
-      <c r="C23" s="238"/>
-      <c r="D23" s="238"/>
-      <c r="E23" s="238"/>
-      <c r="F23" s="238"/>
-      <c r="G23" s="238"/>
-      <c r="H23" s="238"/>
-      <c r="I23" s="238"/>
-      <c r="J23" s="238"/>
-      <c r="K23" s="238"/>
-      <c r="L23" s="239"/>
+      <c r="B23" s="254"/>
+      <c r="C23" s="254"/>
+      <c r="D23" s="254"/>
+      <c r="E23" s="254"/>
+      <c r="F23" s="254"/>
+      <c r="G23" s="254"/>
+      <c r="H23" s="254"/>
+      <c r="I23" s="254"/>
+      <c r="J23" s="254"/>
+      <c r="K23" s="254"/>
+      <c r="L23" s="255"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="240"/>
-      <c r="B24" s="241"/>
-      <c r="C24" s="241"/>
-      <c r="D24" s="241"/>
-      <c r="E24" s="241"/>
-      <c r="F24" s="241"/>
-      <c r="G24" s="241"/>
-      <c r="H24" s="241"/>
-      <c r="I24" s="241"/>
-      <c r="J24" s="241"/>
-      <c r="K24" s="241"/>
-      <c r="L24" s="242"/>
+      <c r="A24" s="256"/>
+      <c r="B24" s="257"/>
+      <c r="C24" s="257"/>
+      <c r="D24" s="257"/>
+      <c r="E24" s="257"/>
+      <c r="F24" s="257"/>
+      <c r="G24" s="257"/>
+      <c r="H24" s="257"/>
+      <c r="I24" s="257"/>
+      <c r="J24" s="257"/>
+      <c r="K24" s="257"/>
+      <c r="L24" s="258"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="240"/>
-      <c r="B25" s="241"/>
-      <c r="C25" s="241"/>
-      <c r="D25" s="241"/>
-      <c r="E25" s="241"/>
-      <c r="F25" s="241"/>
-      <c r="G25" s="241"/>
-      <c r="H25" s="241"/>
-      <c r="I25" s="241"/>
-      <c r="J25" s="241"/>
-      <c r="K25" s="241"/>
-      <c r="L25" s="242"/>
+      <c r="A25" s="256"/>
+      <c r="B25" s="257"/>
+      <c r="C25" s="257"/>
+      <c r="D25" s="257"/>
+      <c r="E25" s="257"/>
+      <c r="F25" s="257"/>
+      <c r="G25" s="257"/>
+      <c r="H25" s="257"/>
+      <c r="I25" s="257"/>
+      <c r="J25" s="257"/>
+      <c r="K25" s="257"/>
+      <c r="L25" s="258"/>
     </row>
     <row r="26" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="240"/>
-      <c r="B26" s="241"/>
-      <c r="C26" s="241"/>
-      <c r="D26" s="241"/>
-      <c r="E26" s="241"/>
-      <c r="F26" s="241"/>
-      <c r="G26" s="241"/>
-      <c r="H26" s="241"/>
-      <c r="I26" s="241"/>
-      <c r="J26" s="241"/>
-      <c r="K26" s="241"/>
-      <c r="L26" s="242"/>
+      <c r="A26" s="256"/>
+      <c r="B26" s="257"/>
+      <c r="C26" s="257"/>
+      <c r="D26" s="257"/>
+      <c r="E26" s="257"/>
+      <c r="F26" s="257"/>
+      <c r="G26" s="257"/>
+      <c r="H26" s="257"/>
+      <c r="I26" s="257"/>
+      <c r="J26" s="257"/>
+      <c r="K26" s="257"/>
+      <c r="L26" s="258"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="243"/>
-      <c r="B27" s="244"/>
-      <c r="C27" s="244"/>
-      <c r="D27" s="244"/>
-      <c r="E27" s="244"/>
-      <c r="F27" s="244"/>
-      <c r="G27" s="244"/>
-      <c r="H27" s="244"/>
-      <c r="I27" s="244"/>
-      <c r="J27" s="244"/>
-      <c r="K27" s="244"/>
-      <c r="L27" s="245"/>
+      <c r="A27" s="259"/>
+      <c r="B27" s="260"/>
+      <c r="C27" s="260"/>
+      <c r="D27" s="260"/>
+      <c r="E27" s="260"/>
+      <c r="F27" s="260"/>
+      <c r="G27" s="260"/>
+      <c r="H27" s="260"/>
+      <c r="I27" s="260"/>
+      <c r="J27" s="260"/>
+      <c r="K27" s="260"/>
+      <c r="L27" s="261"/>
     </row>
     <row r="29" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="234" t="s">
+      <c r="A29" s="262" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="234"/>
-      <c r="C29" s="234"/>
-      <c r="D29" s="234"/>
-      <c r="E29" s="234"/>
-      <c r="F29" s="234"/>
-      <c r="G29" s="234"/>
-      <c r="H29" s="234"/>
-      <c r="I29" s="235"/>
-      <c r="J29" s="235"/>
+      <c r="B29" s="262"/>
+      <c r="C29" s="262"/>
+      <c r="D29" s="262"/>
+      <c r="E29" s="262"/>
+      <c r="F29" s="262"/>
+      <c r="G29" s="262"/>
+      <c r="H29" s="262"/>
+      <c r="I29" s="263"/>
+      <c r="J29" s="263"/>
       <c r="K29" s="63" t="s">
         <v>72</v>
       </c>
@@ -4291,18 +4292,18 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="234" t="s">
+      <c r="A30" s="262" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="234"/>
-      <c r="C30" s="234"/>
-      <c r="D30" s="234"/>
-      <c r="E30" s="234"/>
-      <c r="F30" s="234"/>
-      <c r="G30" s="234"/>
-      <c r="H30" s="234"/>
-      <c r="I30" s="235"/>
-      <c r="J30" s="235"/>
+      <c r="B30" s="262"/>
+      <c r="C30" s="262"/>
+      <c r="D30" s="262"/>
+      <c r="E30" s="262"/>
+      <c r="F30" s="262"/>
+      <c r="G30" s="262"/>
+      <c r="H30" s="262"/>
+      <c r="I30" s="263"/>
+      <c r="J30" s="263"/>
       <c r="K30" s="48" t="s">
         <v>72</v>
       </c>
@@ -4312,18 +4313,18 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="234" t="s">
+      <c r="A31" s="262" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="234"/>
-      <c r="C31" s="234"/>
-      <c r="D31" s="234"/>
-      <c r="E31" s="234"/>
-      <c r="F31" s="234"/>
-      <c r="G31" s="234"/>
-      <c r="H31" s="234"/>
-      <c r="I31" s="235"/>
-      <c r="J31" s="235"/>
+      <c r="B31" s="262"/>
+      <c r="C31" s="262"/>
+      <c r="D31" s="262"/>
+      <c r="E31" s="262"/>
+      <c r="F31" s="262"/>
+      <c r="G31" s="262"/>
+      <c r="H31" s="262"/>
+      <c r="I31" s="263"/>
+      <c r="J31" s="263"/>
       <c r="K31" s="48" t="s">
         <v>75</v>
       </c>
@@ -4333,18 +4334,18 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="234" t="s">
+      <c r="A32" s="262" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="234"/>
-      <c r="C32" s="234"/>
-      <c r="D32" s="234"/>
-      <c r="E32" s="234"/>
-      <c r="F32" s="234"/>
-      <c r="G32" s="234"/>
-      <c r="H32" s="234"/>
-      <c r="I32" s="235"/>
-      <c r="J32" s="235"/>
+      <c r="B32" s="262"/>
+      <c r="C32" s="262"/>
+      <c r="D32" s="262"/>
+      <c r="E32" s="262"/>
+      <c r="F32" s="262"/>
+      <c r="G32" s="262"/>
+      <c r="H32" s="262"/>
+      <c r="I32" s="263"/>
+      <c r="J32" s="263"/>
       <c r="K32" s="48" t="s">
         <v>53</v>
       </c>
@@ -4354,21 +4355,21 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="234" t="s">
+      <c r="A33" s="262" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="234"/>
-      <c r="C33" s="234"/>
-      <c r="D33" s="234"/>
-      <c r="E33" s="234"/>
-      <c r="F33" s="234"/>
-      <c r="G33" s="234"/>
-      <c r="H33" s="234"/>
-      <c r="I33" s="236">
+      <c r="B33" s="262"/>
+      <c r="C33" s="262"/>
+      <c r="D33" s="262"/>
+      <c r="E33" s="262"/>
+      <c r="F33" s="262"/>
+      <c r="G33" s="262"/>
+      <c r="H33" s="262"/>
+      <c r="I33" s="267">
         <f>L21</f>
         <v>0</v>
       </c>
-      <c r="J33" s="236"/>
+      <c r="J33" s="267"/>
       <c r="K33" s="48" t="s">
         <v>75</v>
       </c>
@@ -4390,14 +4391,14 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F35" s="231" t="s">
+      <c r="F35" s="264" t="s">
         <v>79</v>
       </c>
-      <c r="G35" s="232"/>
-      <c r="H35" s="232"/>
-      <c r="I35" s="232"/>
-      <c r="J35" s="232"/>
-      <c r="K35" s="233"/>
+      <c r="G35" s="265"/>
+      <c r="H35" s="265"/>
+      <c r="I35" s="265"/>
+      <c r="J35" s="265"/>
+      <c r="K35" s="266"/>
       <c r="L35" s="67">
         <f>L34/10</f>
         <v>0</v>
@@ -4488,18 +4489,26 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="A23:L27"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="A15:A17"/>
@@ -4516,26 +4525,18 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="A23:L27"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
   </mergeCells>
   <conditionalFormatting sqref="L15:L39 I33:J33">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
@@ -4564,6 +4565,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4629,37 +4648,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4680,9 +4672,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Better cplumn with in excel
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll_2019_mixklass lag(mall).xlsx
+++ b/mallar/Protokoll/Protokoll_2019_mixklass lag(mall).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F6CCD7-F606-42BE-BABB-C141817E02EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A899FA7C-0F34-4E02-8879-5F0813A61ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="8820" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="27" r:id="rId1"/>
@@ -1289,6 +1289,149 @@
     <xf numFmtId="166" fontId="30" fillId="0" borderId="17" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="12" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="2" borderId="21" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="12" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="21" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1306,12 +1449,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1327,14 +1464,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1350,146 +1479,40 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="12" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="21" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="12" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="21" xfId="14" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
@@ -1499,15 +1522,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1529,40 +1543,98 @@
     <xf numFmtId="167" fontId="4" fillId="0" borderId="21" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1571,89 +1643,17 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -1683,11 +1683,29 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1703,19 +1721,19 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1731,30 +1749,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1777,9 +1777,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1817,9 +1817,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1852,26 +1852,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1904,26 +1887,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2474,15 +2440,16 @@
   </sheetPr>
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:E7"/>
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.73046875" style="88" customWidth="1"/>
     <col min="3" max="3" width="11.265625" style="88" customWidth="1"/>
-    <col min="4" max="10" width="7.59765625" style="88" customWidth="1"/>
+    <col min="4" max="9" width="7.59765625" style="88" customWidth="1"/>
+    <col min="10" max="10" width="8.73046875" style="88" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" style="88" customWidth="1"/>
     <col min="12" max="12" width="7.73046875" style="88" hidden="1" customWidth="1"/>
     <col min="13" max="16384" width="9" style="88"/>
@@ -2522,8 +2489,8 @@
         <v>9</v>
       </c>
       <c r="B4" s="131"/>
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
       <c r="E4" s="132"/>
       <c r="G4" s="90"/>
       <c r="H4" s="91" t="s">
@@ -2538,9 +2505,9 @@
         <v>10</v>
       </c>
       <c r="B5" s="133"/>
-      <c r="C5" s="187"/>
-      <c r="D5" s="187"/>
-      <c r="E5" s="187"/>
+      <c r="C5" s="142"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
       <c r="G5" s="90"/>
       <c r="H5" s="91" t="s">
         <v>8</v>
@@ -2566,83 +2533,83 @@
         <v>39</v>
       </c>
       <c r="B7" s="133"/>
-      <c r="C7" s="187"/>
-      <c r="D7" s="187"/>
-      <c r="E7" s="187"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="142"/>
+      <c r="E7" s="142"/>
       <c r="G7" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="197"/>
-      <c r="I7" s="198"/>
-      <c r="J7" s="198"/>
-      <c r="K7" s="198"/>
+      <c r="H7" s="143"/>
+      <c r="I7" s="144"/>
+      <c r="J7" s="144"/>
+      <c r="K7" s="144"/>
     </row>
     <row r="8" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="95" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="131"/>
-      <c r="C8" s="199"/>
-      <c r="D8" s="199"/>
-      <c r="E8" s="199"/>
+      <c r="C8" s="145"/>
+      <c r="D8" s="145"/>
+      <c r="E8" s="145"/>
       <c r="G8" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="188"/>
-      <c r="I8" s="189"/>
-      <c r="J8" s="189"/>
-      <c r="K8" s="189"/>
+      <c r="H8" s="146"/>
+      <c r="I8" s="147"/>
+      <c r="J8" s="147"/>
+      <c r="K8" s="147"/>
     </row>
     <row r="9" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="133"/>
-      <c r="C9" s="187"/>
-      <c r="D9" s="187"/>
-      <c r="E9" s="187"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
       <c r="G9" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="188"/>
-      <c r="I9" s="189"/>
-      <c r="J9" s="189"/>
-      <c r="K9" s="189"/>
+      <c r="H9" s="146"/>
+      <c r="I9" s="147"/>
+      <c r="J9" s="147"/>
+      <c r="K9" s="147"/>
     </row>
     <row r="10" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="96" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="133"/>
-      <c r="C10" s="187"/>
-      <c r="D10" s="187"/>
-      <c r="E10" s="187"/>
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
       <c r="G10" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="188"/>
-      <c r="I10" s="189"/>
-      <c r="J10" s="189"/>
-      <c r="K10" s="189"/>
+      <c r="H10" s="146"/>
+      <c r="I10" s="147"/>
+      <c r="J10" s="147"/>
+      <c r="K10" s="147"/>
     </row>
     <row r="11" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="188"/>
-      <c r="I11" s="189"/>
-      <c r="J11" s="189"/>
-      <c r="K11" s="189"/>
+      <c r="H11" s="146"/>
+      <c r="I11" s="147"/>
+      <c r="J11" s="147"/>
+      <c r="K11" s="147"/>
     </row>
     <row r="12" spans="1:11" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="98"/>
       <c r="G12" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="188"/>
-      <c r="I12" s="189"/>
-      <c r="J12" s="189"/>
-      <c r="K12" s="189"/>
+      <c r="H12" s="146"/>
+      <c r="I12" s="147"/>
+      <c r="J12" s="147"/>
+      <c r="K12" s="147"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="99"/>
@@ -2672,119 +2639,201 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="190" t="s">
+      <c r="A15" s="151" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="191"/>
-      <c r="C15" s="192"/>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
-      <c r="F15" s="135"/>
-      <c r="G15" s="135"/>
-      <c r="H15" s="135"/>
-      <c r="I15" s="135"/>
+      <c r="B15" s="152"/>
+      <c r="C15" s="153"/>
+      <c r="D15" s="135">
+        <v>0</v>
+      </c>
+      <c r="E15" s="135">
+        <v>0</v>
+      </c>
+      <c r="F15" s="135">
+        <v>0</v>
+      </c>
+      <c r="G15" s="135">
+        <v>0</v>
+      </c>
+      <c r="H15" s="135">
+        <v>0</v>
+      </c>
+      <c r="I15" s="135">
+        <v>0</v>
+      </c>
       <c r="J15" s="102">
         <f>SUM(D15:I15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="190" t="s">
+      <c r="A16" s="151" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="191"/>
-      <c r="C16" s="192"/>
-      <c r="D16" s="135"/>
-      <c r="E16" s="135"/>
-      <c r="F16" s="135"/>
-      <c r="G16" s="135"/>
+      <c r="B16" s="152"/>
+      <c r="C16" s="153"/>
+      <c r="D16" s="135">
+        <v>0</v>
+      </c>
+      <c r="E16" s="135">
+        <v>0</v>
+      </c>
+      <c r="F16" s="135">
+        <v>0</v>
+      </c>
+      <c r="G16" s="135">
+        <v>0</v>
+      </c>
       <c r="H16" s="135"/>
-      <c r="I16" s="135"/>
+      <c r="I16" s="135">
+        <v>0</v>
+      </c>
       <c r="J16" s="102">
         <f>SUM(D16:I16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="184" t="s">
+      <c r="A17" s="148" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="185"/>
-      <c r="C17" s="186"/>
-      <c r="D17" s="135"/>
-      <c r="E17" s="135"/>
-      <c r="F17" s="135"/>
-      <c r="G17" s="135"/>
-      <c r="H17" s="135"/>
-      <c r="I17" s="135"/>
+      <c r="B17" s="149"/>
+      <c r="C17" s="150"/>
+      <c r="D17" s="135">
+        <v>0</v>
+      </c>
+      <c r="E17" s="135">
+        <v>0</v>
+      </c>
+      <c r="F17" s="135">
+        <v>0</v>
+      </c>
+      <c r="G17" s="135">
+        <v>0</v>
+      </c>
+      <c r="H17" s="135">
+        <v>0</v>
+      </c>
+      <c r="I17" s="135">
+        <v>0</v>
+      </c>
       <c r="J17" s="102">
         <f t="shared" ref="J17:J21" si="0">SUM(D17:I17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="21.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="184" t="s">
+      <c r="A18" s="148" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="185"/>
-      <c r="C18" s="186"/>
-      <c r="D18" s="135"/>
-      <c r="E18" s="135"/>
-      <c r="F18" s="135"/>
-      <c r="G18" s="135"/>
-      <c r="H18" s="135"/>
-      <c r="I18" s="135"/>
+      <c r="B18" s="149"/>
+      <c r="C18" s="150"/>
+      <c r="D18" s="135">
+        <v>0</v>
+      </c>
+      <c r="E18" s="135">
+        <v>0</v>
+      </c>
+      <c r="F18" s="135">
+        <v>0</v>
+      </c>
+      <c r="G18" s="135">
+        <v>0</v>
+      </c>
+      <c r="H18" s="135">
+        <v>0</v>
+      </c>
+      <c r="I18" s="135">
+        <v>0</v>
+      </c>
       <c r="J18" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="193" t="s">
+      <c r="A19" s="154" t="s">
         <v>109</v>
       </c>
-      <c r="B19" s="194"/>
-      <c r="C19" s="195"/>
-      <c r="D19" s="135"/>
-      <c r="E19" s="135"/>
-      <c r="F19" s="135"/>
-      <c r="G19" s="135"/>
-      <c r="H19" s="135"/>
-      <c r="I19" s="135"/>
+      <c r="B19" s="155"/>
+      <c r="C19" s="156"/>
+      <c r="D19" s="135">
+        <v>0</v>
+      </c>
+      <c r="E19" s="135">
+        <v>0</v>
+      </c>
+      <c r="F19" s="135">
+        <v>0</v>
+      </c>
+      <c r="G19" s="135">
+        <v>0</v>
+      </c>
+      <c r="H19" s="135">
+        <v>0</v>
+      </c>
+      <c r="I19" s="135">
+        <v>0</v>
+      </c>
       <c r="J19" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="20.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="184" t="s">
+      <c r="A20" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="185"/>
-      <c r="C20" s="186"/>
-      <c r="D20" s="135"/>
-      <c r="E20" s="135"/>
-      <c r="F20" s="135"/>
-      <c r="G20" s="135"/>
-      <c r="H20" s="135"/>
-      <c r="I20" s="135"/>
+      <c r="B20" s="149"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="135">
+        <v>0</v>
+      </c>
+      <c r="E20" s="135">
+        <v>0</v>
+      </c>
+      <c r="F20" s="135">
+        <v>0</v>
+      </c>
+      <c r="G20" s="135">
+        <v>0</v>
+      </c>
+      <c r="H20" s="135">
+        <v>0</v>
+      </c>
+      <c r="I20" s="135">
+        <v>0</v>
+      </c>
       <c r="J20" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="160" t="s">
+      <c r="A21" s="157" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="161"/>
-      <c r="C21" s="162"/>
-      <c r="D21" s="135"/>
-      <c r="E21" s="135"/>
-      <c r="F21" s="135"/>
-      <c r="G21" s="135"/>
-      <c r="H21" s="135"/>
-      <c r="I21" s="135"/>
+      <c r="B21" s="158"/>
+      <c r="C21" s="159"/>
+      <c r="D21" s="135">
+        <v>0</v>
+      </c>
+      <c r="E21" s="135">
+        <v>0</v>
+      </c>
+      <c r="F21" s="135">
+        <v>0</v>
+      </c>
+      <c r="G21" s="135">
+        <v>0</v>
+      </c>
+      <c r="H21" s="135">
+        <v>0</v>
+      </c>
+      <c r="I21" s="135">
+        <v>0</v>
+      </c>
       <c r="J21" s="102">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2817,7 +2866,7 @@
         <v>90</v>
       </c>
       <c r="H24" s="136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" s="109"/>
       <c r="J24" s="110">
@@ -2867,91 +2916,91 @@
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
       <c r="F29" s="34"/>
-      <c r="G29" s="163" t="s">
+      <c r="G29" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="H29" s="164"/>
-      <c r="I29" s="165" t="s">
+      <c r="H29" s="161"/>
+      <c r="I29" s="162" t="s">
         <v>38</v>
       </c>
-      <c r="J29" s="166"/>
-      <c r="K29" s="167"/>
+      <c r="J29" s="163"/>
+      <c r="K29" s="164"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="146" t="s">
+      <c r="A30" s="165" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="169" t="s">
+      <c r="B30" s="168" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="169" t="s">
+      <c r="C30" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="169"/>
-      <c r="E30" s="171" t="s">
+      <c r="D30" s="168"/>
+      <c r="E30" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="F30" s="172"/>
-      <c r="G30" s="173"/>
-      <c r="H30" s="174"/>
-      <c r="I30" s="175">
+      <c r="F30" s="171"/>
+      <c r="G30" s="172"/>
+      <c r="H30" s="173"/>
+      <c r="I30" s="174">
         <v>0.2</v>
       </c>
-      <c r="J30" s="178"/>
-      <c r="K30" s="180">
+      <c r="J30" s="177"/>
+      <c r="K30" s="179">
         <f>J30*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="168"/>
-      <c r="B31" s="169"/>
-      <c r="C31" s="169" t="s">
+      <c r="A31" s="166"/>
+      <c r="B31" s="168"/>
+      <c r="C31" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="169"/>
-      <c r="E31" s="182" t="s">
+      <c r="D31" s="168"/>
+      <c r="E31" s="181" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="183"/>
-      <c r="G31" s="153"/>
-      <c r="H31" s="154"/>
-      <c r="I31" s="176"/>
-      <c r="J31" s="178"/>
-      <c r="K31" s="180"/>
+      <c r="F31" s="182"/>
+      <c r="G31" s="183"/>
+      <c r="H31" s="184"/>
+      <c r="I31" s="175"/>
+      <c r="J31" s="177"/>
+      <c r="K31" s="179"/>
     </row>
     <row r="32" spans="1:11" ht="28.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="147"/>
-      <c r="B32" s="170"/>
-      <c r="C32" s="170" t="s">
+      <c r="A32" s="167"/>
+      <c r="B32" s="169"/>
+      <c r="C32" s="169" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="170"/>
-      <c r="E32" s="182" t="s">
+      <c r="D32" s="169"/>
+      <c r="E32" s="181" t="s">
         <v>58</v>
       </c>
-      <c r="F32" s="183"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="142"/>
-      <c r="I32" s="177"/>
-      <c r="J32" s="179"/>
-      <c r="K32" s="181"/>
+      <c r="F32" s="182"/>
+      <c r="G32" s="185"/>
+      <c r="H32" s="186"/>
+      <c r="I32" s="176"/>
+      <c r="J32" s="178"/>
+      <c r="K32" s="180"/>
     </row>
     <row r="33" spans="1:11" ht="30.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="146" t="s">
+      <c r="A33" s="165" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="148" t="s">
+      <c r="B33" s="190" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="149"/>
-      <c r="D33" s="150"/>
-      <c r="E33" s="151" t="s">
+      <c r="C33" s="191"/>
+      <c r="D33" s="192"/>
+      <c r="E33" s="193" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="152"/>
-      <c r="G33" s="153"/>
-      <c r="H33" s="154"/>
+      <c r="F33" s="194"/>
+      <c r="G33" s="183"/>
+      <c r="H33" s="184"/>
       <c r="I33" s="33">
         <v>0.4</v>
       </c>
@@ -2962,18 +3011,18 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="147"/>
-      <c r="B34" s="155" t="s">
+      <c r="A34" s="167"/>
+      <c r="B34" s="195" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="156"/>
-      <c r="D34" s="157"/>
-      <c r="E34" s="158" t="s">
+      <c r="C34" s="196"/>
+      <c r="D34" s="197"/>
+      <c r="E34" s="198" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="159"/>
-      <c r="G34" s="153"/>
-      <c r="H34" s="154"/>
+      <c r="F34" s="199"/>
+      <c r="G34" s="183"/>
+      <c r="H34" s="184"/>
       <c r="I34" s="33">
         <v>0.4</v>
       </c>
@@ -2987,16 +3036,16 @@
       <c r="A35" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="143" t="s">
+      <c r="B35" s="187" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="144"/>
-      <c r="D35" s="144"/>
-      <c r="E35" s="144"/>
-      <c r="F35" s="144"/>
-      <c r="G35" s="144"/>
-      <c r="H35" s="144"/>
-      <c r="I35" s="145"/>
+      <c r="C35" s="188"/>
+      <c r="D35" s="188"/>
+      <c r="E35" s="188"/>
+      <c r="F35" s="188"/>
+      <c r="G35" s="188"/>
+      <c r="H35" s="188"/>
+      <c r="I35" s="189"/>
       <c r="J35" s="122"/>
       <c r="K35" s="137"/>
     </row>
@@ -3080,24 +3129,15 @@
     <row r="48" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B35:I35"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:H34"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="I29:K29"/>
@@ -3114,25 +3154,34 @@
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B35:I35"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
   </mergeCells>
-  <conditionalFormatting sqref="K30:K38">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+  <conditionalFormatting sqref="J30:J35 K30:K38">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="notBetween">
       <formula>0</formula>
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J30:J35 K30:K38">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="notBetween">
+  <conditionalFormatting sqref="K30:K38">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>0</formula>
-      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35">
@@ -3157,7 +3206,7 @@
   </sheetPr>
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A9" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -3200,8 +3249,8 @@
         <v>9</v>
       </c>
       <c r="B4" s="18"/>
-      <c r="C4" s="221"/>
-      <c r="D4" s="221"/>
+      <c r="C4" s="208"/>
+      <c r="D4" s="208"/>
       <c r="E4" s="58"/>
       <c r="G4" s="56"/>
       <c r="H4" s="55" t="s">
@@ -3216,9 +3265,9 @@
         <v>10</v>
       </c>
       <c r="B5" s="51"/>
-      <c r="C5" s="222"/>
-      <c r="D5" s="222"/>
-      <c r="E5" s="222"/>
+      <c r="C5" s="209"/>
+      <c r="D5" s="209"/>
+      <c r="E5" s="209"/>
       <c r="G5" s="56"/>
       <c r="H5" s="55" t="s">
         <v>8</v>
@@ -3240,83 +3289,83 @@
         <v>39</v>
       </c>
       <c r="B7" s="51"/>
-      <c r="C7" s="222"/>
-      <c r="D7" s="222"/>
-      <c r="E7" s="222"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
       <c r="G7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="223"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
+      <c r="H7" s="210"/>
+      <c r="I7" s="211"/>
+      <c r="J7" s="211"/>
+      <c r="K7" s="211"/>
     </row>
     <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="18"/>
-      <c r="C8" s="225"/>
-      <c r="D8" s="225"/>
-      <c r="E8" s="225"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
       <c r="G8" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="216"/>
-      <c r="I8" s="217"/>
-      <c r="J8" s="217"/>
-      <c r="K8" s="217"/>
+      <c r="H8" s="200"/>
+      <c r="I8" s="201"/>
+      <c r="J8" s="201"/>
+      <c r="K8" s="201"/>
     </row>
     <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="51"/>
-      <c r="C9" s="222"/>
-      <c r="D9" s="222"/>
-      <c r="E9" s="222"/>
+      <c r="C9" s="209"/>
+      <c r="D9" s="209"/>
+      <c r="E9" s="209"/>
       <c r="G9" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="216"/>
-      <c r="I9" s="217"/>
-      <c r="J9" s="217"/>
-      <c r="K9" s="217"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="201"/>
+      <c r="J9" s="201"/>
+      <c r="K9" s="201"/>
     </row>
     <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="51" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="51"/>
-      <c r="C10" s="222"/>
-      <c r="D10" s="222"/>
-      <c r="E10" s="222"/>
+      <c r="C10" s="209"/>
+      <c r="D10" s="209"/>
+      <c r="E10" s="209"/>
       <c r="G10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="216"/>
-      <c r="I10" s="217"/>
-      <c r="J10" s="217"/>
-      <c r="K10" s="217"/>
+      <c r="H10" s="200"/>
+      <c r="I10" s="201"/>
+      <c r="J10" s="201"/>
+      <c r="K10" s="201"/>
     </row>
     <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G11" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="216"/>
-      <c r="I11" s="217"/>
-      <c r="J11" s="217"/>
-      <c r="K11" s="217"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="201"/>
+      <c r="J11" s="201"/>
+      <c r="K11" s="201"/>
     </row>
     <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="52"/>
       <c r="G12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="216"/>
-      <c r="I12" s="217"/>
-      <c r="J12" s="217"/>
-      <c r="K12" s="217"/>
+      <c r="H12" s="200"/>
+      <c r="I12" s="201"/>
+      <c r="J12" s="201"/>
+      <c r="K12" s="201"/>
     </row>
     <row r="13" spans="1:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="50"/>
@@ -3346,11 +3395,11 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="218" t="s">
+      <c r="A15" s="202" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="219"/>
-      <c r="C15" s="220"/>
+      <c r="B15" s="203"/>
+      <c r="C15" s="204"/>
       <c r="D15" s="71">
         <v>0</v>
       </c>
@@ -3367,11 +3416,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="207" t="s">
+      <c r="A16" s="205" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="208"/>
-      <c r="C16" s="209"/>
+      <c r="B16" s="206"/>
+      <c r="C16" s="207"/>
       <c r="D16" s="71">
         <v>0</v>
       </c>
@@ -3388,11 +3437,11 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="207" t="s">
+      <c r="A17" s="205" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="208"/>
-      <c r="C17" s="209"/>
+      <c r="B17" s="206"/>
+      <c r="C17" s="207"/>
       <c r="D17" s="71">
         <v>0</v>
       </c>
@@ -3409,11 +3458,11 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="204" t="s">
+      <c r="A18" s="213" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="205"/>
-      <c r="C18" s="206"/>
+      <c r="B18" s="214"/>
+      <c r="C18" s="215"/>
       <c r="D18" s="71">
         <v>0</v>
       </c>
@@ -3430,11 +3479,11 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="207" t="s">
+      <c r="A19" s="205" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="208"/>
-      <c r="C19" s="209"/>
+      <c r="B19" s="206"/>
+      <c r="C19" s="207"/>
       <c r="D19" s="71">
         <v>0</v>
       </c>
@@ -3451,11 +3500,11 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="207" t="s">
+      <c r="A20" s="205" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="208"/>
-      <c r="C20" s="209"/>
+      <c r="B20" s="206"/>
+      <c r="C20" s="207"/>
       <c r="D20" s="71">
         <v>0</v>
       </c>
@@ -3548,91 +3597,91 @@
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
       <c r="F28" s="34"/>
-      <c r="G28" s="163" t="s">
+      <c r="G28" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="H28" s="164"/>
-      <c r="I28" s="165" t="s">
+      <c r="H28" s="161"/>
+      <c r="I28" s="162" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="146" t="s">
+      <c r="A29" s="165" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="169" t="s">
+      <c r="B29" s="168" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="169" t="s">
+      <c r="C29" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="169"/>
-      <c r="E29" s="171" t="s">
+      <c r="D29" s="168"/>
+      <c r="E29" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="F29" s="172"/>
-      <c r="G29" s="210"/>
-      <c r="H29" s="211"/>
-      <c r="I29" s="175">
+      <c r="F29" s="171"/>
+      <c r="G29" s="216"/>
+      <c r="H29" s="217"/>
+      <c r="I29" s="174">
         <v>0.2</v>
       </c>
-      <c r="J29" s="212"/>
-      <c r="K29" s="214">
+      <c r="J29" s="218"/>
+      <c r="K29" s="220">
         <f>J29*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="168"/>
-      <c r="B30" s="169"/>
-      <c r="C30" s="169" t="s">
+      <c r="A30" s="166"/>
+      <c r="B30" s="168"/>
+      <c r="C30" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="169"/>
-      <c r="E30" s="182" t="s">
+      <c r="D30" s="168"/>
+      <c r="E30" s="181" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="183"/>
-      <c r="G30" s="202"/>
-      <c r="H30" s="203"/>
-      <c r="I30" s="176"/>
-      <c r="J30" s="212"/>
-      <c r="K30" s="214"/>
+      <c r="F30" s="182"/>
+      <c r="G30" s="222"/>
+      <c r="H30" s="223"/>
+      <c r="I30" s="175"/>
+      <c r="J30" s="218"/>
+      <c r="K30" s="220"/>
     </row>
     <row r="31" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="147"/>
-      <c r="B31" s="170"/>
-      <c r="C31" s="170" t="s">
+      <c r="A31" s="167"/>
+      <c r="B31" s="169"/>
+      <c r="C31" s="169" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="170"/>
-      <c r="E31" s="182" t="s">
+      <c r="D31" s="169"/>
+      <c r="E31" s="181" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="183"/>
-      <c r="G31" s="200"/>
-      <c r="H31" s="201"/>
-      <c r="I31" s="177"/>
-      <c r="J31" s="213"/>
-      <c r="K31" s="215"/>
+      <c r="F31" s="182"/>
+      <c r="G31" s="224"/>
+      <c r="H31" s="225"/>
+      <c r="I31" s="176"/>
+      <c r="J31" s="219"/>
+      <c r="K31" s="221"/>
     </row>
     <row r="32" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="146" t="s">
+      <c r="A32" s="165" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="148" t="s">
+      <c r="B32" s="190" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="149"/>
-      <c r="D32" s="150"/>
-      <c r="E32" s="151" t="s">
+      <c r="C32" s="191"/>
+      <c r="D32" s="192"/>
+      <c r="E32" s="193" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="152"/>
-      <c r="G32" s="202"/>
-      <c r="H32" s="203"/>
+      <c r="F32" s="194"/>
+      <c r="G32" s="222"/>
+      <c r="H32" s="223"/>
       <c r="I32" s="33">
         <v>0.4</v>
       </c>
@@ -3643,18 +3692,18 @@
       </c>
     </row>
     <row r="33" spans="1:11" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="147"/>
-      <c r="B33" s="155" t="s">
+      <c r="A33" s="167"/>
+      <c r="B33" s="195" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="156"/>
-      <c r="D33" s="157"/>
-      <c r="E33" s="158" t="s">
+      <c r="C33" s="196"/>
+      <c r="D33" s="197"/>
+      <c r="E33" s="198" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="159"/>
-      <c r="G33" s="202"/>
-      <c r="H33" s="203"/>
+      <c r="F33" s="199"/>
+      <c r="G33" s="222"/>
+      <c r="H33" s="223"/>
       <c r="I33" s="33">
         <v>0.4</v>
       </c>
@@ -3668,16 +3717,16 @@
       <c r="A34" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="143" t="s">
+      <c r="B34" s="187" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="144"/>
-      <c r="D34" s="144"/>
-      <c r="E34" s="144"/>
-      <c r="F34" s="144"/>
-      <c r="G34" s="144"/>
-      <c r="H34" s="144"/>
-      <c r="I34" s="145"/>
+      <c r="C34" s="188"/>
+      <c r="D34" s="188"/>
+      <c r="E34" s="188"/>
+      <c r="F34" s="188"/>
+      <c r="G34" s="188"/>
+      <c r="H34" s="188"/>
+      <c r="I34" s="189"/>
       <c r="J34" s="75"/>
       <c r="K34" s="74"/>
     </row>
@@ -3761,21 +3810,17 @@
     <row r="47" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="B34:I34"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="G28:H28"/>
@@ -3792,27 +3837,31 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="B34:I34"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
   </mergeCells>
-  <conditionalFormatting sqref="K29:K37">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="J29:J34 K29:K37">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="notBetween">
       <formula>0</formula>
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J29:J34 K29:K37">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="notBetween">
+  <conditionalFormatting sqref="K29:K37">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>0</formula>
-      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
@@ -3886,9 +3935,9 @@
         <v>9</v>
       </c>
       <c r="B4" s="18"/>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
-      <c r="E4" s="225"/>
+      <c r="C4" s="212"/>
+      <c r="D4" s="212"/>
+      <c r="E4" s="212"/>
       <c r="F4" s="58"/>
       <c r="H4" s="56"/>
       <c r="I4" s="55" t="s">
@@ -3903,10 +3952,10 @@
         <v>10</v>
       </c>
       <c r="B5" s="51"/>
-      <c r="C5" s="222"/>
-      <c r="D5" s="222"/>
-      <c r="E5" s="222"/>
-      <c r="F5" s="222"/>
+      <c r="C5" s="209"/>
+      <c r="D5" s="209"/>
+      <c r="E5" s="209"/>
+      <c r="F5" s="209"/>
       <c r="H5" s="56"/>
       <c r="I5" s="55" t="s">
         <v>8</v>
@@ -3928,87 +3977,87 @@
         <v>39</v>
       </c>
       <c r="B7" s="51"/>
-      <c r="C7" s="222"/>
-      <c r="D7" s="222"/>
-      <c r="E7" s="222"/>
-      <c r="F7" s="222"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
+      <c r="E7" s="209"/>
+      <c r="F7" s="209"/>
       <c r="H7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="223"/>
-      <c r="J7" s="224"/>
-      <c r="K7" s="224"/>
-      <c r="L7" s="224"/>
+      <c r="I7" s="210"/>
+      <c r="J7" s="211"/>
+      <c r="K7" s="211"/>
+      <c r="L7" s="211"/>
     </row>
     <row r="8" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="18"/>
-      <c r="C8" s="225"/>
-      <c r="D8" s="225"/>
-      <c r="E8" s="225"/>
-      <c r="F8" s="225"/>
+      <c r="C8" s="212"/>
+      <c r="D8" s="212"/>
+      <c r="E8" s="212"/>
+      <c r="F8" s="212"/>
       <c r="H8" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="216"/>
-      <c r="J8" s="217"/>
-      <c r="K8" s="217"/>
-      <c r="L8" s="217"/>
+      <c r="I8" s="200"/>
+      <c r="J8" s="201"/>
+      <c r="K8" s="201"/>
+      <c r="L8" s="201"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="51"/>
-      <c r="C9" s="222"/>
-      <c r="D9" s="222"/>
-      <c r="E9" s="222"/>
-      <c r="F9" s="222"/>
+      <c r="C9" s="209"/>
+      <c r="D9" s="209"/>
+      <c r="E9" s="209"/>
+      <c r="F9" s="209"/>
       <c r="H9" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="216"/>
-      <c r="J9" s="217"/>
-      <c r="K9" s="217"/>
-      <c r="L9" s="217"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="201"/>
+      <c r="K9" s="201"/>
+      <c r="L9" s="201"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="51" t="s">
         <v>37</v>
       </c>
       <c r="B10" s="51"/>
-      <c r="C10" s="222"/>
-      <c r="D10" s="222"/>
-      <c r="E10" s="222"/>
-      <c r="F10" s="222"/>
+      <c r="C10" s="209"/>
+      <c r="D10" s="209"/>
+      <c r="E10" s="209"/>
+      <c r="F10" s="209"/>
       <c r="H10" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="216"/>
-      <c r="J10" s="217"/>
-      <c r="K10" s="217"/>
-      <c r="L10" s="217"/>
+      <c r="I10" s="200"/>
+      <c r="J10" s="201"/>
+      <c r="K10" s="201"/>
+      <c r="L10" s="201"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H11" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="216"/>
-      <c r="J11" s="217"/>
-      <c r="K11" s="217"/>
-      <c r="L11" s="217"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="201"/>
+      <c r="K11" s="201"/>
+      <c r="L11" s="201"/>
     </row>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="52"/>
       <c r="H12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="216"/>
-      <c r="J12" s="217"/>
-      <c r="K12" s="217"/>
-      <c r="L12" s="217"/>
+      <c r="I12" s="200"/>
+      <c r="J12" s="201"/>
+      <c r="K12" s="201"/>
+      <c r="L12" s="201"/>
     </row>
     <row r="13" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="50"/>
@@ -4024,97 +4073,97 @@
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
-      <c r="H14" s="163" t="s">
+      <c r="H14" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="164"/>
-      <c r="J14" s="165" t="s">
+      <c r="I14" s="161"/>
+      <c r="J14" s="162" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="166"/>
-      <c r="L14" s="167"/>
+      <c r="K14" s="163"/>
+      <c r="L14" s="164"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="241" t="s">
+      <c r="A15" s="226" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="254" t="s">
+      <c r="B15" s="229" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="254" t="s">
+      <c r="C15" s="229" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="254"/>
-      <c r="E15" s="254"/>
-      <c r="F15" s="246" t="s">
+      <c r="D15" s="229"/>
+      <c r="E15" s="229"/>
+      <c r="F15" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="256"/>
-      <c r="H15" s="210"/>
-      <c r="I15" s="211"/>
-      <c r="J15" s="175">
+      <c r="G15" s="232"/>
+      <c r="H15" s="216"/>
+      <c r="I15" s="217"/>
+      <c r="J15" s="174">
         <v>0.2</v>
       </c>
-      <c r="K15" s="212">
-        <v>0</v>
-      </c>
-      <c r="L15" s="214">
+      <c r="K15" s="218">
+        <v>0</v>
+      </c>
+      <c r="L15" s="220">
         <f>K15*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="253"/>
-      <c r="B16" s="254"/>
-      <c r="C16" s="254" t="s">
+      <c r="A16" s="227"/>
+      <c r="B16" s="229"/>
+      <c r="C16" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="254"/>
-      <c r="E16" s="254"/>
-      <c r="F16" s="257" t="s">
+      <c r="D16" s="229"/>
+      <c r="E16" s="229"/>
+      <c r="F16" s="233" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="258"/>
-      <c r="H16" s="202"/>
-      <c r="I16" s="203"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="212"/>
-      <c r="L16" s="214"/>
+      <c r="G16" s="234"/>
+      <c r="H16" s="222"/>
+      <c r="I16" s="223"/>
+      <c r="J16" s="175"/>
+      <c r="K16" s="218"/>
+      <c r="L16" s="220"/>
     </row>
     <row r="17" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="242"/>
-      <c r="B17" s="255"/>
-      <c r="C17" s="255" t="s">
+      <c r="A17" s="228"/>
+      <c r="B17" s="230"/>
+      <c r="C17" s="230" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="255"/>
-      <c r="E17" s="255"/>
-      <c r="F17" s="257" t="s">
+      <c r="D17" s="230"/>
+      <c r="E17" s="230"/>
+      <c r="F17" s="233" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="258"/>
-      <c r="H17" s="200"/>
-      <c r="I17" s="201"/>
-      <c r="J17" s="177"/>
-      <c r="K17" s="213"/>
-      <c r="L17" s="215"/>
+      <c r="G17" s="234"/>
+      <c r="H17" s="224"/>
+      <c r="I17" s="225"/>
+      <c r="J17" s="176"/>
+      <c r="K17" s="219"/>
+      <c r="L17" s="221"/>
     </row>
     <row r="18" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="241" t="s">
+      <c r="A18" s="226" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="243" t="s">
+      <c r="B18" s="235" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="244"/>
-      <c r="D18" s="244"/>
-      <c r="E18" s="245"/>
-      <c r="F18" s="246" t="s">
+      <c r="C18" s="236"/>
+      <c r="D18" s="236"/>
+      <c r="E18" s="237"/>
+      <c r="F18" s="231" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="247"/>
-      <c r="H18" s="202"/>
-      <c r="I18" s="203"/>
+      <c r="G18" s="238"/>
+      <c r="H18" s="222"/>
+      <c r="I18" s="223"/>
       <c r="J18" s="33">
         <v>0.4</v>
       </c>
@@ -4128,19 +4177,19 @@
       <c r="M18" s="61"/>
     </row>
     <row r="19" spans="1:13" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="242"/>
-      <c r="B19" s="248" t="s">
+      <c r="A19" s="228"/>
+      <c r="B19" s="239" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="249"/>
-      <c r="D19" s="249"/>
-      <c r="E19" s="250"/>
-      <c r="F19" s="251" t="s">
+      <c r="C19" s="240"/>
+      <c r="D19" s="240"/>
+      <c r="E19" s="241"/>
+      <c r="F19" s="242" t="s">
         <v>23</v>
       </c>
-      <c r="G19" s="252"/>
-      <c r="H19" s="202"/>
-      <c r="I19" s="203"/>
+      <c r="G19" s="243"/>
+      <c r="H19" s="222"/>
+      <c r="I19" s="223"/>
       <c r="J19" s="33">
         <v>0.4</v>
       </c>
@@ -4156,17 +4205,17 @@
       <c r="A20" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="143" t="s">
+      <c r="B20" s="187" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="144"/>
-      <c r="D20" s="144"/>
-      <c r="E20" s="144"/>
-      <c r="F20" s="144"/>
-      <c r="G20" s="144"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="144"/>
-      <c r="J20" s="145"/>
+      <c r="C20" s="188"/>
+      <c r="D20" s="188"/>
+      <c r="E20" s="188"/>
+      <c r="F20" s="188"/>
+      <c r="G20" s="188"/>
+      <c r="H20" s="188"/>
+      <c r="I20" s="188"/>
+      <c r="J20" s="189"/>
       <c r="K20" s="32"/>
       <c r="L20" s="76"/>
     </row>
@@ -4184,90 +4233,90 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="232" t="s">
+      <c r="A23" s="244" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="233"/>
-      <c r="C23" s="233"/>
-      <c r="D23" s="233"/>
-      <c r="E23" s="233"/>
-      <c r="F23" s="233"/>
-      <c r="G23" s="233"/>
-      <c r="H23" s="233"/>
-      <c r="I23" s="233"/>
-      <c r="J23" s="233"/>
-      <c r="K23" s="233"/>
-      <c r="L23" s="234"/>
+      <c r="B23" s="245"/>
+      <c r="C23" s="245"/>
+      <c r="D23" s="245"/>
+      <c r="E23" s="245"/>
+      <c r="F23" s="245"/>
+      <c r="G23" s="245"/>
+      <c r="H23" s="245"/>
+      <c r="I23" s="245"/>
+      <c r="J23" s="245"/>
+      <c r="K23" s="245"/>
+      <c r="L23" s="246"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="235"/>
-      <c r="B24" s="236"/>
-      <c r="C24" s="236"/>
-      <c r="D24" s="236"/>
-      <c r="E24" s="236"/>
-      <c r="F24" s="236"/>
-      <c r="G24" s="236"/>
-      <c r="H24" s="236"/>
-      <c r="I24" s="236"/>
-      <c r="J24" s="236"/>
-      <c r="K24" s="236"/>
-      <c r="L24" s="237"/>
+      <c r="A24" s="247"/>
+      <c r="B24" s="248"/>
+      <c r="C24" s="248"/>
+      <c r="D24" s="248"/>
+      <c r="E24" s="248"/>
+      <c r="F24" s="248"/>
+      <c r="G24" s="248"/>
+      <c r="H24" s="248"/>
+      <c r="I24" s="248"/>
+      <c r="J24" s="248"/>
+      <c r="K24" s="248"/>
+      <c r="L24" s="249"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="235"/>
-      <c r="B25" s="236"/>
-      <c r="C25" s="236"/>
-      <c r="D25" s="236"/>
-      <c r="E25" s="236"/>
-      <c r="F25" s="236"/>
-      <c r="G25" s="236"/>
-      <c r="H25" s="236"/>
-      <c r="I25" s="236"/>
-      <c r="J25" s="236"/>
-      <c r="K25" s="236"/>
-      <c r="L25" s="237"/>
+      <c r="A25" s="247"/>
+      <c r="B25" s="248"/>
+      <c r="C25" s="248"/>
+      <c r="D25" s="248"/>
+      <c r="E25" s="248"/>
+      <c r="F25" s="248"/>
+      <c r="G25" s="248"/>
+      <c r="H25" s="248"/>
+      <c r="I25" s="248"/>
+      <c r="J25" s="248"/>
+      <c r="K25" s="248"/>
+      <c r="L25" s="249"/>
     </row>
     <row r="26" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="235"/>
-      <c r="B26" s="236"/>
-      <c r="C26" s="236"/>
-      <c r="D26" s="236"/>
-      <c r="E26" s="236"/>
-      <c r="F26" s="236"/>
-      <c r="G26" s="236"/>
-      <c r="H26" s="236"/>
-      <c r="I26" s="236"/>
-      <c r="J26" s="236"/>
-      <c r="K26" s="236"/>
-      <c r="L26" s="237"/>
+      <c r="A26" s="247"/>
+      <c r="B26" s="248"/>
+      <c r="C26" s="248"/>
+      <c r="D26" s="248"/>
+      <c r="E26" s="248"/>
+      <c r="F26" s="248"/>
+      <c r="G26" s="248"/>
+      <c r="H26" s="248"/>
+      <c r="I26" s="248"/>
+      <c r="J26" s="248"/>
+      <c r="K26" s="248"/>
+      <c r="L26" s="249"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="238"/>
-      <c r="B27" s="239"/>
-      <c r="C27" s="239"/>
-      <c r="D27" s="239"/>
-      <c r="E27" s="239"/>
-      <c r="F27" s="239"/>
-      <c r="G27" s="239"/>
-      <c r="H27" s="239"/>
-      <c r="I27" s="239"/>
-      <c r="J27" s="239"/>
-      <c r="K27" s="239"/>
-      <c r="L27" s="240"/>
+      <c r="A27" s="250"/>
+      <c r="B27" s="251"/>
+      <c r="C27" s="251"/>
+      <c r="D27" s="251"/>
+      <c r="E27" s="251"/>
+      <c r="F27" s="251"/>
+      <c r="G27" s="251"/>
+      <c r="H27" s="251"/>
+      <c r="I27" s="251"/>
+      <c r="J27" s="251"/>
+      <c r="K27" s="251"/>
+      <c r="L27" s="252"/>
     </row>
     <row r="29" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="229" t="s">
+      <c r="A29" s="253" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="229"/>
-      <c r="C29" s="229"/>
-      <c r="D29" s="229"/>
-      <c r="E29" s="229"/>
-      <c r="F29" s="229"/>
-      <c r="G29" s="229"/>
-      <c r="H29" s="229"/>
-      <c r="I29" s="230"/>
-      <c r="J29" s="230"/>
+      <c r="B29" s="253"/>
+      <c r="C29" s="253"/>
+      <c r="D29" s="253"/>
+      <c r="E29" s="253"/>
+      <c r="F29" s="253"/>
+      <c r="G29" s="253"/>
+      <c r="H29" s="253"/>
+      <c r="I29" s="254"/>
+      <c r="J29" s="254"/>
       <c r="K29" s="63" t="s">
         <v>72</v>
       </c>
@@ -4277,18 +4326,18 @@
       </c>
     </row>
     <row r="30" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="229" t="s">
+      <c r="A30" s="253" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="229"/>
-      <c r="C30" s="229"/>
-      <c r="D30" s="229"/>
-      <c r="E30" s="229"/>
-      <c r="F30" s="229"/>
-      <c r="G30" s="229"/>
-      <c r="H30" s="229"/>
-      <c r="I30" s="230"/>
-      <c r="J30" s="230"/>
+      <c r="B30" s="253"/>
+      <c r="C30" s="253"/>
+      <c r="D30" s="253"/>
+      <c r="E30" s="253"/>
+      <c r="F30" s="253"/>
+      <c r="G30" s="253"/>
+      <c r="H30" s="253"/>
+      <c r="I30" s="254"/>
+      <c r="J30" s="254"/>
       <c r="K30" s="48" t="s">
         <v>72</v>
       </c>
@@ -4298,18 +4347,18 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="229" t="s">
+      <c r="A31" s="253" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="229"/>
-      <c r="C31" s="229"/>
-      <c r="D31" s="229"/>
-      <c r="E31" s="229"/>
-      <c r="F31" s="229"/>
-      <c r="G31" s="229"/>
-      <c r="H31" s="229"/>
-      <c r="I31" s="230"/>
-      <c r="J31" s="230"/>
+      <c r="B31" s="253"/>
+      <c r="C31" s="253"/>
+      <c r="D31" s="253"/>
+      <c r="E31" s="253"/>
+      <c r="F31" s="253"/>
+      <c r="G31" s="253"/>
+      <c r="H31" s="253"/>
+      <c r="I31" s="254"/>
+      <c r="J31" s="254"/>
       <c r="K31" s="48" t="s">
         <v>75</v>
       </c>
@@ -4319,18 +4368,18 @@
       </c>
     </row>
     <row r="32" spans="1:13" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="229" t="s">
+      <c r="A32" s="253" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="229"/>
-      <c r="C32" s="229"/>
-      <c r="D32" s="229"/>
-      <c r="E32" s="229"/>
-      <c r="F32" s="229"/>
-      <c r="G32" s="229"/>
-      <c r="H32" s="229"/>
-      <c r="I32" s="230"/>
-      <c r="J32" s="230"/>
+      <c r="B32" s="253"/>
+      <c r="C32" s="253"/>
+      <c r="D32" s="253"/>
+      <c r="E32" s="253"/>
+      <c r="F32" s="253"/>
+      <c r="G32" s="253"/>
+      <c r="H32" s="253"/>
+      <c r="I32" s="254"/>
+      <c r="J32" s="254"/>
       <c r="K32" s="48" t="s">
         <v>53</v>
       </c>
@@ -4340,21 +4389,21 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="229" t="s">
+      <c r="A33" s="253" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="229"/>
-      <c r="C33" s="229"/>
-      <c r="D33" s="229"/>
-      <c r="E33" s="229"/>
-      <c r="F33" s="229"/>
-      <c r="G33" s="229"/>
-      <c r="H33" s="229"/>
-      <c r="I33" s="231">
+      <c r="B33" s="253"/>
+      <c r="C33" s="253"/>
+      <c r="D33" s="253"/>
+      <c r="E33" s="253"/>
+      <c r="F33" s="253"/>
+      <c r="G33" s="253"/>
+      <c r="H33" s="253"/>
+      <c r="I33" s="258">
         <f>L21</f>
         <v>0</v>
       </c>
-      <c r="J33" s="231"/>
+      <c r="J33" s="258"/>
       <c r="K33" s="48" t="s">
         <v>75</v>
       </c>
@@ -4376,14 +4425,14 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="13.9" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F35" s="226" t="s">
+      <c r="F35" s="255" t="s">
         <v>79</v>
       </c>
-      <c r="G35" s="227"/>
-      <c r="H35" s="227"/>
-      <c r="I35" s="227"/>
-      <c r="J35" s="227"/>
-      <c r="K35" s="228"/>
+      <c r="G35" s="256"/>
+      <c r="H35" s="256"/>
+      <c r="I35" s="256"/>
+      <c r="J35" s="256"/>
+      <c r="K35" s="257"/>
       <c r="L35" s="67">
         <f>L34/10</f>
         <v>0</v>
@@ -4474,18 +4523,26 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="A31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="A23:L27"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="A15:A17"/>
@@ -4502,36 +4559,28 @@
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="A23:L27"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="A31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
   </mergeCells>
-  <conditionalFormatting sqref="L15:L39 I33:J33">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="K15:K20 L15:L39 I29:J33">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="notBetween">
       <formula>0</formula>
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15:K20 I29:J33 L15:L39">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="notBetween">
+  <conditionalFormatting sqref="L15:L39 I33:J33">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
-      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
@@ -4550,12 +4599,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4625,18 +4674,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64838F1D-7ECA-4F32-944F-43492487C498}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4659,16 +4715,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64838F1D-7ECA-4F32-944F-43492487C498}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>